<commit_message>
R385 has correct value now
</commit_message>
<xml_diff>
--- a/radiant_bom.xlsx
+++ b/radiant_bom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="570">
   <si>
     <t>Item</t>
   </si>
@@ -965,9 +965,6 @@
     <t>RESISTOR,3.24k</t>
   </si>
   <si>
-    <t>R385 R387</t>
-  </si>
-  <si>
     <t>RESISTOR,32k</t>
   </si>
   <si>
@@ -1412,9 +1409,6 @@
     <t>1050270001</t>
   </si>
   <si>
-    <t>SI5338Q-B-GM</t>
-  </si>
-  <si>
     <t>PE42440MLBB-Z</t>
   </si>
   <si>
@@ -1646,9 +1640,6 @@
     <t>Rohm</t>
   </si>
   <si>
-    <t>RE1C002UN</t>
-  </si>
-  <si>
     <t>MOSFET N-CH 20V 0.2A EMT3</t>
   </si>
   <si>
@@ -1728,6 +1719,21 @@
   </si>
   <si>
     <t>EXAR</t>
+  </si>
+  <si>
+    <t>R387</t>
+  </si>
+  <si>
+    <t>R385</t>
+  </si>
+  <si>
+    <t>RESISTOR,53.6k</t>
+  </si>
+  <si>
+    <t>RE1C002UNTCL</t>
+  </si>
+  <si>
+    <t>SI5338C-B-GM</t>
   </si>
 </sst>
 </file>
@@ -2069,8 +2075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection sqref="A1:H165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2090,16 +2096,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>4</v>
+        <v>436</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>6</v>
@@ -2116,16 +2122,16 @@
         <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>428</v>
-      </c>
       <c r="G2" s="3" t="s">
-        <v>8</v>
+        <v>427</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>10</v>
@@ -2142,16 +2148,16 @@
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>429</v>
-      </c>
       <c r="G3" s="3" t="s">
-        <v>430</v>
+        <v>437</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>13</v>
@@ -2168,16 +2174,16 @@
         <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>16</v>
+        <v>438</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>18</v>
@@ -2194,13 +2200,13 @@
         <v>19</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>20</v>
@@ -2220,16 +2226,16 @@
         <v>22</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>26</v>
@@ -2246,13 +2252,13 @@
         <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>28</v>
@@ -2272,16 +2278,16 @@
         <v>31</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>440</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="G8" s="3" t="s">
-        <v>32</v>
+        <v>439</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>33</v>
@@ -2298,16 +2304,16 @@
         <v>34</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="G9" s="3" t="s">
-        <v>36</v>
+        <v>440</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>38</v>
@@ -2324,16 +2330,16 @@
         <v>39</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="G10" s="3" t="s">
-        <v>41</v>
+        <v>441</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>43</v>
@@ -2350,16 +2356,16 @@
         <v>44</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>443</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="G11" s="3" t="s">
-        <v>46</v>
+        <v>442</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>48</v>
@@ -2376,16 +2382,16 @@
         <v>49</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>444</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="G12" s="3" t="s">
-        <v>51</v>
+        <v>443</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>53</v>
@@ -2402,16 +2408,16 @@
         <v>54</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G13" s="3" t="s">
-        <v>56</v>
+        <v>444</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>58</v>
@@ -2428,16 +2434,16 @@
         <v>59</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="G14" s="3" t="s">
-        <v>61</v>
+        <v>445</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>63</v>
@@ -2454,16 +2460,16 @@
         <v>64</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="G15" s="3" t="s">
-        <v>66</v>
+        <v>446</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>68</v>
@@ -2480,16 +2486,16 @@
         <v>69</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>448</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="G16" s="3" t="s">
-        <v>71</v>
+        <v>447</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>73</v>
@@ -2505,14 +2511,14 @@
       <c r="C17" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
@@ -2524,14 +2530,14 @@
       <c r="C18" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>78</v>
       </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
@@ -2543,14 +2549,14 @@
       <c r="C19" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>78</v>
       </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
@@ -2562,14 +2568,14 @@
       <c r="C20" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
@@ -2581,14 +2587,14 @@
       <c r="C21" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>85</v>
       </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
@@ -2600,14 +2606,14 @@
       <c r="C22" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="G22" s="3" t="s">
+      <c r="D22" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
@@ -2620,16 +2626,16 @@
         <v>86</v>
       </c>
       <c r="D23" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="G23" s="3" t="s">
-        <v>88</v>
+        <v>448</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>90</v>
@@ -2643,16 +2649,16 @@
         <v>174</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>417</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
@@ -2662,16 +2668,16 @@
         <v>62</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
@@ -2681,16 +2687,16 @@
         <v>169</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>418</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>85</v>
       </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
@@ -2702,14 +2708,14 @@
       <c r="C27" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
@@ -2721,14 +2727,14 @@
       <c r="C28" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
@@ -2738,16 +2744,16 @@
         <v>25</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>420</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
@@ -2757,16 +2763,16 @@
         <v>62</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>425</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
@@ -2778,14 +2784,14 @@
       <c r="C31" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
@@ -2797,14 +2803,14 @@
       <c r="C32" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
     </row>
     <row r="33" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
@@ -2816,14 +2822,14 @@
       <c r="C33" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
@@ -2835,14 +2841,14 @@
       <c r="C34" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3" t="s">
-        <v>421</v>
-      </c>
-      <c r="G34" s="3" t="s">
+      <c r="D34" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
@@ -2854,14 +2860,14 @@
       <c r="C35" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="G35" s="3" t="s">
+      <c r="D35" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
@@ -2871,16 +2877,16 @@
         <v>122</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>426</v>
-      </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
     </row>
     <row r="37" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
@@ -2892,14 +2898,14 @@
       <c r="C37" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
@@ -2911,14 +2917,14 @@
       <c r="C38" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>88</v>
       </c>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
     </row>
     <row r="39" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
@@ -2930,14 +2936,14 @@
       <c r="C39" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
     </row>
     <row r="40" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
@@ -2949,14 +2955,14 @@
       <c r="C40" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
@@ -2968,14 +2974,14 @@
       <c r="C41" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="E41" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
     </row>
     <row r="42" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
@@ -2987,14 +2993,14 @@
       <c r="C42" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
@@ -3006,14 +3012,14 @@
       <c r="C43" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
     </row>
     <row r="44" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
@@ -3025,14 +3031,14 @@
       <c r="C44" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
@@ -3044,14 +3050,14 @@
       <c r="C45" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3" t="s">
+      <c r="D45" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="E45" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
@@ -3063,14 +3069,14 @@
       <c r="C46" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="E46" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
@@ -3082,14 +3088,14 @@
       <c r="C47" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3" t="s">
+      <c r="D47" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="E47" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
@@ -3099,16 +3105,16 @@
         <v>37</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>427</v>
-      </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="G48" s="3" t="s">
+      <c r="E48" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
     </row>
     <row r="49" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
@@ -3120,14 +3126,14 @@
       <c r="C49" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3" t="s">
+      <c r="D49" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="G49" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
     </row>
     <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
@@ -3139,14 +3145,14 @@
       <c r="C50" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3" t="s">
+      <c r="D50" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G50" s="3" t="s">
+      <c r="E50" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
     </row>
     <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
@@ -3158,14 +3164,14 @@
       <c r="C51" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3" t="s">
+      <c r="D51" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="G51" s="3" t="s">
+      <c r="E51" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
     </row>
     <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
@@ -3175,16 +3181,16 @@
         <v>9</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>431</v>
-      </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="E52" s="3" t="s">
         <v>95</v>
       </c>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
     </row>
     <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
@@ -3196,14 +3202,14 @@
       <c r="C53" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="G53" s="3" t="s">
+      <c r="D53" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
     </row>
     <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
@@ -3215,14 +3221,14 @@
       <c r="C54" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3" t="s">
+      <c r="D54" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="G54" s="3" t="s">
+      <c r="E54" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
     </row>
     <row r="55" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
@@ -3234,14 +3240,14 @@
       <c r="C55" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3" t="s">
+      <c r="D55" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G55" s="3" t="s">
+      <c r="E55" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
     </row>
     <row r="56" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
@@ -3253,14 +3259,14 @@
       <c r="C56" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3" t="s">
+      <c r="D56" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="G56" s="3" t="s">
+      <c r="E56" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
     </row>
     <row r="57" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
@@ -3272,14 +3278,14 @@
       <c r="C57" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3" t="s">
-        <v>424</v>
-      </c>
-      <c r="G57" s="3" t="s">
+      <c r="D57" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
     </row>
     <row r="58" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
@@ -3292,16 +3298,16 @@
         <v>151</v>
       </c>
       <c r="D58" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F58" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E58" s="3" t="s">
-        <v>450</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="G58" s="3" t="s">
-        <v>153</v>
+        <v>449</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>155</v>
@@ -3318,16 +3324,16 @@
         <v>156</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>465</v>
+        <v>157</v>
       </c>
       <c r="E59" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="G59" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>159</v>
@@ -3344,16 +3350,16 @@
         <v>160</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>380</v>
+        <v>161</v>
       </c>
       <c r="E60" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="G60" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>162</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>163</v>
@@ -3370,19 +3376,19 @@
         <v>164</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>466</v>
+        <v>165</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>466</v>
+        <v>166</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>165</v>
+        <v>464</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>166</v>
+        <v>464</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3396,16 +3402,16 @@
         <v>167</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>467</v>
+        <v>168</v>
       </c>
       <c r="E62" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="G62" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>169</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>170</v>
@@ -3419,19 +3425,19 @@
         <v>49</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D63" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F63" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="E63" s="3" t="s">
-        <v>451</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>171</v>
-      </c>
       <c r="G63" s="3" t="s">
-        <v>173</v>
+        <v>450</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3445,16 +3451,16 @@
         <v>175</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>469</v>
+        <v>176</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>452</v>
+        <v>172</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>176</v>
+        <v>467</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>172</v>
+        <v>451</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3468,19 +3474,19 @@
         <v>177</v>
       </c>
       <c r="D65" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F65" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E65" s="3" t="s">
-        <v>470</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="G65" s="3" t="s">
-        <v>179</v>
+        <v>468</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="66" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3494,19 +3500,19 @@
         <v>180</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>469</v>
+        <v>181</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>472</v>
+        <v>181</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>181</v>
+        <v>467</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>181</v>
+        <v>470</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="67" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3520,16 +3526,16 @@
         <v>182</v>
       </c>
       <c r="D67" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="F67" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E67" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>183</v>
-      </c>
       <c r="G67" s="3" t="s">
-        <v>432</v>
+        <v>452</v>
       </c>
     </row>
     <row r="68" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3543,16 +3549,16 @@
         <v>184</v>
       </c>
       <c r="D68" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="F68" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E68" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>185</v>
-      </c>
       <c r="G68" s="3" t="s">
-        <v>433</v>
+        <v>453</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3566,16 +3572,16 @@
         <v>186</v>
       </c>
       <c r="D69" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="F69" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E69" s="3" t="s">
-        <v>455</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="G69" s="3" t="s">
-        <v>433</v>
+        <v>454</v>
       </c>
     </row>
     <row r="70" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3589,16 +3595,16 @@
         <v>188</v>
       </c>
       <c r="D70" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="F70" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="E70" s="3" t="s">
-        <v>456</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>189</v>
-      </c>
       <c r="G70" s="3" t="s">
-        <v>434</v>
+        <v>455</v>
       </c>
     </row>
     <row r="71" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3612,19 +3618,19 @@
         <v>190</v>
       </c>
       <c r="D71" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="F71" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E71" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>191</v>
-      </c>
       <c r="G71" s="3" t="s">
-        <v>434</v>
+        <v>472</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="72" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3638,19 +3644,19 @@
         <v>192</v>
       </c>
       <c r="D72" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="F72" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E72" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>193</v>
-      </c>
       <c r="G72" s="3" t="s">
-        <v>434</v>
+        <v>474</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="73" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3664,19 +3670,19 @@
         <v>194</v>
       </c>
       <c r="D73" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="F73" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E73" s="3" t="s">
-        <v>478</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>195</v>
-      </c>
       <c r="G73" s="3" t="s">
-        <v>434</v>
+        <v>476</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3690,19 +3696,19 @@
         <v>196</v>
       </c>
       <c r="D74" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="F74" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E74" s="3" t="s">
-        <v>480</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>197</v>
-      </c>
       <c r="G74" s="3" t="s">
-        <v>434</v>
+        <v>478</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="75" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3716,19 +3722,19 @@
         <v>198</v>
       </c>
       <c r="D75" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="F75" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E75" s="3" t="s">
-        <v>482</v>
-      </c>
-      <c r="F75" s="3" t="s">
-        <v>199</v>
-      </c>
       <c r="G75" s="3" t="s">
-        <v>434</v>
+        <v>480</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3742,16 +3748,16 @@
         <v>200</v>
       </c>
       <c r="D76" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="F76" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E76" s="3" t="s">
-        <v>457</v>
-      </c>
-      <c r="F76" s="3" t="s">
-        <v>201</v>
-      </c>
       <c r="G76" s="3" t="s">
-        <v>435</v>
+        <v>456</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>202</v>
@@ -3767,14 +3773,14 @@
       <c r="C77" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3" t="s">
+      <c r="D77" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="G77" s="3" t="s">
+      <c r="E77" s="3" t="s">
         <v>204</v>
       </c>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
     </row>
     <row r="78" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
@@ -3787,19 +3793,19 @@
         <v>205</v>
       </c>
       <c r="D78" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="H78" s="2" t="s">
         <v>484</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>485</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="G78" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="H78" s="2" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3813,10 +3819,10 @@
         <v>208</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="F79" s="3" t="s">
         <v>487</v>
@@ -3825,7 +3831,7 @@
         <v>488</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3839,19 +3845,19 @@
         <v>211</v>
       </c>
       <c r="D80" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="H80" s="2" t="s">
         <v>492</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>493</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="G80" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="H80" s="2" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="81" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3865,19 +3871,19 @@
         <v>214</v>
       </c>
       <c r="D81" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F81" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E81" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="F81" s="3" t="s">
-        <v>215</v>
-      </c>
       <c r="G81" s="3" t="s">
-        <v>216</v>
+        <v>493</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="82" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3891,16 +3897,16 @@
         <v>217</v>
       </c>
       <c r="D82" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F82" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E82" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>218</v>
-      </c>
       <c r="G82" s="3" t="s">
-        <v>219</v>
+        <v>495</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>220</v>
@@ -3917,19 +3923,19 @@
         <v>221</v>
       </c>
       <c r="D83" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F83" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E83" s="3" t="s">
-        <v>498</v>
-      </c>
-      <c r="F83" s="3" t="s">
-        <v>222</v>
-      </c>
       <c r="G83" s="3" t="s">
-        <v>223</v>
+        <v>496</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="84" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3942,18 +3948,18 @@
       <c r="C84" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="D84" s="3"/>
+      <c r="D84" s="3" t="s">
+        <v>225</v>
+      </c>
       <c r="E84" s="3" t="s">
-        <v>500</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>225</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="F84" s="3"/>
       <c r="G84" s="3" t="s">
-        <v>226</v>
+        <v>498</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="85" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3967,16 +3973,16 @@
         <v>227</v>
       </c>
       <c r="D85" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="F85" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E85" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>228</v>
-      </c>
       <c r="G85" s="3" t="s">
-        <v>229</v>
+        <v>457</v>
       </c>
       <c r="H85" s="2" t="s">
         <v>230</v>
@@ -3993,16 +3999,16 @@
         <v>231</v>
       </c>
       <c r="D86" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="F86" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E86" s="3" t="s">
-        <v>459</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>232</v>
-      </c>
       <c r="G86" s="3" t="s">
-        <v>233</v>
+        <v>458</v>
       </c>
       <c r="H86" s="2" t="s">
         <v>234</v>
@@ -4019,16 +4025,16 @@
         <v>235</v>
       </c>
       <c r="D87" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="F87" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="E87" s="3" t="s">
-        <v>460</v>
-      </c>
-      <c r="F87" s="3" t="s">
-        <v>236</v>
-      </c>
       <c r="G87" s="3" t="s">
-        <v>237</v>
+        <v>459</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>239</v>
@@ -4045,16 +4051,16 @@
         <v>240</v>
       </c>
       <c r="D88" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="F88" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E88" s="3" t="s">
+      <c r="G88" s="3" t="s">
         <v>241</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>242</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>243</v>
@@ -4071,19 +4077,19 @@
         <v>244</v>
       </c>
       <c r="D89" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F89" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E89" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="F89" s="3" t="s">
-        <v>245</v>
-      </c>
       <c r="G89" s="3" t="s">
-        <v>245</v>
+        <v>460</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="90" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -4097,16 +4103,16 @@
         <v>246</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>503</v>
+        <v>247</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>504</v>
+        <v>248</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>247</v>
+        <v>501</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>248</v>
+        <v>502</v>
       </c>
     </row>
     <row r="91" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -4120,19 +4126,19 @@
         <v>249</v>
       </c>
       <c r="D91" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F91" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E91" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>250</v>
-      </c>
       <c r="G91" s="3" t="s">
-        <v>251</v>
+        <v>503</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="92" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -4146,19 +4152,19 @@
         <v>252</v>
       </c>
       <c r="D92" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="F92" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E92" s="3" t="s">
+      <c r="G92" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="F92" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="G92" s="3" t="s">
-        <v>254</v>
-      </c>
       <c r="H92" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="93" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -4172,19 +4178,19 @@
         <v>255</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>508</v>
+        <v>256</v>
       </c>
       <c r="E93" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="G93" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="F93" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="G93" s="3" t="s">
-        <v>257</v>
-      </c>
       <c r="H93" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="94" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -4198,19 +4204,19 @@
         <v>258</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>508</v>
+        <v>259</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>259</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>259</v>
+        <v>506</v>
       </c>
       <c r="G94" s="3" t="s">
         <v>259</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="95" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -4224,19 +4230,19 @@
         <v>260</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>508</v>
+        <v>261</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>261</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>261</v>
+        <v>506</v>
       </c>
       <c r="G95" s="3" t="s">
         <v>261</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="96" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -4250,16 +4256,16 @@
         <v>262</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>517</v>
+        <v>263</v>
       </c>
       <c r="E96" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="G96" s="3" t="s">
         <v>263</v>
-      </c>
-      <c r="F96" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>264</v>
       </c>
       <c r="H96" s="2" t="s">
         <v>265</v>
@@ -4276,19 +4282,19 @@
         <v>266</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>466</v>
+        <v>267</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>466</v>
+        <v>268</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>267</v>
+        <v>464</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>268</v>
+        <v>464</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="98" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -4302,19 +4308,19 @@
         <v>269</v>
       </c>
       <c r="D98" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="F98" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E98" s="3" t="s">
-        <v>518</v>
-      </c>
-      <c r="F98" s="3" t="s">
-        <v>270</v>
-      </c>
       <c r="G98" s="3" t="s">
-        <v>271</v>
+        <v>516</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="99" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -4328,16 +4334,16 @@
         <v>272</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>520</v>
+        <v>273</v>
       </c>
       <c r="E99" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="G99" s="3" t="s">
         <v>273</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="G99" s="3" t="s">
-        <v>274</v>
       </c>
       <c r="H99" s="2" t="s">
         <v>275</v>
@@ -4354,19 +4360,19 @@
         <v>276</v>
       </c>
       <c r="D100" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="H100" s="2" t="s">
         <v>521</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>522</v>
-      </c>
-      <c r="F100" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="G100" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="H100" s="2" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="101" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -4379,14 +4385,14 @@
       <c r="C101" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="D101" s="5"/>
-      <c r="E101" s="5"/>
-      <c r="F101" s="5" t="s">
+      <c r="D101" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G101" s="5" t="s">
+      <c r="E101" s="5" t="s">
         <v>280</v>
       </c>
+      <c r="F101" s="5"/>
+      <c r="G101" s="5"/>
     </row>
     <row r="102" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4">
@@ -4396,16 +4402,16 @@
         <v>73</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>524</v>
-      </c>
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
-      <c r="F102" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="D102" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="G102" s="5" t="s">
+      <c r="E102" s="5" t="s">
         <v>280</v>
       </c>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
     </row>
     <row r="103" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="4">
@@ -4415,16 +4421,16 @@
         <v>6</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>525</v>
-      </c>
-      <c r="D103" s="5"/>
-      <c r="E103" s="5"/>
-      <c r="F103" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="D103" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="G103" s="5" t="s">
-        <v>433</v>
-      </c>
+      <c r="E103" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="F103" s="5"/>
+      <c r="G103" s="5"/>
     </row>
     <row r="104" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4">
@@ -4434,16 +4440,16 @@
         <v>51</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>526</v>
-      </c>
-      <c r="D104" s="5"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="D104" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="G104" s="5" t="s">
+      <c r="E104" s="5" t="s">
         <v>280</v>
       </c>
+      <c r="F104" s="5"/>
+      <c r="G104" s="5"/>
     </row>
     <row r="105" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="4">
@@ -4453,16 +4459,16 @@
         <v>247</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>527</v>
-      </c>
-      <c r="D105" s="5"/>
-      <c r="E105" s="5"/>
-      <c r="F105" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="D105" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="G105" s="5" t="s">
+      <c r="E105" s="5" t="s">
         <v>280</v>
       </c>
+      <c r="F105" s="5"/>
+      <c r="G105" s="5"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106">
@@ -4474,10 +4480,10 @@
       <c r="C106" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="F106" s="1" t="s">
+      <c r="D106" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="G106" s="1" t="s">
+      <c r="E106" s="1" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4491,10 +4497,10 @@
       <c r="C107" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="F107" s="1" t="s">
+      <c r="D107" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="G107" s="1" t="s">
+      <c r="E107" s="1" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4508,10 +4514,10 @@
       <c r="C108" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="F108" s="1" t="s">
-        <v>528</v>
-      </c>
-      <c r="G108" s="1" t="s">
+      <c r="D108" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="E108" s="1" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4523,12 +4529,12 @@
         <v>1</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>529</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="G109" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="E109" s="1" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4540,13 +4546,13 @@
         <v>12</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>330</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="G110" s="1" t="s">
-        <v>433</v>
+        <v>329</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
@@ -4559,10 +4565,10 @@
       <c r="C111" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="F111" s="1" t="s">
+      <c r="D111" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="G111" s="1" t="s">
+      <c r="E111" s="1" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4576,14 +4582,14 @@
       <c r="C112" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="F112" s="1" t="s">
+      <c r="D112" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="G112" s="1" t="s">
+      <c r="E112" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4593,14 +4599,14 @@
       <c r="C113" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="F113" s="1" t="s">
+      <c r="D113" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="G113" s="1" t="s">
+      <c r="E113" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4610,14 +4616,14 @@
       <c r="C114" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="F114" s="1" t="s">
+      <c r="D114" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="G114" s="1" t="s">
+      <c r="E114" s="1" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4627,14 +4633,14 @@
       <c r="C115" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="F115" s="1" t="s">
+      <c r="D115" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="G115" s="1" t="s">
+      <c r="E115" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4644,14 +4650,14 @@
       <c r="C116" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="F116" s="1" t="s">
+      <c r="D116" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="G116" s="1" t="s">
+      <c r="E116" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -4661,14 +4667,14 @@
       <c r="C117" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="F117" s="1" t="s">
+      <c r="D117" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="G117" s="1" t="s">
+      <c r="E117" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -4678,14 +4684,14 @@
       <c r="C118" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="F118" s="1" t="s">
+      <c r="D118" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="G118" s="1" t="s">
+      <c r="E118" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -4695,14 +4701,14 @@
       <c r="C119" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="F119" s="1" t="s">
+      <c r="D119" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="G119" s="1" t="s">
+      <c r="E119" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -4712,14 +4718,14 @@
       <c r="C120" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="F120" s="1" t="s">
+      <c r="D120" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="G120" s="1" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E120" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -4729,14 +4735,14 @@
       <c r="C121" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="F121" s="1" t="s">
+      <c r="D121" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="G121" s="1" t="s">
+      <c r="E121" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
@@ -4746,31 +4752,31 @@
       <c r="C122" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="F122" s="1" t="s">
+      <c r="D122" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="G122" s="1" t="s">
+      <c r="E122" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
       <c r="B123">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C123" s="8" t="s">
+        <v>565</v>
+      </c>
+      <c r="D123" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="F123" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="G123" s="1" t="s">
+      <c r="E123" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
@@ -4778,16 +4784,16 @@
         <v>8</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>531</v>
-      </c>
-      <c r="F124" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="G124" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E124" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
@@ -4795,16 +4801,16 @@
         <v>1</v>
       </c>
       <c r="C125" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="D125" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="F125" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="G125" s="1" t="s">
+      <c r="E125" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
@@ -4812,16 +4818,16 @@
         <v>1</v>
       </c>
       <c r="C126" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="D126" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="F126" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="G126" s="1" t="s">
+      <c r="E126" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
@@ -4829,16 +4835,16 @@
         <v>101</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>532</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="G127" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E127" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
@@ -4846,12 +4852,12 @@
         <v>1</v>
       </c>
       <c r="C128" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="D128" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="F128" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="G128" s="1" t="s">
+      <c r="E128" s="1" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4863,12 +4869,12 @@
         <v>1</v>
       </c>
       <c r="C129" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="D129" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="F129" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="G129" s="1" t="s">
+      <c r="E129" s="1" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4880,13 +4886,13 @@
         <v>1</v>
       </c>
       <c r="C130" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="D130" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="F130" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="G130" s="1" t="s">
-        <v>433</v>
+      <c r="E130" s="1" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
@@ -4897,12 +4903,12 @@
         <v>55</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>533</v>
-      </c>
-      <c r="F131" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="G131" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E131" s="1" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4914,12 +4920,12 @@
         <v>25</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>534</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="G132" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E132" s="1" t="s">
         <v>296</v>
       </c>
     </row>
@@ -4931,12 +4937,12 @@
         <v>6</v>
       </c>
       <c r="C133" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="D133" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="F133" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="G133" s="1" t="s">
+      <c r="E133" s="1" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4945,15 +4951,15 @@
         <v>133</v>
       </c>
       <c r="B134">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="F134" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="G134" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="E134" s="1" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4962,15 +4968,15 @@
         <v>134</v>
       </c>
       <c r="B135">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="F135" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="G135" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E135" s="1" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4982,12 +4988,12 @@
         <v>1</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="F136" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="G136" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E136" s="1" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4996,15 +5002,15 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>337</v>
-      </c>
-      <c r="F137" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="G137" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E137" s="1" t="s">
         <v>280</v>
       </c>
     </row>
@@ -5013,15 +5019,15 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="F138" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="G138" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="E138" s="1" t="s">
         <v>280</v>
       </c>
     </row>
@@ -5030,15 +5036,15 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>535</v>
-      </c>
-      <c r="F139" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="G139" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="E139" s="1" t="s">
         <v>280</v>
       </c>
     </row>
@@ -5047,51 +5053,44 @@
         <v>139</v>
       </c>
       <c r="B140" s="2">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>342</v>
+        <v>533</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>536</v>
+        <v>340</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>537</v>
-      </c>
-      <c r="F140" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="G140" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="H140" s="2" t="s">
-        <v>538</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="F140" s="3"/>
+      <c r="G140" s="3"/>
     </row>
     <row r="141" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2">
         <v>140</v>
       </c>
       <c r="B141" s="2">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>539</v>
+        <v>342</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>540</v>
+        <v>343</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>346</v>
+        <v>534</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>347</v>
+        <v>535</v>
       </c>
       <c r="H141" s="2" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.3">
@@ -5099,25 +5098,25 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>542</v>
+        <v>346</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>349</v>
+        <v>537</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>350</v>
+        <v>568</v>
       </c>
       <c r="H142" t="s">
-        <v>352</v>
+        <v>538</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.3">
@@ -5125,25 +5124,25 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>209</v>
+        <v>348</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>355</v>
+        <v>539</v>
       </c>
       <c r="H143" t="s">
-        <v>543</v>
+        <v>351</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
@@ -5151,25 +5150,25 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>462</v>
+        <v>354</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>357</v>
+        <v>209</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="H144" t="s">
-        <v>360</v>
+        <v>540</v>
       </c>
     </row>
     <row r="145" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5177,22 +5176,25 @@
         <v>144</v>
       </c>
       <c r="B145" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>463</v>
+        <v>357</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G145" s="3" t="s">
-        <v>344</v>
+        <v>569</v>
+      </c>
+      <c r="H145" s="2" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="146" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5200,25 +5202,22 @@
         <v>145</v>
       </c>
       <c r="B146" s="2">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>544</v>
+        <v>361</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>365</v>
+        <v>343</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="G146" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="H146" s="2" t="s">
-        <v>545</v>
+        <v>461</v>
       </c>
     </row>
     <row r="147" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5226,25 +5225,25 @@
         <v>146</v>
       </c>
       <c r="B147" s="2">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>544</v>
+        <v>364</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>546</v>
+        <v>365</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>368</v>
+        <v>541</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="H147" s="2" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
     </row>
     <row r="148" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5252,25 +5251,25 @@
         <v>147</v>
       </c>
       <c r="B148" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>548</v>
+        <v>366</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>550</v>
+        <v>367</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>551</v>
+        <v>368</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>370</v>
+        <v>543</v>
       </c>
       <c r="H148" s="2" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
     </row>
     <row r="149" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5278,25 +5277,25 @@
         <v>148</v>
       </c>
       <c r="B149" s="2">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>539</v>
+        <v>546</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>555</v>
+        <v>369</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="G149" s="3" t="s">
-        <v>370</v>
+        <v>548</v>
       </c>
       <c r="H149" s="2" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
     </row>
     <row r="150" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5304,25 +5303,25 @@
         <v>149</v>
       </c>
       <c r="B150" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>210</v>
+        <v>550</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>514</v>
+        <v>551</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>515</v>
+        <v>369</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>512</v>
+        <v>537</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>513</v>
+        <v>552</v>
       </c>
       <c r="H150" s="2" t="s">
-        <v>516</v>
+        <v>553</v>
       </c>
     </row>
     <row r="151" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5330,25 +5329,25 @@
         <v>150</v>
       </c>
       <c r="B151" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>371</v>
+        <v>210</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>466</v>
+        <v>510</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>466</v>
+        <v>511</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>372</v>
+        <v>512</v>
       </c>
       <c r="G151" s="3" t="s">
-        <v>372</v>
+        <v>513</v>
       </c>
       <c r="H151" s="2" t="s">
-        <v>557</v>
+        <v>514</v>
       </c>
     </row>
     <row r="152" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5356,25 +5355,25 @@
         <v>151</v>
       </c>
       <c r="B152" s="2">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>209</v>
+        <v>371</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>558</v>
+        <v>371</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>374</v>
+        <v>464</v>
       </c>
       <c r="G152" s="3" t="s">
-        <v>375</v>
+        <v>464</v>
       </c>
       <c r="H152" s="2" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
     </row>
     <row r="153" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5382,25 +5381,25 @@
         <v>152</v>
       </c>
       <c r="B153" s="2">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D153" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="F153" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="E153" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="F153" s="3" t="s">
-        <v>377</v>
-      </c>
       <c r="G153" s="3" t="s">
-        <v>375</v>
+        <v>555</v>
       </c>
       <c r="H153" s="2" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="154" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5408,25 +5407,25 @@
         <v>153</v>
       </c>
       <c r="B154" s="2">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C154" s="6" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>464</v>
+        <v>374</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>379</v>
+        <v>209</v>
       </c>
       <c r="G154" s="3" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="H154" s="2" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
     </row>
     <row r="155" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5434,25 +5433,25 @@
         <v>154</v>
       </c>
       <c r="B155" s="2">
-        <v>106</v>
+        <v>24</v>
       </c>
       <c r="C155" s="6" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>466</v>
+        <v>378</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>466</v>
+        <v>378</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="G155" s="3" t="s">
-        <v>383</v>
+        <v>462</v>
       </c>
       <c r="H155" s="2" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="156" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5460,25 +5459,25 @@
         <v>155</v>
       </c>
       <c r="B156" s="2">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="C156" s="6" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>465</v>
+        <v>381</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>385</v>
+        <v>464</v>
       </c>
       <c r="G156" s="3" t="s">
-        <v>386</v>
+        <v>464</v>
       </c>
       <c r="H156" s="2" t="s">
-        <v>387</v>
+        <v>559</v>
       </c>
     </row>
     <row r="157" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5486,25 +5485,25 @@
         <v>156</v>
       </c>
       <c r="B157" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C157" s="6" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>465</v>
+        <v>384</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>389</v>
+        <v>463</v>
       </c>
       <c r="G157" s="3" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="H157" s="2" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="158" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5512,25 +5511,25 @@
         <v>157</v>
       </c>
       <c r="B158" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C158" s="6" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>465</v>
+        <v>388</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="F158" s="3" t="s">
-        <v>393</v>
+        <v>463</v>
       </c>
       <c r="G158" s="3" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="H158" s="2" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
     </row>
     <row r="159" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5541,22 +5540,22 @@
         <v>1</v>
       </c>
       <c r="C159" s="6" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>465</v>
+        <v>392</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>563</v>
+        <v>393</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>393</v>
+        <v>463</v>
       </c>
       <c r="G159" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="H159" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="H159" s="2" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="160" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5567,22 +5566,22 @@
         <v>1</v>
       </c>
       <c r="C160" s="6" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>465</v>
+        <v>392</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="F160" s="3" t="s">
-        <v>399</v>
+        <v>463</v>
       </c>
       <c r="G160" s="3" t="s">
-        <v>400</v>
+        <v>560</v>
       </c>
       <c r="H160" s="2" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="161" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5593,22 +5592,22 @@
         <v>1</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>465</v>
+        <v>398</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="F161" s="3" t="s">
-        <v>403</v>
+        <v>463</v>
       </c>
       <c r="G161" s="3" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="H161" s="2" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="162" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5619,22 +5618,22 @@
         <v>1</v>
       </c>
       <c r="C162" s="6" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>564</v>
+        <v>402</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>565</v>
+        <v>403</v>
       </c>
       <c r="F162" s="3" t="s">
-        <v>407</v>
+        <v>463</v>
       </c>
       <c r="G162" s="3" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="H162" s="2" t="s">
-        <v>566</v>
+        <v>404</v>
       </c>
     </row>
     <row r="163" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5645,22 +5644,22 @@
         <v>1</v>
       </c>
       <c r="C163" s="6" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>517</v>
+        <v>406</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="F163" s="3" t="s">
-        <v>410</v>
+        <v>561</v>
       </c>
       <c r="G163" s="3" t="s">
-        <v>411</v>
+        <v>562</v>
       </c>
       <c r="H163" s="2" t="s">
-        <v>412</v>
+        <v>563</v>
       </c>
     </row>
     <row r="164" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5668,33 +5667,52 @@
         <v>163</v>
       </c>
       <c r="B164" s="2">
+        <v>1</v>
+      </c>
+      <c r="C164" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="F164" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="G164" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="H164" s="2" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="2">
+        <v>164</v>
+      </c>
+      <c r="B165" s="2">
         <v>7</v>
       </c>
-      <c r="C164" s="6" t="s">
+      <c r="C165" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="D165" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="D164" s="3" t="s">
-        <v>567</v>
-      </c>
-      <c r="E164" s="3" t="s">
+      <c r="E165" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="F164" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="G164" s="3" t="s">
+      <c r="F165" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="G165" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="H165" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="H164" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C165" s="6"/>
-      <c r="D165" s="3"/>
-      <c r="E165" s="3"/>
-      <c r="F165" s="3"/>
-      <c r="G165" s="3"/>
     </row>
     <row r="166" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C166" s="6"/>

</xml_diff>

<commit_message>
add final gerbers, XYRS, BOM
</commit_message>
<xml_diff>
--- a/radiant_bom.xlsx
+++ b/radiant_bom.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="720">
   <si>
     <t>Item</t>
   </si>
@@ -1571,9 +1572,6 @@
     <t>TP35</t>
   </si>
   <si>
-    <t>Test Point</t>
-  </si>
-  <si>
     <t>U40</t>
   </si>
   <si>
@@ -2136,6 +2134,57 @@
   </si>
   <si>
     <t>Customer Supplied</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>N1-N8</t>
+  </si>
+  <si>
+    <t>FIDUCIAL10-20</t>
+  </si>
+  <si>
+    <t>161</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>X49-X58</t>
+  </si>
+  <si>
+    <t>ALIGNMENT_HOLE</t>
+  </si>
+  <si>
+    <t>ALIGNHOLE2M5</t>
   </si>
 </sst>
 </file>
@@ -2473,10 +2522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H160"/>
+  <dimension ref="A1:H162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="A162" sqref="A162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3083,10 +3132,10 @@
         <v>117</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>562</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -3161,10 +3210,10 @@
         <v>93</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>564</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -3187,10 +3236,10 @@
         <v>93</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>566</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -3213,10 +3262,10 @@
         <v>227</v>
       </c>
       <c r="G28" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>568</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -3239,10 +3288,10 @@
         <v>227</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>570</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -3262,13 +3311,13 @@
         <v>92</v>
       </c>
       <c r="F30" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>573</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -3279,7 +3328,7 @@
         <v>10</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>137</v>
@@ -3291,10 +3340,10 @@
         <v>93</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>575</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3317,10 +3366,10 @@
         <v>93</v>
       </c>
       <c r="G32" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>577</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3343,10 +3392,10 @@
         <v>93</v>
       </c>
       <c r="G33" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>579</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3369,10 +3418,10 @@
         <v>93</v>
       </c>
       <c r="G34" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>582</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3395,10 +3444,10 @@
         <v>87</v>
       </c>
       <c r="G35" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>584</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3421,10 +3470,10 @@
         <v>227</v>
       </c>
       <c r="G36" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>586</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3435,7 +3484,7 @@
         <v>7</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>148</v>
@@ -3447,10 +3496,10 @@
         <v>93</v>
       </c>
       <c r="G37" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>589</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3473,10 +3522,10 @@
         <v>227</v>
       </c>
       <c r="G38" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>591</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3499,10 +3548,10 @@
         <v>93</v>
       </c>
       <c r="G39" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>593</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3525,10 +3574,10 @@
         <v>227</v>
       </c>
       <c r="G40" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>595</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -3551,10 +3600,10 @@
         <v>93</v>
       </c>
       <c r="G41" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>597</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3577,10 +3626,10 @@
         <v>120</v>
       </c>
       <c r="G42" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>621</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -3594,7 +3643,7 @@
         <v>165</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>116</v>
@@ -3603,10 +3652,10 @@
         <v>87</v>
       </c>
       <c r="G43" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>600</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -3629,10 +3678,10 @@
         <v>111</v>
       </c>
       <c r="G44" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>623</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3655,10 +3704,10 @@
         <v>87</v>
       </c>
       <c r="G45" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>625</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3681,10 +3730,10 @@
         <v>227</v>
       </c>
       <c r="G46" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>602</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3707,10 +3756,10 @@
         <v>227</v>
       </c>
       <c r="G47" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>604</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3733,10 +3782,10 @@
         <v>120</v>
       </c>
       <c r="G48" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="H48" s="1" t="s">
         <v>606</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -3759,10 +3808,10 @@
         <v>111</v>
       </c>
       <c r="G49" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>608</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -3785,10 +3834,10 @@
         <v>93</v>
       </c>
       <c r="G50" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>610</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -3811,10 +3860,10 @@
         <v>227</v>
       </c>
       <c r="G51" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>612</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -3837,10 +3886,10 @@
         <v>93</v>
       </c>
       <c r="G52" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>614</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -4388,13 +4437,13 @@
         <v>265</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -5029,13 +5078,13 @@
         <v>380</v>
       </c>
       <c r="F99" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="G99" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="G99" s="1" t="s">
+      <c r="H99" s="1" t="s">
         <v>628</v>
-      </c>
-      <c r="H99" s="1" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -5081,13 +5130,13 @@
         <v>380</v>
       </c>
       <c r="F101" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="G101" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="G101" s="1" t="s">
+      <c r="H101" s="1" t="s">
         <v>631</v>
-      </c>
-      <c r="H101" s="1" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -5098,10 +5147,10 @@
         <v>6</v>
       </c>
       <c r="C102" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>633</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>634</v>
       </c>
       <c r="E102" s="1">
         <v>603</v>
@@ -5110,10 +5159,10 @@
         <v>19</v>
       </c>
       <c r="G102" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="H102" s="1" t="s">
         <v>635</v>
-      </c>
-      <c r="H102" s="1" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -5133,13 +5182,13 @@
         <v>380</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G103" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="H103" s="1" t="s">
         <v>637</v>
-      </c>
-      <c r="H103" s="1" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -5150,7 +5199,7 @@
         <v>247</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>389</v>
@@ -5159,13 +5208,13 @@
         <v>380</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G104" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="H104" s="1" t="s">
         <v>639</v>
-      </c>
-      <c r="H104" s="1" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -5185,13 +5234,13 @@
         <v>380</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G105" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="H105" s="1" t="s">
         <v>680</v>
-      </c>
-      <c r="H105" s="1" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -5202,7 +5251,7 @@
         <v>3</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>392</v>
@@ -5211,13 +5260,13 @@
         <v>380</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G106" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="H106" s="1" t="s">
         <v>643</v>
-      </c>
-      <c r="H106" s="1" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -5237,13 +5286,13 @@
         <v>603</v>
       </c>
       <c r="F107" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="G107" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="G107" s="1" t="s">
+      <c r="H107" s="1" t="s">
         <v>646</v>
-      </c>
-      <c r="H107" s="1" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -5263,13 +5312,13 @@
         <v>380</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G108" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="H108" s="1" t="s">
         <v>648</v>
-      </c>
-      <c r="H108" s="1" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -5289,13 +5338,13 @@
         <v>380</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G109" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="H109" s="1" t="s">
         <v>650</v>
-      </c>
-      <c r="H109" s="1" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -5315,13 +5364,13 @@
         <v>380</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G110" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="H110" s="1" t="s">
         <v>652</v>
-      </c>
-      <c r="H110" s="1" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -5341,13 +5390,13 @@
         <v>380</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G111" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="H111" s="1" t="s">
         <v>654</v>
-      </c>
-      <c r="H111" s="1" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -5367,13 +5416,13 @@
         <v>380</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G112" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="H112" s="1" t="s">
         <v>656</v>
-      </c>
-      <c r="H112" s="1" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -5393,13 +5442,13 @@
         <v>380</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G113" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="H113" s="1" t="s">
         <v>658</v>
-      </c>
-      <c r="H113" s="1" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -5419,13 +5468,13 @@
         <v>380</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G114" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="H114" s="1" t="s">
         <v>660</v>
-      </c>
-      <c r="H114" s="1" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -5445,13 +5494,13 @@
         <v>603</v>
       </c>
       <c r="F115" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="G115" s="1" t="s">
         <v>662</v>
       </c>
-      <c r="G115" s="1" t="s">
+      <c r="H115" s="1" t="s">
         <v>663</v>
-      </c>
-      <c r="H115" s="1" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -5462,7 +5511,7 @@
         <v>26</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>413</v>
@@ -5471,13 +5520,13 @@
         <v>380</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G116" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="H116" s="1" t="s">
         <v>666</v>
-      </c>
-      <c r="H116" s="1" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -5488,7 +5537,7 @@
         <v>1</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>414</v>
@@ -5497,13 +5546,13 @@
         <v>380</v>
       </c>
       <c r="F117" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="G117" s="1" t="s">
         <v>668</v>
       </c>
-      <c r="G117" s="1" t="s">
+      <c r="H117" s="1" t="s">
         <v>669</v>
-      </c>
-      <c r="H117" s="1" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -5523,13 +5572,13 @@
         <v>380</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G118" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="H118" s="1" t="s">
         <v>671</v>
-      </c>
-      <c r="H118" s="1" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -5540,7 +5589,7 @@
         <v>2</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>417</v>
@@ -5549,13 +5598,13 @@
         <v>380</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G119" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="H119" s="1" t="s">
         <v>673</v>
-      </c>
-      <c r="H119" s="1" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -5575,13 +5624,13 @@
         <v>380</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G120" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="H120" s="1" t="s">
         <v>675</v>
-      </c>
-      <c r="H120" s="1" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -5601,13 +5650,13 @@
         <v>402</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G121" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="H121" s="1" t="s">
         <v>675</v>
-      </c>
-      <c r="H121" s="1" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -5618,7 +5667,7 @@
         <v>102</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>420</v>
@@ -5627,13 +5676,13 @@
         <v>380</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G122" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="H122" s="1" t="s">
         <v>678</v>
-      </c>
-      <c r="H122" s="1" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -5653,13 +5702,13 @@
         <v>380</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G123" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="H123" s="1" t="s">
         <v>683</v>
-      </c>
-      <c r="H123" s="1" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -5679,13 +5728,13 @@
         <v>603</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="G124" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="H124" s="1" t="s">
         <v>685</v>
-      </c>
-      <c r="H124" s="1" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -5705,13 +5754,13 @@
         <v>380</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G125" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="H125" s="1" t="s">
         <v>687</v>
-      </c>
-      <c r="H125" s="1" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -5722,22 +5771,22 @@
         <v>25</v>
       </c>
       <c r="C126" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="D126" s="1" t="s">
         <v>689</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>690</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>402</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G126" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="H126" s="1" t="s">
         <v>691</v>
-      </c>
-      <c r="H126" s="1" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -5757,13 +5806,13 @@
         <v>380</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G127" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="H127" s="1" t="s">
         <v>693</v>
-      </c>
-      <c r="H127" s="1" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -5774,22 +5823,22 @@
         <v>1</v>
       </c>
       <c r="C128" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="D128" s="1" t="s">
         <v>618</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>619</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>380</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G128" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="H128" s="1" t="s">
         <v>695</v>
-      </c>
-      <c r="H128" s="1" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -5809,13 +5858,13 @@
         <v>380</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G129" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="H129" s="1" t="s">
         <v>695</v>
-      </c>
-      <c r="H129" s="1" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -5835,13 +5884,13 @@
         <v>380</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G130" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="H130" s="1" t="s">
         <v>697</v>
-      </c>
-      <c r="H130" s="1" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -5861,13 +5910,13 @@
         <v>380</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G131" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="H131" s="1" t="s">
         <v>699</v>
-      </c>
-      <c r="H131" s="1" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -5887,13 +5936,13 @@
         <v>380</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G132" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="H132" s="1" t="s">
         <v>701</v>
-      </c>
-      <c r="H132" s="1" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -5904,7 +5953,7 @@
         <v>89</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>437</v>
@@ -6332,7 +6381,7 @@
         <v>200</v>
       </c>
       <c r="H149" s="1" t="s">
-        <v>515</v>
+        <v>200</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -6343,22 +6392,22 @@
         <v>1</v>
       </c>
       <c r="C150" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="D150" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="D150" s="1" t="s">
+      <c r="E150" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G150" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="H150" s="1" t="s">
         <v>518</v>
-      </c>
-      <c r="H150" s="1" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -6369,22 +6418,22 @@
         <v>1</v>
       </c>
       <c r="C151" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="D151" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="D151" s="1" t="s">
+      <c r="E151" s="1" t="s">
         <v>521</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>522</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H151" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -6395,22 +6444,22 @@
         <v>1</v>
       </c>
       <c r="C152" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="E152" s="1" t="s">
         <v>524</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="E152" s="1" t="s">
-        <v>525</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H152" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -6421,22 +6470,22 @@
         <v>1</v>
       </c>
       <c r="C153" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D153" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="D153" s="1" t="s">
+      <c r="E153" s="1" t="s">
         <v>527</v>
-      </c>
-      <c r="E153" s="1" t="s">
-        <v>528</v>
       </c>
       <c r="F153" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="H153" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -6447,22 +6496,22 @@
         <v>1</v>
       </c>
       <c r="C154" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="E154" s="1" t="s">
         <v>530</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="E154" s="1" t="s">
-        <v>531</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G154" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="H154" s="1" t="s">
         <v>532</v>
-      </c>
-      <c r="H154" s="1" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -6473,22 +6522,22 @@
         <v>1</v>
       </c>
       <c r="C155" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="D155" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="D155" s="1" t="s">
+      <c r="E155" s="1" t="s">
         <v>535</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>536</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H155" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -6499,22 +6548,22 @@
         <v>1</v>
       </c>
       <c r="C156" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="D156" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="D156" s="1" t="s">
+      <c r="E156" s="1" t="s">
         <v>539</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>540</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H156" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
@@ -6525,22 +6574,22 @@
         <v>1</v>
       </c>
       <c r="C157" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="D157" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="D157" s="1" t="s">
+      <c r="E157" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="E157" s="1" t="s">
+      <c r="F157" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="F157" s="1" t="s">
+      <c r="G157" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="G157" s="1" t="s">
+      <c r="H157" s="1" t="s">
         <v>546</v>
-      </c>
-      <c r="H157" s="1" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -6551,22 +6600,22 @@
         <v>1</v>
       </c>
       <c r="C158" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="D158" s="1" t="s">
         <v>548</v>
       </c>
-      <c r="D158" s="1" t="s">
+      <c r="E158" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="E158" s="1" t="s">
+      <c r="F158" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="F158" s="1" t="s">
+      <c r="G158" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="G158" s="1" t="s">
+      <c r="H158" s="1" t="s">
         <v>552</v>
-      </c>
-      <c r="H158" s="1" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -6577,22 +6626,22 @@
         <v>1</v>
       </c>
       <c r="C159" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="D159" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="D159" s="1" t="s">
+      <c r="E159" s="1" t="s">
         <v>555</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>556</v>
       </c>
       <c r="F159" s="1" t="s">
         <v>354</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H159" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -6603,26 +6652,122 @@
         <v>7</v>
       </c>
       <c r="C160" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="D160" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="D160" s="1" t="s">
+      <c r="E160" s="1" t="s">
         <v>559</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>560</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H160" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G161" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="H161" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G162" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="H162" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>703</v>
+      </c>
+      <c r="B1" t="s">
+        <v>704</v>
+      </c>
+      <c r="C1" t="s">
+        <v>705</v>
+      </c>
+      <c r="D1" t="s">
+        <v>706</v>
+      </c>
+      <c r="E1" t="s">
+        <v>707</v>
+      </c>
+      <c r="F1" t="s">
+        <v>708</v>
+      </c>
+      <c r="G1" t="s">
+        <v>709</v>
+      </c>
+      <c r="H1" t="s">
+        <v>710</v>
+      </c>
+      <c r="I1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix missing pullups on the missing aux CPLD INITs
</commit_message>
<xml_diff>
--- a/radiant_bom.xlsx
+++ b/radiant_bom.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="712">
   <si>
     <t>Item</t>
   </si>
@@ -1308,9 +1308,6 @@
     <t>RESISTOR,49.9</t>
   </si>
   <si>
-    <t>R77 R695 R871 R873 R875 R877 R879</t>
-  </si>
-  <si>
     <t>RESISTOR,49.9k</t>
   </si>
   <si>
@@ -1536,6 +1533,9 @@
     <t>PL-008</t>
   </si>
   <si>
+    <t>TCD-10-4X+</t>
+  </si>
+  <si>
     <t>Directional Couplers, Surface Mount, 6 to 30 dB Coupling , Up To 10 Watts, 2 MHz to 6000 MHz</t>
   </si>
   <si>
@@ -2130,9 +2130,6 @@
     <t>909 Ohms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Moisture Resistant Thick Film</t>
   </si>
   <si>
-    <t>Customer Supplied</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -2157,34 +2154,13 @@
     <t>J10</t>
   </si>
   <si>
-    <t>160</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>N1-N8</t>
-  </si>
-  <si>
-    <t>FIDUCIAL10-20</t>
-  </si>
-  <si>
-    <t>161</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>X49-X58</t>
-  </si>
-  <si>
-    <t>ALIGNMENT_HOLE</t>
-  </si>
-  <si>
-    <t>ALIGNHOLE2M5</t>
-  </si>
-  <si>
-    <t>TCD-10-1WX+</t>
+    <t>J22-23</t>
+  </si>
+  <si>
+    <t>R77 R695 R871 R873 R875 R877 R879 R882-883</t>
+  </si>
+  <si>
+    <t>Test Point</t>
   </si>
 </sst>
 </file>
@@ -2522,10 +2498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H162"/>
+  <dimension ref="A1:H160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="G147" sqref="G147"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4174,10 +4150,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>229</v>
+        <v>709</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>230</v>
@@ -4436,15 +4412,6 @@
       <c r="E74" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="F74" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="H74" s="1" t="s">
-        <v>701</v>
-      </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
@@ -5794,13 +5761,13 @@
         <v>126</v>
       </c>
       <c r="B127" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C127" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="D127" s="1" t="s">
         <v>427</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>428</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>380</v>
@@ -5849,10 +5816,10 @@
         <v>2</v>
       </c>
       <c r="C129" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D129" s="1" t="s">
         <v>429</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>430</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>380</v>
@@ -5875,10 +5842,10 @@
         <v>1</v>
       </c>
       <c r="C130" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="D130" s="1" t="s">
         <v>431</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>432</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>380</v>
@@ -5901,10 +5868,10 @@
         <v>2</v>
       </c>
       <c r="C131" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D131" s="1" t="s">
         <v>433</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>434</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>380</v>
@@ -5927,10 +5894,10 @@
         <v>1</v>
       </c>
       <c r="C132" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="D132" s="1" t="s">
         <v>435</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>436</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>380</v>
@@ -5956,7 +5923,7 @@
         <v>618</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>380</v>
@@ -5965,9 +5932,6 @@
         <v>200</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="H133" s="1" t="s">
         <v>200</v>
       </c>
     </row>
@@ -5979,22 +5943,22 @@
         <v>48</v>
       </c>
       <c r="C134" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="D134" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="D134" s="1" t="s">
+      <c r="E134" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="E134" s="1" t="s">
+      <c r="F134" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="F134" s="1" t="s">
+      <c r="G134" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="G134" s="1" t="s">
+      <c r="H134" s="1" t="s">
         <v>442</v>
-      </c>
-      <c r="H134" s="1" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -6005,22 +5969,22 @@
         <v>66</v>
       </c>
       <c r="C135" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="D135" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="D135" s="1" t="s">
+      <c r="E135" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="E135" s="1" t="s">
+      <c r="F135" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="F135" s="1" t="s">
+      <c r="G135" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="G135" s="1" t="s">
+      <c r="H135" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="H135" s="1" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -6031,22 +5995,22 @@
         <v>1</v>
       </c>
       <c r="C136" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="D136" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="D136" s="1" t="s">
+      <c r="E136" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="E136" s="1" t="s">
+      <c r="F136" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="F136" s="1" t="s">
+      <c r="G136" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="G136" s="1" t="s">
+      <c r="H136" s="1" t="s">
         <v>454</v>
-      </c>
-      <c r="H136" s="1" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -6057,22 +6021,22 @@
         <v>6</v>
       </c>
       <c r="C137" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D137" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="D137" s="1" t="s">
+      <c r="E137" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="E137" s="1" t="s">
+      <c r="F137" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="F137" s="1" t="s">
+      <c r="G137" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="H137" s="1" t="s">
         <v>459</v>
-      </c>
-      <c r="G137" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="H137" s="1" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -6083,22 +6047,22 @@
         <v>1</v>
       </c>
       <c r="C138" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="D138" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="D138" s="1" t="s">
+      <c r="E138" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="E138" s="1" t="s">
+      <c r="F138" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="F138" s="1" t="s">
+      <c r="G138" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="G138" s="1" t="s">
+      <c r="H138" s="1" t="s">
         <v>465</v>
-      </c>
-      <c r="H138" s="1" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -6109,19 +6073,19 @@
         <v>2</v>
       </c>
       <c r="C139" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="D139" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="D139" s="1" t="s">
+      <c r="E139" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F139" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="E139" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="F139" s="1" t="s">
+      <c r="G139" s="1" t="s">
         <v>469</v>
-      </c>
-      <c r="G139" s="1" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -6132,22 +6096,22 @@
         <v>30</v>
       </c>
       <c r="C140" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D140" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="D140" s="1" t="s">
+      <c r="E140" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="E140" s="1" t="s">
+      <c r="F140" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="F140" s="1" t="s">
+      <c r="G140" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="H140" s="1" t="s">
         <v>474</v>
-      </c>
-      <c r="G140" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="H140" s="1" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -6158,22 +6122,22 @@
         <v>24</v>
       </c>
       <c r="C141" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="D141" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="D141" s="1" t="s">
+      <c r="E141" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="E141" s="1" t="s">
+      <c r="F141" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="G141" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="F141" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="G141" s="1" t="s">
+      <c r="H141" s="1" t="s">
         <v>479</v>
-      </c>
-      <c r="H141" s="1" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
@@ -6184,22 +6148,22 @@
         <v>23</v>
       </c>
       <c r="C142" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="D142" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="D142" s="1" t="s">
+      <c r="E142" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="E142" s="1" t="s">
+      <c r="F142" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="F142" s="1" t="s">
+      <c r="G142" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="G142" s="1" t="s">
+      <c r="H142" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="H142" s="1" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -6210,22 +6174,22 @@
         <v>7</v>
       </c>
       <c r="C143" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="D143" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="D143" s="1" t="s">
+      <c r="E143" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="G143" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="E143" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="F143" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="G143" s="1" t="s">
+      <c r="H143" s="1" t="s">
         <v>489</v>
-      </c>
-      <c r="H143" s="1" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -6236,22 +6200,22 @@
         <v>1</v>
       </c>
       <c r="C144" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="D144" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="D144" s="1" t="s">
+      <c r="E144" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="E144" s="1" t="s">
+      <c r="F144" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="F144" s="1" t="s">
+      <c r="G144" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="G144" s="1" t="s">
+      <c r="H144" s="1" t="s">
         <v>495</v>
-      </c>
-      <c r="H144" s="1" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -6262,13 +6226,13 @@
         <v>2</v>
       </c>
       <c r="C145" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D145" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="D145" s="1" t="s">
-        <v>498</v>
-      </c>
       <c r="E145" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F145" s="1" t="s">
         <v>200</v>
@@ -6277,7 +6241,7 @@
         <v>200</v>
       </c>
       <c r="H145" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
@@ -6288,19 +6252,19 @@
         <v>24</v>
       </c>
       <c r="C146" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="D146" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="D146" s="1" t="s">
+      <c r="E146" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="E146" s="1" t="s">
+      <c r="F146" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="G146" t="s">
         <v>502</v>
-      </c>
-      <c r="F146" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="G146" t="s">
-        <v>719</v>
       </c>
       <c r="H146" s="1" t="s">
         <v>503</v>
@@ -6320,10 +6284,10 @@
         <v>505</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G147" s="1" t="s">
         <v>505</v>
@@ -6381,7 +6345,7 @@
         <v>200</v>
       </c>
       <c r="H149" s="1" t="s">
-        <v>200</v>
+        <v>711</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -6668,58 +6632,6 @@
       </c>
       <c r="H160" s="1" t="s">
         <v>559</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A161" s="1" t="s">
-        <v>710</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>711</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>712</v>
-      </c>
-      <c r="D161" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="F161" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="G161" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="H161" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A162" s="1" t="s">
-        <v>714</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>715</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>716</v>
-      </c>
-      <c r="D162" s="1" t="s">
-        <v>717</v>
-      </c>
-      <c r="E162" s="1" t="s">
-        <v>718</v>
-      </c>
-      <c r="F162" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="G162" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="H162" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -6740,28 +6652,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B1" t="s">
         <v>702</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>703</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>704</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>705</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>706</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>707</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>708</v>
-      </c>
-      <c r="H1" t="s">
-        <v>709</v>
       </c>
       <c r="I1" t="s">
         <v>229</v>

</xml_diff>

<commit_message>
add missing pin 1 indicator on board manager
</commit_message>
<xml_diff>
--- a/radiant_bom.xlsx
+++ b/radiant_bom.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="713">
   <si>
     <t>Item</t>
   </si>
@@ -1533,9 +1533,6 @@
     <t>PL-008</t>
   </si>
   <si>
-    <t>TCD-10-4X+</t>
-  </si>
-  <si>
     <t>Directional Couplers, Surface Mount, 6 to 30 dB Coupling , Up To 10 Watts, 2 MHz to 6000 MHz</t>
   </si>
   <si>
@@ -2161,6 +2158,12 @@
   </si>
   <si>
     <t>Test Point</t>
+  </si>
+  <si>
+    <t>Customer Supplied</t>
+  </si>
+  <si>
+    <t>TCD-10-1WX+</t>
   </si>
 </sst>
 </file>
@@ -2500,8 +2503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="F147" sqref="F147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3108,10 +3111,10 @@
         <v>117</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>560</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -3186,10 +3189,10 @@
         <v>93</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>562</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -3212,10 +3215,10 @@
         <v>93</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>564</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -3238,10 +3241,10 @@
         <v>227</v>
       </c>
       <c r="G28" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>566</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -3264,10 +3267,10 @@
         <v>227</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>568</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -3287,13 +3290,13 @@
         <v>92</v>
       </c>
       <c r="F30" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>571</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -3304,7 +3307,7 @@
         <v>10</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>137</v>
@@ -3316,10 +3319,10 @@
         <v>93</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>573</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3342,10 +3345,10 @@
         <v>93</v>
       </c>
       <c r="G32" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>575</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3368,10 +3371,10 @@
         <v>93</v>
       </c>
       <c r="G33" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>577</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3394,10 +3397,10 @@
         <v>93</v>
       </c>
       <c r="G34" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>580</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3420,10 +3423,10 @@
         <v>87</v>
       </c>
       <c r="G35" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>582</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3446,10 +3449,10 @@
         <v>227</v>
       </c>
       <c r="G36" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>584</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3460,7 +3463,7 @@
         <v>7</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>148</v>
@@ -3472,10 +3475,10 @@
         <v>93</v>
       </c>
       <c r="G37" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>587</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3498,10 +3501,10 @@
         <v>227</v>
       </c>
       <c r="G38" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>589</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3524,10 +3527,10 @@
         <v>93</v>
       </c>
       <c r="G39" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>591</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3550,10 +3553,10 @@
         <v>227</v>
       </c>
       <c r="G40" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>593</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -3576,10 +3579,10 @@
         <v>93</v>
       </c>
       <c r="G41" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>595</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3602,10 +3605,10 @@
         <v>120</v>
       </c>
       <c r="G42" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>619</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -3619,7 +3622,7 @@
         <v>165</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>116</v>
@@ -3628,10 +3631,10 @@
         <v>87</v>
       </c>
       <c r="G43" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>598</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -3654,10 +3657,10 @@
         <v>111</v>
       </c>
       <c r="G44" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>621</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3680,10 +3683,10 @@
         <v>87</v>
       </c>
       <c r="G45" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>623</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3706,10 +3709,10 @@
         <v>227</v>
       </c>
       <c r="G46" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>600</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3732,10 +3735,10 @@
         <v>227</v>
       </c>
       <c r="G47" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>602</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3758,10 +3761,10 @@
         <v>120</v>
       </c>
       <c r="G48" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="H48" s="1" t="s">
         <v>604</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -3784,10 +3787,10 @@
         <v>111</v>
       </c>
       <c r="G49" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>606</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -3810,10 +3813,10 @@
         <v>93</v>
       </c>
       <c r="G50" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>608</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -3836,10 +3839,10 @@
         <v>227</v>
       </c>
       <c r="G51" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>610</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -3862,10 +3865,10 @@
         <v>93</v>
       </c>
       <c r="G52" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>612</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -4153,7 +4156,7 @@
         <v>2</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>230</v>
@@ -4412,6 +4415,15 @@
       <c r="E74" s="1" t="s">
         <v>265</v>
       </c>
+      <c r="F74" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>711</v>
+      </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
@@ -5045,13 +5057,13 @@
         <v>380</v>
       </c>
       <c r="F99" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="G99" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="G99" s="1" t="s">
+      <c r="H99" s="1" t="s">
         <v>626</v>
-      </c>
-      <c r="H99" s="1" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -5097,13 +5109,13 @@
         <v>380</v>
       </c>
       <c r="F101" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="G101" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="G101" s="1" t="s">
+      <c r="H101" s="1" t="s">
         <v>629</v>
-      </c>
-      <c r="H101" s="1" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -5114,10 +5126,10 @@
         <v>6</v>
       </c>
       <c r="C102" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>631</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>632</v>
       </c>
       <c r="E102" s="1">
         <v>603</v>
@@ -5126,10 +5138,10 @@
         <v>19</v>
       </c>
       <c r="G102" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="H102" s="1" t="s">
         <v>633</v>
-      </c>
-      <c r="H102" s="1" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -5149,13 +5161,13 @@
         <v>380</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G103" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="H103" s="1" t="s">
         <v>635</v>
-      </c>
-      <c r="H103" s="1" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -5166,7 +5178,7 @@
         <v>247</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>389</v>
@@ -5175,13 +5187,13 @@
         <v>380</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G104" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="H104" s="1" t="s">
         <v>637</v>
-      </c>
-      <c r="H104" s="1" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -5201,13 +5213,13 @@
         <v>380</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G105" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="H105" s="1" t="s">
         <v>678</v>
-      </c>
-      <c r="H105" s="1" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -5218,7 +5230,7 @@
         <v>3</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>392</v>
@@ -5227,13 +5239,13 @@
         <v>380</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G106" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="H106" s="1" t="s">
         <v>641</v>
-      </c>
-      <c r="H106" s="1" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -5253,13 +5265,13 @@
         <v>603</v>
       </c>
       <c r="F107" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="G107" s="1" t="s">
         <v>643</v>
       </c>
-      <c r="G107" s="1" t="s">
+      <c r="H107" s="1" t="s">
         <v>644</v>
-      </c>
-      <c r="H107" s="1" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -5279,13 +5291,13 @@
         <v>380</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G108" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="H108" s="1" t="s">
         <v>646</v>
-      </c>
-      <c r="H108" s="1" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -5305,13 +5317,13 @@
         <v>380</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G109" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="H109" s="1" t="s">
         <v>648</v>
-      </c>
-      <c r="H109" s="1" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -5331,13 +5343,13 @@
         <v>380</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G110" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="H110" s="1" t="s">
         <v>650</v>
-      </c>
-      <c r="H110" s="1" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -5357,13 +5369,13 @@
         <v>380</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G111" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="H111" s="1" t="s">
         <v>652</v>
-      </c>
-      <c r="H111" s="1" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -5383,13 +5395,13 @@
         <v>380</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G112" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="H112" s="1" t="s">
         <v>654</v>
-      </c>
-      <c r="H112" s="1" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -5409,13 +5421,13 @@
         <v>380</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G113" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="H113" s="1" t="s">
         <v>656</v>
-      </c>
-      <c r="H113" s="1" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -5435,13 +5447,13 @@
         <v>380</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G114" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="H114" s="1" t="s">
         <v>658</v>
-      </c>
-      <c r="H114" s="1" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -5461,13 +5473,13 @@
         <v>603</v>
       </c>
       <c r="F115" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="G115" s="1" t="s">
         <v>660</v>
       </c>
-      <c r="G115" s="1" t="s">
+      <c r="H115" s="1" t="s">
         <v>661</v>
-      </c>
-      <c r="H115" s="1" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -5478,7 +5490,7 @@
         <v>26</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>413</v>
@@ -5487,13 +5499,13 @@
         <v>380</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G116" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="H116" s="1" t="s">
         <v>664</v>
-      </c>
-      <c r="H116" s="1" t="s">
-        <v>665</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -5504,7 +5516,7 @@
         <v>1</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>414</v>
@@ -5513,13 +5525,13 @@
         <v>380</v>
       </c>
       <c r="F117" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="G117" s="1" t="s">
         <v>666</v>
       </c>
-      <c r="G117" s="1" t="s">
+      <c r="H117" s="1" t="s">
         <v>667</v>
-      </c>
-      <c r="H117" s="1" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -5539,13 +5551,13 @@
         <v>380</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G118" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="H118" s="1" t="s">
         <v>669</v>
-      </c>
-      <c r="H118" s="1" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -5556,7 +5568,7 @@
         <v>2</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>417</v>
@@ -5565,13 +5577,13 @@
         <v>380</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G119" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="H119" s="1" t="s">
         <v>671</v>
-      </c>
-      <c r="H119" s="1" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -5591,13 +5603,13 @@
         <v>380</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G120" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="H120" s="1" t="s">
         <v>673</v>
-      </c>
-      <c r="H120" s="1" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -5617,13 +5629,13 @@
         <v>402</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G121" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="H121" s="1" t="s">
         <v>673</v>
-      </c>
-      <c r="H121" s="1" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -5634,7 +5646,7 @@
         <v>102</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>420</v>
@@ -5643,13 +5655,13 @@
         <v>380</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G122" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="H122" s="1" t="s">
         <v>676</v>
-      </c>
-      <c r="H122" s="1" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -5669,13 +5681,13 @@
         <v>380</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G123" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="H123" s="1" t="s">
         <v>681</v>
-      </c>
-      <c r="H123" s="1" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -5695,13 +5707,13 @@
         <v>603</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G124" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="H124" s="1" t="s">
         <v>683</v>
-      </c>
-      <c r="H124" s="1" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -5721,13 +5733,13 @@
         <v>380</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G125" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="H125" s="1" t="s">
         <v>685</v>
-      </c>
-      <c r="H125" s="1" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -5738,22 +5750,22 @@
         <v>25</v>
       </c>
       <c r="C126" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="D126" s="1" t="s">
         <v>687</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>688</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>402</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G126" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="H126" s="1" t="s">
         <v>689</v>
-      </c>
-      <c r="H126" s="1" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -5764,7 +5776,7 @@
         <v>9</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>427</v>
@@ -5773,13 +5785,13 @@
         <v>380</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G127" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="H127" s="1" t="s">
         <v>691</v>
-      </c>
-      <c r="H127" s="1" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -5790,22 +5802,22 @@
         <v>1</v>
       </c>
       <c r="C128" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="D128" s="1" t="s">
         <v>616</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>617</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>380</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G128" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="H128" s="1" t="s">
         <v>693</v>
-      </c>
-      <c r="H128" s="1" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -5825,13 +5837,13 @@
         <v>380</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G129" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="H129" s="1" t="s">
         <v>693</v>
-      </c>
-      <c r="H129" s="1" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -5851,13 +5863,13 @@
         <v>380</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G130" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="H130" s="1" t="s">
         <v>695</v>
-      </c>
-      <c r="H130" s="1" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -5877,13 +5889,13 @@
         <v>380</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G131" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="H131" s="1" t="s">
         <v>697</v>
-      </c>
-      <c r="H131" s="1" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -5903,13 +5915,13 @@
         <v>380</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G132" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="H132" s="1" t="s">
         <v>699</v>
-      </c>
-      <c r="H132" s="1" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -5920,7 +5932,7 @@
         <v>89</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>436</v>
@@ -6264,10 +6276,10 @@
         <v>458</v>
       </c>
       <c r="G146" t="s">
+        <v>712</v>
+      </c>
+      <c r="H146" s="1" t="s">
         <v>502</v>
-      </c>
-      <c r="H146" s="1" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -6278,10 +6290,10 @@
         <v>1</v>
       </c>
       <c r="C147" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="D147" s="1" t="s">
         <v>504</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>505</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>501</v>
@@ -6290,10 +6302,10 @@
         <v>458</v>
       </c>
       <c r="G147" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="H147" s="1" t="s">
         <v>505</v>
-      </c>
-      <c r="H147" s="1" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
@@ -6304,22 +6316,22 @@
         <v>24</v>
       </c>
       <c r="C148" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="D148" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="D148" s="1" t="s">
-        <v>508</v>
-      </c>
       <c r="E148" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>111</v>
       </c>
       <c r="G148" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="H148" s="1" t="s">
         <v>509</v>
-      </c>
-      <c r="H148" s="1" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -6330,13 +6342,13 @@
         <v>125</v>
       </c>
       <c r="C149" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="D149" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="D149" s="1" t="s">
+      <c r="E149" s="1" t="s">
         <v>512</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>513</v>
       </c>
       <c r="F149" s="1" t="s">
         <v>200</v>
@@ -6345,7 +6357,7 @@
         <v>200</v>
       </c>
       <c r="H149" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -6356,22 +6368,22 @@
         <v>1</v>
       </c>
       <c r="C150" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D150" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D150" s="1" t="s">
+      <c r="E150" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G150" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="H150" s="1" t="s">
         <v>516</v>
-      </c>
-      <c r="H150" s="1" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -6382,22 +6394,22 @@
         <v>1</v>
       </c>
       <c r="C151" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="D151" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="D151" s="1" t="s">
+      <c r="E151" s="1" t="s">
         <v>519</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>520</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H151" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -6408,22 +6420,22 @@
         <v>1</v>
       </c>
       <c r="C152" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="E152" s="1" t="s">
         <v>522</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="E152" s="1" t="s">
-        <v>523</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H152" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -6434,22 +6446,22 @@
         <v>1</v>
       </c>
       <c r="C153" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="D153" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="D153" s="1" t="s">
+      <c r="E153" s="1" t="s">
         <v>525</v>
-      </c>
-      <c r="E153" s="1" t="s">
-        <v>526</v>
       </c>
       <c r="F153" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H153" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -6460,22 +6472,22 @@
         <v>1</v>
       </c>
       <c r="C154" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="E154" s="1" t="s">
         <v>528</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="E154" s="1" t="s">
-        <v>529</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G154" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="H154" s="1" t="s">
         <v>530</v>
-      </c>
-      <c r="H154" s="1" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -6486,22 +6498,22 @@
         <v>1</v>
       </c>
       <c r="C155" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="D155" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="D155" s="1" t="s">
+      <c r="E155" s="1" t="s">
         <v>533</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>534</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="H155" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -6512,22 +6524,22 @@
         <v>1</v>
       </c>
       <c r="C156" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="D156" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="D156" s="1" t="s">
+      <c r="E156" s="1" t="s">
         <v>537</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>538</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="H156" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
@@ -6538,22 +6550,22 @@
         <v>1</v>
       </c>
       <c r="C157" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="D157" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="D157" s="1" t="s">
+      <c r="E157" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="E157" s="1" t="s">
+      <c r="F157" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="F157" s="1" t="s">
+      <c r="G157" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="G157" s="1" t="s">
+      <c r="H157" s="1" t="s">
         <v>544</v>
-      </c>
-      <c r="H157" s="1" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -6564,22 +6576,22 @@
         <v>1</v>
       </c>
       <c r="C158" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="D158" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="D158" s="1" t="s">
+      <c r="E158" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="E158" s="1" t="s">
+      <c r="F158" s="1" t="s">
         <v>548</v>
       </c>
-      <c r="F158" s="1" t="s">
+      <c r="G158" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="G158" s="1" t="s">
+      <c r="H158" s="1" t="s">
         <v>550</v>
-      </c>
-      <c r="H158" s="1" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -6590,22 +6602,22 @@
         <v>1</v>
       </c>
       <c r="C159" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="D159" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="D159" s="1" t="s">
+      <c r="E159" s="1" t="s">
         <v>553</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>554</v>
       </c>
       <c r="F159" s="1" t="s">
         <v>354</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H159" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -6616,22 +6628,22 @@
         <v>7</v>
       </c>
       <c r="C160" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="D160" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="D160" s="1" t="s">
+      <c r="E160" s="1" t="s">
         <v>557</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>558</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="H160" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
   </sheetData>
@@ -6652,28 +6664,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B1" t="s">
         <v>701</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>702</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>703</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>704</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>705</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>706</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>707</v>
-      </c>
-      <c r="H1" t="s">
-        <v>708</v>
       </c>
       <c r="I1" t="s">
         <v>229</v>

</xml_diff>

<commit_message>
fix part number for JTAG connector
</commit_message>
<xml_diff>
--- a/radiant_bom.xlsx
+++ b/radiant_bom.xlsx
@@ -813,12 +813,6 @@
     <t>JTAG_2MM</t>
   </si>
   <si>
-    <t>87831-1419</t>
-  </si>
-  <si>
-    <t>Conn Shrouded Header HDR 14 POS 2mm Solder ST Thru-Hole Milli-Grid™ Tube</t>
-  </si>
-  <si>
     <t>LAB1-24</t>
   </si>
   <si>
@@ -2164,6 +2158,12 @@
   </si>
   <si>
     <t>TCD-10-1WX+</t>
+  </si>
+  <si>
+    <t>87832-1422</t>
+  </si>
+  <si>
+    <t>Conn Shrouded Header (4 Sides) HDR 14 POS 2mm Solder ST Top Entry SMD Milli-Grid™ Tube</t>
   </si>
 </sst>
 </file>
@@ -2503,8 +2503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="F147" sqref="F147"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="H79" sqref="H79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3111,10 +3111,10 @@
         <v>117</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -3189,10 +3189,10 @@
         <v>93</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -3215,10 +3215,10 @@
         <v>93</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -3241,10 +3241,10 @@
         <v>227</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -3267,10 +3267,10 @@
         <v>227</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -3290,13 +3290,13 @@
         <v>92</v>
       </c>
       <c r="F30" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>569</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>570</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -3307,7 +3307,7 @@
         <v>10</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>137</v>
@@ -3319,10 +3319,10 @@
         <v>93</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3345,10 +3345,10 @@
         <v>93</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3371,10 +3371,10 @@
         <v>93</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3397,10 +3397,10 @@
         <v>93</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3423,10 +3423,10 @@
         <v>87</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3449,10 +3449,10 @@
         <v>227</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3463,7 +3463,7 @@
         <v>7</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>148</v>
@@ -3475,10 +3475,10 @@
         <v>93</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3501,10 +3501,10 @@
         <v>227</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3527,10 +3527,10 @@
         <v>93</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3553,10 +3553,10 @@
         <v>227</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -3579,10 +3579,10 @@
         <v>93</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3605,10 +3605,10 @@
         <v>120</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -3622,7 +3622,7 @@
         <v>165</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>116</v>
@@ -3631,10 +3631,10 @@
         <v>87</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -3657,10 +3657,10 @@
         <v>111</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3683,10 +3683,10 @@
         <v>87</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3709,10 +3709,10 @@
         <v>227</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3735,10 +3735,10 @@
         <v>227</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3761,10 +3761,10 @@
         <v>120</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -3787,10 +3787,10 @@
         <v>111</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -3813,10 +3813,10 @@
         <v>93</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -3839,10 +3839,10 @@
         <v>227</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -3865,10 +3865,10 @@
         <v>93</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -4156,7 +4156,7 @@
         <v>2</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>230</v>
@@ -4393,10 +4393,10 @@
         <v>13</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>262</v>
+        <v>711</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>263</v>
+        <v>712</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -4407,22 +4407,22 @@
         <v>24</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -4433,22 +4433,22 @@
         <v>2</v>
       </c>
       <c r="C75" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E75" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="F75" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="G75" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="F75" s="1" t="s">
+      <c r="H75" s="1" t="s">
         <v>269</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -4459,22 +4459,22 @@
         <v>1</v>
       </c>
       <c r="C76" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E76" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="F76" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="G76" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="F76" s="1" t="s">
+      <c r="H76" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="H76" s="1" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -4485,22 +4485,22 @@
         <v>1</v>
       </c>
       <c r="C77" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E77" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="F77" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="G77" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="F77" s="1" t="s">
+      <c r="H77" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="H77" s="1" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -4511,22 +4511,22 @@
         <v>6</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>286</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>69</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -4537,22 +4537,22 @@
         <v>2</v>
       </c>
       <c r="C79" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E79" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>291</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>69</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -4563,22 +4563,22 @@
         <v>24</v>
       </c>
       <c r="C80" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E80" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>69</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -4589,19 +4589,19 @@
         <v>24</v>
       </c>
       <c r="C81" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E81" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>301</v>
       </c>
       <c r="G81" s="1">
         <v>733660061</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -4612,22 +4612,22 @@
         <v>1</v>
       </c>
       <c r="C82" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>305</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>69</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -4638,22 +4638,22 @@
         <v>1</v>
       </c>
       <c r="C83" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>310</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>69</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -4664,22 +4664,22 @@
         <v>24</v>
       </c>
       <c r="C84" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E84" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="F84" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="G84" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="F84" s="1" t="s">
+      <c r="H84" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -4690,22 +4690,22 @@
         <v>24</v>
       </c>
       <c r="C85" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>319</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>69</v>
       </c>
       <c r="G85" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="H85" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -4716,13 +4716,13 @@
         <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>13</v>
@@ -4731,7 +4731,7 @@
         <v>1050270001</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -4742,19 +4742,19 @@
         <v>1</v>
       </c>
       <c r="C87" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E87" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="F87" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="G87" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -4765,22 +4765,22 @@
         <v>74</v>
       </c>
       <c r="C88" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="E88" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>333</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>227</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -4791,22 +4791,22 @@
         <v>6</v>
       </c>
       <c r="C89" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E89" s="1" t="s">
         <v>336</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>338</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>81</v>
       </c>
       <c r="G89" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="H89" s="1" t="s">
         <v>337</v>
-      </c>
-      <c r="H89" s="1" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -4817,22 +4817,22 @@
         <v>2</v>
       </c>
       <c r="C90" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="E90" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="F90" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="E90" s="1" t="s">
+      <c r="G90" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="H90" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="H90" s="1" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -4843,22 +4843,22 @@
         <v>24</v>
       </c>
       <c r="C91" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="H91" s="1" t="s">
         <v>345</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="H91" s="1" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -4869,22 +4869,22 @@
         <v>4</v>
       </c>
       <c r="C92" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="H92" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="H92" s="1" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -4895,22 +4895,22 @@
         <v>1</v>
       </c>
       <c r="C93" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="E93" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="F93" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="G93" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="H93" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="H93" s="1" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -4921,13 +4921,13 @@
         <v>18</v>
       </c>
       <c r="C94" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="E94" s="1" t="s">
         <v>356</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>358</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>200</v>
@@ -4947,22 +4947,22 @@
         <v>2</v>
       </c>
       <c r="C95" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="E95" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>361</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>227</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -4973,22 +4973,22 @@
         <v>1</v>
       </c>
       <c r="C96" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E96" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="F96" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="G96" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="H96" s="1" t="s">
         <v>366</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="H96" s="1" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -4999,19 +4999,19 @@
         <v>1</v>
       </c>
       <c r="C97" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="E97" s="1" t="s">
         <v>369</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>371</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>69</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -5022,22 +5022,22 @@
         <v>24</v>
       </c>
       <c r="C98" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="F98" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="G98" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="E98" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="F98" s="1" t="s">
+      <c r="H98" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="H98" s="1" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -5048,22 +5048,22 @@
         <v>49</v>
       </c>
       <c r="C99" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E99" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="D99" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>380</v>
-      </c>
       <c r="F99" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="H99" s="1" t="s">
         <v>624</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="H99" s="1" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -5074,22 +5074,22 @@
         <v>6</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>182</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -5100,22 +5100,22 @@
         <v>73</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F101" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="H101" s="1" t="s">
         <v>627</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>628</v>
-      </c>
-      <c r="H101" s="1" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -5126,10 +5126,10 @@
         <v>6</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="E102" s="1">
         <v>603</v>
@@ -5138,10 +5138,10 @@
         <v>19</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -5152,22 +5152,22 @@
         <v>51</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -5178,22 +5178,22 @@
         <v>247</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -5204,22 +5204,22 @@
         <v>24</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -5230,22 +5230,22 @@
         <v>3</v>
       </c>
       <c r="C106" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="H106" s="1" t="s">
         <v>639</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>624</v>
-      </c>
-      <c r="G106" s="1" t="s">
-        <v>640</v>
-      </c>
-      <c r="H106" s="1" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -5256,22 +5256,22 @@
         <v>13</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E107" s="1">
         <v>603</v>
       </c>
       <c r="F107" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="H107" s="1" t="s">
         <v>642</v>
-      </c>
-      <c r="G107" s="1" t="s">
-        <v>643</v>
-      </c>
-      <c r="H107" s="1" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -5282,22 +5282,22 @@
         <v>48</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -5308,22 +5308,22 @@
         <v>48</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -5334,22 +5334,22 @@
         <v>25</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -5360,22 +5360,22 @@
         <v>1</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -5386,22 +5386,22 @@
         <v>7</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -5412,22 +5412,22 @@
         <v>2</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -5438,22 +5438,22 @@
         <v>1</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -5464,22 +5464,22 @@
         <v>24</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E115" s="1">
         <v>603</v>
       </c>
       <c r="F115" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="H115" s="1" t="s">
         <v>659</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>660</v>
-      </c>
-      <c r="H115" s="1" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -5490,22 +5490,22 @@
         <v>26</v>
       </c>
       <c r="C116" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="H116" s="1" t="s">
         <v>662</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>624</v>
-      </c>
-      <c r="G116" s="1" t="s">
-        <v>663</v>
-      </c>
-      <c r="H116" s="1" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -5516,22 +5516,22 @@
         <v>1</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F117" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="H117" s="1" t="s">
         <v>665</v>
-      </c>
-      <c r="G117" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="H117" s="1" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -5542,22 +5542,22 @@
         <v>8</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -5568,22 +5568,22 @@
         <v>2</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -5594,22 +5594,22 @@
         <v>1</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -5620,22 +5620,22 @@
         <v>24</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -5646,22 +5646,22 @@
         <v>102</v>
       </c>
       <c r="C122" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="H122" s="1" t="s">
         <v>674</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="F122" s="1" t="s">
-        <v>624</v>
-      </c>
-      <c r="G122" s="1" t="s">
-        <v>675</v>
-      </c>
-      <c r="H122" s="1" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -5672,22 +5672,22 @@
         <v>1</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -5698,22 +5698,22 @@
         <v>1</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E124" s="1">
         <v>603</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -5724,22 +5724,22 @@
         <v>55</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -5750,22 +5750,22 @@
         <v>25</v>
       </c>
       <c r="C126" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="G126" s="1" t="s">
         <v>686</v>
       </c>
-      <c r="D126" s="1" t="s">
+      <c r="H126" s="1" t="s">
         <v>687</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="F126" s="1" t="s">
-        <v>627</v>
-      </c>
-      <c r="G126" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="H126" s="1" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -5776,22 +5776,22 @@
         <v>9</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -5802,22 +5802,22 @@
         <v>1</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -5828,22 +5828,22 @@
         <v>2</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -5854,22 +5854,22 @@
         <v>1</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="H130" s="1" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -5880,22 +5880,22 @@
         <v>2</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="H131" s="1" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -5906,22 +5906,22 @@
         <v>1</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -5932,13 +5932,13 @@
         <v>89</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>200</v>
@@ -5955,22 +5955,22 @@
         <v>48</v>
       </c>
       <c r="C134" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="E134" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="D134" s="1" t="s">
+      <c r="F134" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="E134" s="1" t="s">
+      <c r="G134" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="F134" s="1" t="s">
+      <c r="H134" s="1" t="s">
         <v>440</v>
-      </c>
-      <c r="G134" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="H134" s="1" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -5981,22 +5981,22 @@
         <v>66</v>
       </c>
       <c r="C135" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="E135" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="D135" s="1" t="s">
+      <c r="F135" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="E135" s="1" t="s">
+      <c r="G135" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="F135" s="1" t="s">
+      <c r="H135" s="1" t="s">
         <v>446</v>
-      </c>
-      <c r="G135" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="H135" s="1" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -6007,22 +6007,22 @@
         <v>1</v>
       </c>
       <c r="C136" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="E136" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="D136" s="1" t="s">
+      <c r="F136" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="E136" s="1" t="s">
+      <c r="G136" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="F136" s="1" t="s">
+      <c r="H136" s="1" t="s">
         <v>452</v>
-      </c>
-      <c r="G136" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="H136" s="1" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -6033,22 +6033,22 @@
         <v>6</v>
       </c>
       <c r="C137" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="E137" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="D137" s="1" t="s">
+      <c r="F137" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="E137" s="1" t="s">
+      <c r="G137" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="H137" s="1" t="s">
         <v>457</v>
-      </c>
-      <c r="F137" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="G137" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="H137" s="1" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -6059,22 +6059,22 @@
         <v>1</v>
       </c>
       <c r="C138" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="E138" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="D138" s="1" t="s">
+      <c r="F138" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="E138" s="1" t="s">
+      <c r="G138" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="F138" s="1" t="s">
+      <c r="H138" s="1" t="s">
         <v>463</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="H138" s="1" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -6085,19 +6085,19 @@
         <v>2</v>
       </c>
       <c r="C139" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="F139" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="D139" s="1" t="s">
+      <c r="G139" s="1" t="s">
         <v>467</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="F139" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="G139" s="1" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -6108,22 +6108,22 @@
         <v>30</v>
       </c>
       <c r="C140" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="E140" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="D140" s="1" t="s">
+      <c r="F140" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="E140" s="1" t="s">
+      <c r="G140" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="H140" s="1" t="s">
         <v>472</v>
-      </c>
-      <c r="F140" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="G140" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="H140" s="1" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -6134,22 +6134,22 @@
         <v>24</v>
       </c>
       <c r="C141" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="E141" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="D141" s="1" t="s">
+      <c r="F141" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="G141" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="E141" s="1" t="s">
+      <c r="H141" s="1" t="s">
         <v>477</v>
-      </c>
-      <c r="F141" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="G141" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="H141" s="1" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
@@ -6160,22 +6160,22 @@
         <v>23</v>
       </c>
       <c r="C142" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="E142" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="D142" s="1" t="s">
+      <c r="F142" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="E142" s="1" t="s">
+      <c r="G142" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="F142" s="1" t="s">
+      <c r="H142" s="1" t="s">
         <v>483</v>
-      </c>
-      <c r="G142" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="H142" s="1" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -6186,22 +6186,22 @@
         <v>7</v>
       </c>
       <c r="C143" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="G143" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="D143" s="1" t="s">
+      <c r="H143" s="1" t="s">
         <v>487</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="F143" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="G143" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="H143" s="1" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -6212,22 +6212,22 @@
         <v>1</v>
       </c>
       <c r="C144" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="E144" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="D144" s="1" t="s">
+      <c r="F144" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="E144" s="1" t="s">
+      <c r="G144" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="F144" s="1" t="s">
+      <c r="H144" s="1" t="s">
         <v>493</v>
-      </c>
-      <c r="G144" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="H144" s="1" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -6238,13 +6238,13 @@
         <v>2</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="F145" s="1" t="s">
         <v>200</v>
@@ -6253,7 +6253,7 @@
         <v>200</v>
       </c>
       <c r="H145" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
@@ -6264,22 +6264,22 @@
         <v>24</v>
       </c>
       <c r="C146" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="E146" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="D146" s="1" t="s">
+      <c r="F146" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="G146" t="s">
+        <v>710</v>
+      </c>
+      <c r="H146" s="1" t="s">
         <v>500</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="F146" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="G146" t="s">
-        <v>712</v>
-      </c>
-      <c r="H146" s="1" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -6290,22 +6290,22 @@
         <v>1</v>
       </c>
       <c r="C147" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="H147" s="1" t="s">
         <v>503</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="F147" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="G147" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="H147" s="1" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
@@ -6316,22 +6316,22 @@
         <v>24</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>111</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="H148" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -6342,13 +6342,13 @@
         <v>125</v>
       </c>
       <c r="C149" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="E149" s="1" t="s">
         <v>510</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>512</v>
       </c>
       <c r="F149" s="1" t="s">
         <v>200</v>
@@ -6357,7 +6357,7 @@
         <v>200</v>
       </c>
       <c r="H149" s="1" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -6368,22 +6368,22 @@
         <v>1</v>
       </c>
       <c r="C150" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="E150" s="1" t="s">
         <v>513</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>515</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="H150" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -6394,22 +6394,22 @@
         <v>1</v>
       </c>
       <c r="C151" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="E151" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>519</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G151" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="H151" s="1" t="s">
         <v>518</v>
-      </c>
-      <c r="H151" s="1" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -6420,22 +6420,22 @@
         <v>1</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G152" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="H152" s="1" t="s">
         <v>518</v>
-      </c>
-      <c r="H152" s="1" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -6446,22 +6446,22 @@
         <v>1</v>
       </c>
       <c r="C153" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E153" s="1" t="s">
         <v>523</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="E153" s="1" t="s">
-        <v>525</v>
       </c>
       <c r="F153" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G153" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="H153" s="1" t="s">
         <v>524</v>
-      </c>
-      <c r="H153" s="1" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -6472,22 +6472,22 @@
         <v>1</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="H154" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -6498,22 +6498,22 @@
         <v>1</v>
       </c>
       <c r="C155" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="E155" s="1" t="s">
         <v>531</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>533</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G155" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="H155" s="1" t="s">
         <v>532</v>
-      </c>
-      <c r="H155" s="1" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -6524,22 +6524,22 @@
         <v>1</v>
       </c>
       <c r="C156" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="E156" s="1" t="s">
         <v>535</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>537</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G156" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="H156" s="1" t="s">
         <v>536</v>
-      </c>
-      <c r="H156" s="1" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
@@ -6550,22 +6550,22 @@
         <v>1</v>
       </c>
       <c r="C157" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="E157" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="D157" s="1" t="s">
+      <c r="F157" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="E157" s="1" t="s">
+      <c r="G157" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="F157" s="1" t="s">
+      <c r="H157" s="1" t="s">
         <v>542</v>
-      </c>
-      <c r="G157" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="H157" s="1" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -6576,22 +6576,22 @@
         <v>1</v>
       </c>
       <c r="C158" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="E158" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="D158" s="1" t="s">
+      <c r="F158" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="E158" s="1" t="s">
+      <c r="G158" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="F158" s="1" t="s">
+      <c r="H158" s="1" t="s">
         <v>548</v>
-      </c>
-      <c r="G158" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="H158" s="1" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -6602,22 +6602,22 @@
         <v>1</v>
       </c>
       <c r="C159" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="E159" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="D159" s="1" t="s">
+      <c r="F159" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G159" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="H159" s="1" t="s">
         <v>552</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="F159" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="G159" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="H159" s="1" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -6628,22 +6628,22 @@
         <v>7</v>
       </c>
       <c r="C160" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="E160" s="1" t="s">
         <v>555</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>557</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="H160" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
   </sheetData>
@@ -6664,28 +6664,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>698</v>
+      </c>
+      <c r="B1" t="s">
+        <v>699</v>
+      </c>
+      <c r="C1" t="s">
         <v>700</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>701</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>702</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>703</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>704</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>705</v>
-      </c>
-      <c r="G1" t="s">
-        <v>706</v>
-      </c>
-      <c r="H1" t="s">
-        <v>707</v>
       </c>
       <c r="I1" t="s">
         <v>229</v>

</xml_diff>

<commit_message>
really connect all grounds
</commit_message>
<xml_diff>
--- a/radiant_bom.xlsx
+++ b/radiant_bom.xlsx
@@ -2207,7 +2207,7 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -2216,11 +2216,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2503,30 +2509,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="H79" sqref="H79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="5" customWidth="1"/>
     <col min="4" max="4" width="38.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="30.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="8" max="8" width="101.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -2535,13 +2541,13 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2552,7 +2558,7 @@
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1">
@@ -2561,13 +2567,13 @@
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="1">
         <v>744071039</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2578,7 +2584,7 @@
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="1">
@@ -2587,13 +2593,13 @@
       <c r="E3" s="1">
         <v>21471100001</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2604,7 +2610,7 @@
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -2613,13 +2619,13 @@
       <c r="E4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2630,7 +2636,7 @@
       <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -2639,13 +2645,13 @@
       <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2656,7 +2662,7 @@
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -2665,13 +2671,13 @@
       <c r="E6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2682,7 +2688,7 @@
       <c r="B7" s="1">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -2691,13 +2697,13 @@
       <c r="E7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" t="s">
         <v>31</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2708,7 +2714,7 @@
       <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -2717,13 +2723,13 @@
       <c r="E8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="1">
         <v>39281043</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2734,7 +2740,7 @@
       <c r="B9" s="1">
         <v>1</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -2743,24 +2749,24 @@
       <c r="E9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" t="s">
         <v>39</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>30</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -2769,13 +2775,13 @@
       <c r="E10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" t="s">
         <v>45</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2786,7 +2792,7 @@
       <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -2795,13 +2801,13 @@
       <c r="E11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" t="s">
         <v>51</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2812,7 +2818,7 @@
       <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="5" t="s">
         <v>54</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -2821,24 +2827,24 @@
       <c r="E12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>6</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="5" t="s">
         <v>60</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -2847,13 +2853,13 @@
       <c r="E13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" t="s">
         <v>63</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2864,7 +2870,7 @@
       <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="5" t="s">
         <v>66</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -2873,24 +2879,24 @@
       <c r="E14" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" t="s">
         <v>69</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1">
         <v>24</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="5" t="s">
         <v>72</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -2899,24 +2905,24 @@
       <c r="E15" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" t="s">
         <v>75</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>24</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="5" t="s">
         <v>78</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -2925,24 +2931,24 @@
       <c r="E16" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" t="s">
         <v>81</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>44</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="5" t="s">
         <v>84</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -2951,24 +2957,24 @@
       <c r="E17" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" t="s">
         <v>87</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>441</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="5" t="s">
         <v>90</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -2977,24 +2983,24 @@
       <c r="E18" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" t="s">
         <v>93</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="210" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1">
         <v>105</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="5" t="s">
         <v>96</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -3003,24 +3009,24 @@
       <c r="E19" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" t="s">
         <v>87</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="345" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>73</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -3029,24 +3035,24 @@
       <c r="E20" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" t="s">
         <v>87</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>219</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="5" t="s">
         <v>104</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -3055,24 +3061,24 @@
       <c r="E21" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" t="s">
         <v>87</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1">
         <v>24</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="5" t="s">
         <v>109</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -3081,13 +3087,13 @@
       <c r="E22" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" t="s">
         <v>111</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3098,7 +3104,7 @@
       <c r="B23" s="1">
         <v>1</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="5" t="s">
         <v>114</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -3107,24 +3113,24 @@
       <c r="E23" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" t="s">
         <v>117</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H23" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>175</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="5" t="s">
         <v>118</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -3133,24 +3139,24 @@
       <c r="E24" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" t="s">
         <v>120</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>62</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="5" t="s">
         <v>123</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -3159,13 +3165,13 @@
       <c r="E25" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" t="s">
         <v>93</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" t="s">
         <v>126</v>
       </c>
     </row>
@@ -3176,7 +3182,7 @@
       <c r="B26" s="1">
         <v>1</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="5" t="s">
         <v>127</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -3185,13 +3191,13 @@
       <c r="E26" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" t="s">
         <v>93</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H26" t="s">
         <v>560</v>
       </c>
     </row>
@@ -3202,7 +3208,7 @@
       <c r="B27" s="1">
         <v>1</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="5" t="s">
         <v>129</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -3211,24 +3217,24 @@
       <c r="E27" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" t="s">
         <v>93</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="H27" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1">
         <v>25</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="5" t="s">
         <v>131</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -3237,24 +3243,24 @@
       <c r="E28" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" t="s">
         <v>227</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="405" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1">
         <v>62</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="5" t="s">
         <v>133</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -3263,24 +3269,24 @@
       <c r="E29" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" t="s">
         <v>227</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="360" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="1">
         <v>48</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="5" t="s">
         <v>135</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -3289,24 +3295,24 @@
       <c r="E30" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" t="s">
         <v>567</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H30" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1">
         <v>10</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="5" t="s">
         <v>576</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -3315,13 +3321,13 @@
       <c r="E31" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" t="s">
         <v>93</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="H31" t="s">
         <v>571</v>
       </c>
     </row>
@@ -3332,7 +3338,7 @@
       <c r="B32" s="1">
         <v>1</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="5" t="s">
         <v>138</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -3341,13 +3347,13 @@
       <c r="E32" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" t="s">
         <v>93</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="H32" t="s">
         <v>573</v>
       </c>
     </row>
@@ -3358,7 +3364,7 @@
       <c r="B33" s="1">
         <v>1</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="5" t="s">
         <v>140</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -3367,24 +3373,24 @@
       <c r="E33" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" t="s">
         <v>93</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H33" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="1">
         <v>122</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="5" t="s">
         <v>142</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -3393,24 +3399,24 @@
       <c r="E34" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" t="s">
         <v>93</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="H34" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="1">
         <v>5</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="5" t="s">
         <v>144</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -3419,24 +3425,24 @@
       <c r="E35" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" t="s">
         <v>87</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="H35" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="270" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1">
         <v>48</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="5" t="s">
         <v>146</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -3445,24 +3451,24 @@
       <c r="E36" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F36" t="s">
         <v>227</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>581</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="H36" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="1">
         <v>7</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="5" t="s">
         <v>583</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -3471,13 +3477,13 @@
       <c r="E37" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F37" t="s">
         <v>93</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>584</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="H37" t="s">
         <v>585</v>
       </c>
     </row>
@@ -3488,7 +3494,7 @@
       <c r="B38" s="1">
         <v>1</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="5" t="s">
         <v>149</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -3497,24 +3503,24 @@
       <c r="E38" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F38" t="s">
         <v>227</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="H38" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="360" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="1">
         <v>48</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="5" t="s">
         <v>151</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -3523,13 +3529,13 @@
       <c r="E39" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" t="s">
         <v>93</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>588</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H39" t="s">
         <v>589</v>
       </c>
     </row>
@@ -3540,7 +3546,7 @@
       <c r="B40" s="1">
         <v>1</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="5" t="s">
         <v>153</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -3549,24 +3555,24 @@
       <c r="E40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" t="s">
         <v>227</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>590</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="H40" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="360" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="1">
         <v>48</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="5" t="s">
         <v>155</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -3575,24 +3581,24 @@
       <c r="E41" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F41" t="s">
         <v>93</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>592</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H41" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="1">
         <v>37</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="5" t="s">
         <v>157</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -3601,24 +3607,24 @@
       <c r="E42" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F42" t="s">
         <v>120</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H42" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="1">
         <v>4</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="5" t="s">
         <v>165</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -3627,24 +3633,24 @@
       <c r="E43" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F43" t="s">
         <v>87</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>595</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H43" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="1">
         <v>7</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="5" t="s">
         <v>159</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -3653,13 +3659,13 @@
       <c r="E44" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F44" t="s">
         <v>111</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="H44" t="s">
         <v>619</v>
       </c>
     </row>
@@ -3670,7 +3676,7 @@
       <c r="B45" s="1">
         <v>1</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="5" t="s">
         <v>161</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -3679,13 +3685,13 @@
       <c r="E45" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F45" t="s">
         <v>87</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>620</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="H45" t="s">
         <v>621</v>
       </c>
     </row>
@@ -3696,7 +3702,7 @@
       <c r="B46" s="1">
         <v>1</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="5" t="s">
         <v>163</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -3705,24 +3711,24 @@
       <c r="E46" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F46" t="s">
         <v>227</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="H46" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" s="1">
         <v>4</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="5" t="s">
         <v>167</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -3731,13 +3737,13 @@
       <c r="E47" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F47" t="s">
         <v>227</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="H47" t="s">
         <v>600</v>
       </c>
     </row>
@@ -3748,7 +3754,7 @@
       <c r="B48" s="1">
         <v>2</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="5" t="s">
         <v>169</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -3757,13 +3763,13 @@
       <c r="E48" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="F48" t="s">
         <v>120</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="H48" t="s">
         <v>602</v>
       </c>
     </row>
@@ -3774,7 +3780,7 @@
       <c r="B49" s="1">
         <v>1</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="5" t="s">
         <v>171</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -3783,24 +3789,24 @@
       <c r="E49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="F49" t="s">
         <v>111</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>603</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="H49" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" s="1">
         <v>96</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="5" t="s">
         <v>173</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -3809,24 +3815,24 @@
       <c r="E50" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F50" t="s">
         <v>93</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="H50" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="360" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
       <c r="B51" s="1">
         <v>48</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="5" t="s">
         <v>175</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -3835,13 +3841,13 @@
       <c r="E51" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F51" t="s">
         <v>227</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="H51" t="s">
         <v>608</v>
       </c>
     </row>
@@ -3852,7 +3858,7 @@
       <c r="B52" s="1">
         <v>1</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="5" t="s">
         <v>177</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -3861,13 +3867,13 @@
       <c r="E52" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="F52" t="s">
         <v>93</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="H52" t="s">
         <v>610</v>
       </c>
     </row>
@@ -3878,7 +3884,7 @@
       <c r="B53" s="1">
         <v>1</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="5" t="s">
         <v>179</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -3887,13 +3893,13 @@
       <c r="E53" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="F53" t="s">
         <v>182</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="H53" s="1" t="s">
+      <c r="H53" t="s">
         <v>184</v>
       </c>
     </row>
@@ -3904,7 +3910,7 @@
       <c r="B54" s="1">
         <v>2</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="5" t="s">
         <v>185</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -3913,13 +3919,13 @@
       <c r="E54" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="F54" t="s">
         <v>188</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="H54" t="s">
         <v>189</v>
       </c>
     </row>
@@ -3930,7 +3936,7 @@
       <c r="B55" s="1">
         <v>2</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="5" t="s">
         <v>190</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -3939,13 +3945,13 @@
       <c r="E55" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="F55" t="s">
         <v>111</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="H55" t="s">
         <v>193</v>
       </c>
     </row>
@@ -3956,7 +3962,7 @@
       <c r="B56" s="1">
         <v>2</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="5" t="s">
         <v>194</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -3965,13 +3971,13 @@
       <c r="E56" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="F56" t="s">
         <v>200</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="H56" t="s">
         <v>200</v>
       </c>
     </row>
@@ -3982,7 +3988,7 @@
       <c r="B57" s="1">
         <v>6</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="5" t="s">
         <v>197</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -3991,13 +3997,13 @@
       <c r="E57" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="F57" t="s">
         <v>200</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="H57" t="s">
         <v>200</v>
       </c>
     </row>
@@ -4008,7 +4014,7 @@
       <c r="B58" s="1">
         <v>1</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="5" t="s">
         <v>201</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -4017,24 +4023,24 @@
       <c r="E58" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="F58" t="s">
         <v>204</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="H58" s="1" t="s">
+      <c r="H58" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
       <c r="B59" s="1">
         <v>49</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="5" t="s">
         <v>206</v>
       </c>
       <c r="D59" s="1" t="s">
@@ -4043,7 +4049,7 @@
       <c r="E59" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="F59" t="s">
         <v>209</v>
       </c>
       <c r="G59" s="1" t="s">
@@ -4057,7 +4063,7 @@
       <c r="B60" s="1">
         <v>1</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="5" t="s">
         <v>211</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -4066,7 +4072,7 @@
       <c r="E60" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="F60" t="s">
         <v>214</v>
       </c>
       <c r="G60" s="1" t="s">
@@ -4080,7 +4086,7 @@
       <c r="B61" s="1">
         <v>1</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="5" t="s">
         <v>216</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -4089,24 +4095,24 @@
       <c r="E61" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="F61" t="s">
         <v>69</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="H61" s="1" t="s">
+      <c r="H61" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
       <c r="B62" s="1">
         <v>4</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="5" t="s">
         <v>221</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -4115,13 +4121,13 @@
       <c r="E62" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="F62" s="1" t="s">
+      <c r="F62" t="s">
         <v>214</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="H62" s="1" t="s">
+      <c r="H62" t="s">
         <v>224</v>
       </c>
     </row>
@@ -4132,7 +4138,7 @@
       <c r="B63" s="1">
         <v>6</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="5" t="s">
         <v>225</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -4141,7 +4147,7 @@
       <c r="E63" s="1">
         <v>402</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="F63" t="s">
         <v>227</v>
       </c>
       <c r="G63" s="1" t="s">
@@ -4155,7 +4161,7 @@
       <c r="B64" s="1">
         <v>2</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="5" t="s">
         <v>706</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -4164,24 +4170,24 @@
       <c r="E64" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="F64" t="s">
         <v>200</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H64" s="1" t="s">
+      <c r="H64" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
       <c r="B65" s="1">
         <v>102</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="5" t="s">
         <v>232</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -4190,21 +4196,21 @@
       <c r="E65" s="1">
         <v>603</v>
       </c>
-      <c r="F65" s="1" t="s">
+      <c r="F65" t="s">
         <v>227</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="240" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
       <c r="B66" s="1">
         <v>48</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="5" t="s">
         <v>235</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -4213,21 +4219,21 @@
       <c r="E66" s="1">
         <v>603</v>
       </c>
-      <c r="F66" s="1" t="s">
+      <c r="F66" t="s">
         <v>10</v>
       </c>
       <c r="G66" s="1">
         <v>744917215</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
       <c r="B67" s="1">
         <v>24</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="5" t="s">
         <v>237</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -4236,7 +4242,7 @@
       <c r="E67" s="1">
         <v>805</v>
       </c>
-      <c r="F67" s="1" t="s">
+      <c r="F67" t="s">
         <v>87</v>
       </c>
       <c r="G67" s="1" t="s">
@@ -4250,7 +4256,7 @@
       <c r="B68" s="1">
         <v>1</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="5" t="s">
         <v>240</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -4259,13 +4265,13 @@
       <c r="E68" s="1">
         <v>805</v>
       </c>
-      <c r="F68" s="1" t="s">
+      <c r="F68" t="s">
         <v>227</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="H68" s="1" t="s">
+      <c r="H68" t="s">
         <v>243</v>
       </c>
     </row>
@@ -4276,7 +4282,7 @@
       <c r="B69" s="1">
         <v>1</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" s="5" t="s">
         <v>244</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -4285,13 +4291,13 @@
       <c r="E69" s="1">
         <v>805</v>
       </c>
-      <c r="F69" s="1" t="s">
+      <c r="F69" t="s">
         <v>227</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="H69" s="1" t="s">
+      <c r="H69" t="s">
         <v>247</v>
       </c>
     </row>
@@ -4302,7 +4308,7 @@
       <c r="B70" s="1">
         <v>1</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="5" t="s">
         <v>248</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -4311,24 +4317,24 @@
       <c r="E70" s="1">
         <v>805</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="F70" t="s">
         <v>227</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="H70" s="1" t="s">
+      <c r="H70" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="240" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
       <c r="B71" s="1">
         <v>48</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="5" t="s">
         <v>252</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -4337,13 +4343,13 @@
       <c r="E71" s="1">
         <v>805</v>
       </c>
-      <c r="F71" s="1" t="s">
+      <c r="F71" t="s">
         <v>227</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="H71" s="1" t="s">
+      <c r="H71" t="s">
         <v>255</v>
       </c>
     </row>
@@ -4354,7 +4360,7 @@
       <c r="B72" s="1">
         <v>1</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="5" t="s">
         <v>256</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -4363,13 +4369,13 @@
       <c r="E72" s="1">
         <v>805</v>
       </c>
-      <c r="F72" s="1" t="s">
+      <c r="F72" t="s">
         <v>227</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="H72" s="1" t="s">
+      <c r="H72" t="s">
         <v>259</v>
       </c>
     </row>
@@ -4380,7 +4386,7 @@
       <c r="B73" s="1">
         <v>1</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="5" t="s">
         <v>260</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -4389,13 +4395,13 @@
       <c r="E73" s="1">
         <v>878321422</v>
       </c>
-      <c r="F73" s="1" t="s">
+      <c r="F73" t="s">
         <v>13</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>711</v>
       </c>
-      <c r="H73" s="1" t="s">
+      <c r="H73" t="s">
         <v>712</v>
       </c>
     </row>
@@ -4406,7 +4412,7 @@
       <c r="B74" s="1">
         <v>24</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="5" t="s">
         <v>262</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -4415,13 +4421,13 @@
       <c r="E74" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="F74" s="1" t="s">
+      <c r="F74" t="s">
         <v>709</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>709</v>
       </c>
-      <c r="H74" s="1" t="s">
+      <c r="H74" t="s">
         <v>709</v>
       </c>
     </row>
@@ -4432,7 +4438,7 @@
       <c r="B75" s="1">
         <v>2</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" s="5" t="s">
         <v>264</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -4441,13 +4447,13 @@
       <c r="E75" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="F75" s="1" t="s">
+      <c r="F75" t="s">
         <v>267</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="H75" s="1" t="s">
+      <c r="H75" t="s">
         <v>269</v>
       </c>
     </row>
@@ -4458,7 +4464,7 @@
       <c r="B76" s="1">
         <v>1</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="5" t="s">
         <v>270</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -4467,13 +4473,13 @@
       <c r="E76" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="F76" s="1" t="s">
+      <c r="F76" t="s">
         <v>273</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="H76" s="1" t="s">
+      <c r="H76" t="s">
         <v>275</v>
       </c>
     </row>
@@ -4484,7 +4490,7 @@
       <c r="B77" s="1">
         <v>1</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="5" t="s">
         <v>276</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -4493,24 +4499,24 @@
       <c r="E77" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="F77" s="1" t="s">
+      <c r="F77" t="s">
         <v>279</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="H77" s="1" t="s">
+      <c r="H77" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
       <c r="B78" s="1">
         <v>6</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="5" t="s">
         <v>282</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -4519,13 +4525,13 @@
       <c r="E78" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="F78" s="1" t="s">
+      <c r="F78" t="s">
         <v>69</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="H78" s="1" t="s">
+      <c r="H78" t="s">
         <v>286</v>
       </c>
     </row>
@@ -4536,7 +4542,7 @@
       <c r="B79" s="1">
         <v>2</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" s="5" t="s">
         <v>287</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -4545,13 +4551,13 @@
       <c r="E79" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="F79" s="1" t="s">
+      <c r="F79" t="s">
         <v>69</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="H79" s="1" t="s">
+      <c r="H79" t="s">
         <v>291</v>
       </c>
     </row>
@@ -4562,7 +4568,7 @@
       <c r="B80" s="1">
         <v>24</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="5" t="s">
         <v>292</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -4571,24 +4577,24 @@
       <c r="E80" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="F80" s="1" t="s">
+      <c r="F80" t="s">
         <v>69</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="H80" s="1" t="s">
+      <c r="H80" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
       <c r="B81" s="1">
         <v>24</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" s="5" t="s">
         <v>297</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -4600,7 +4606,7 @@
       <c r="G81" s="1">
         <v>733660061</v>
       </c>
-      <c r="H81" s="1" t="s">
+      <c r="H81" t="s">
         <v>300</v>
       </c>
     </row>
@@ -4611,7 +4617,7 @@
       <c r="B82" s="1">
         <v>1</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" s="5" t="s">
         <v>301</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -4620,13 +4626,13 @@
       <c r="E82" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F82" s="1" t="s">
+      <c r="F82" t="s">
         <v>69</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="H82" s="1" t="s">
+      <c r="H82" t="s">
         <v>305</v>
       </c>
     </row>
@@ -4637,7 +4643,7 @@
       <c r="B83" s="1">
         <v>1</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" s="5" t="s">
         <v>306</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -4646,24 +4652,24 @@
       <c r="E83" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="F83" s="1" t="s">
+      <c r="F83" t="s">
         <v>69</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="H83" s="1" t="s">
+      <c r="H83" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
       <c r="B84" s="1">
         <v>24</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" s="5" t="s">
         <v>311</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -4672,24 +4678,24 @@
       <c r="E84" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="F84" s="1" t="s">
+      <c r="F84" t="s">
         <v>314</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="H84" s="1" t="s">
+      <c r="H84" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>84</v>
       </c>
       <c r="B85" s="1">
         <v>24</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" s="5" t="s">
         <v>317</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -4698,13 +4704,13 @@
       <c r="E85" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="F85" s="1" t="s">
+      <c r="F85" t="s">
         <v>69</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="H85" s="1" t="s">
+      <c r="H85" t="s">
         <v>320</v>
       </c>
     </row>
@@ -4715,7 +4721,7 @@
       <c r="B86" s="1">
         <v>1</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" s="5" t="s">
         <v>321</v>
       </c>
       <c r="D86" s="1" t="s">
@@ -4724,13 +4730,13 @@
       <c r="E86" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="F86" s="1" t="s">
+      <c r="F86" t="s">
         <v>13</v>
       </c>
       <c r="G86" s="1">
         <v>1050270001</v>
       </c>
-      <c r="H86" s="1" t="s">
+      <c r="H86" t="s">
         <v>323</v>
       </c>
     </row>
@@ -4741,7 +4747,7 @@
       <c r="B87" s="1">
         <v>1</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" s="5" t="s">
         <v>324</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -4750,21 +4756,21 @@
       <c r="E87" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="F87" s="1" t="s">
+      <c r="F87" t="s">
         <v>327</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>87</v>
       </c>
       <c r="B88" s="1">
         <v>74</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" s="5" t="s">
         <v>329</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -4773,24 +4779,24 @@
       <c r="E88" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="F88" s="1" t="s">
+      <c r="F88" t="s">
         <v>227</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="H88" s="1" t="s">
+      <c r="H88" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>88</v>
       </c>
       <c r="B89" s="1">
         <v>6</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" s="5" t="s">
         <v>334</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -4799,13 +4805,13 @@
       <c r="E89" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="F89" s="1" t="s">
+      <c r="F89" t="s">
         <v>81</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="H89" s="1" t="s">
+      <c r="H89" t="s">
         <v>337</v>
       </c>
     </row>
@@ -4816,7 +4822,7 @@
       <c r="B90" s="1">
         <v>2</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" s="5" t="s">
         <v>338</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -4825,24 +4831,24 @@
       <c r="E90" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="F90" s="1" t="s">
+      <c r="F90" t="s">
         <v>341</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="H90" s="1" t="s">
+      <c r="H90" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>90</v>
       </c>
       <c r="B91" s="1">
         <v>24</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" s="5" t="s">
         <v>343</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -4851,13 +4857,13 @@
       <c r="E91" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="F91" s="1" t="s">
+      <c r="F91" t="s">
         <v>341</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="H91" s="1" t="s">
+      <c r="H91" t="s">
         <v>345</v>
       </c>
     </row>
@@ -4868,7 +4874,7 @@
       <c r="B92" s="1">
         <v>4</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" s="5" t="s">
         <v>346</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -4877,13 +4883,13 @@
       <c r="E92" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="F92" s="1" t="s">
+      <c r="F92" t="s">
         <v>341</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="H92" s="1" t="s">
+      <c r="H92" t="s">
         <v>348</v>
       </c>
     </row>
@@ -4894,7 +4900,7 @@
       <c r="B93" s="1">
         <v>1</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" s="5" t="s">
         <v>349</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -4903,24 +4909,24 @@
       <c r="E93" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="F93" s="1" t="s">
+      <c r="F93" t="s">
         <v>352</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="H93" s="1" t="s">
+      <c r="H93" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>93</v>
       </c>
       <c r="B94" s="1">
         <v>18</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" s="5" t="s">
         <v>354</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -4929,13 +4935,13 @@
       <c r="E94" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="F94" s="1" t="s">
+      <c r="F94" t="s">
         <v>200</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H94" s="1" t="s">
+      <c r="H94" t="s">
         <v>200</v>
       </c>
     </row>
@@ -4946,7 +4952,7 @@
       <c r="B95" s="1">
         <v>2</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" s="5" t="s">
         <v>357</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -4955,13 +4961,13 @@
       <c r="E95" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="F95" s="1" t="s">
+      <c r="F95" t="s">
         <v>227</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="H95" s="1" t="s">
+      <c r="H95" t="s">
         <v>361</v>
       </c>
     </row>
@@ -4972,7 +4978,7 @@
       <c r="B96" s="1">
         <v>1</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" s="5" t="s">
         <v>362</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -4981,13 +4987,13 @@
       <c r="E96" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="F96" s="1" t="s">
+      <c r="F96" t="s">
         <v>365</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="H96" s="1" t="s">
+      <c r="H96" t="s">
         <v>366</v>
       </c>
     </row>
@@ -4998,7 +5004,7 @@
       <c r="B97" s="1">
         <v>1</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C97" s="5" t="s">
         <v>367</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -5007,21 +5013,21 @@
       <c r="E97" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="F97" s="1" t="s">
+      <c r="F97" t="s">
         <v>69</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
       <c r="B98" s="1">
         <v>24</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C98" s="5" t="s">
         <v>371</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -5030,24 +5036,24 @@
       <c r="E98" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="F98" s="1" t="s">
+      <c r="F98" t="s">
         <v>373</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="H98" s="1" t="s">
+      <c r="H98" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="360" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>98</v>
       </c>
       <c r="B99" s="1">
         <v>49</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" s="5" t="s">
         <v>376</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -5056,24 +5062,24 @@
       <c r="E99" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F99" s="1" t="s">
+      <c r="F99" t="s">
         <v>622</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>623</v>
       </c>
-      <c r="H99" s="1" t="s">
+      <c r="H99" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
       <c r="B100" s="1">
         <v>6</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C100" s="5" t="s">
         <v>379</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -5082,24 +5088,24 @@
       <c r="E100" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F100" s="1" t="s">
+      <c r="F100" t="s">
         <v>182</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="H100" s="1" t="s">
+      <c r="H100" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="345" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>100</v>
       </c>
       <c r="B101" s="1">
         <v>73</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" s="5" t="s">
         <v>383</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -5108,24 +5114,24 @@
       <c r="E101" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F101" s="1" t="s">
+      <c r="F101" t="s">
         <v>625</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="H101" s="1" t="s">
+      <c r="H101" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
       <c r="B102" s="1">
         <v>6</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C102" s="5" t="s">
         <v>628</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -5134,24 +5140,24 @@
       <c r="E102" s="1">
         <v>603</v>
       </c>
-      <c r="F102" s="1" t="s">
+      <c r="F102" t="s">
         <v>19</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="H102" s="1" t="s">
+      <c r="H102" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="360" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>102</v>
       </c>
       <c r="B103" s="1">
         <v>51</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" s="5" t="s">
         <v>385</v>
       </c>
       <c r="D103" s="1" t="s">
@@ -5160,24 +5166,24 @@
       <c r="E103" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F103" s="1" t="s">
+      <c r="F103" t="s">
         <v>625</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="H103" s="1" t="s">
+      <c r="H103" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>103</v>
       </c>
       <c r="B104" s="1">
         <v>247</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="5" t="s">
         <v>611</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -5186,24 +5192,24 @@
       <c r="E104" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F104" s="1" t="s">
+      <c r="F104" t="s">
         <v>625</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>634</v>
       </c>
-      <c r="H104" s="1" t="s">
+      <c r="H104" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>104</v>
       </c>
       <c r="B105" s="1">
         <v>24</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C105" s="5" t="s">
         <v>388</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -5212,24 +5218,24 @@
       <c r="E105" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F105" s="1" t="s">
+      <c r="F105" t="s">
         <v>625</v>
       </c>
       <c r="G105" s="1" t="s">
         <v>675</v>
       </c>
-      <c r="H105" s="1" t="s">
+      <c r="H105" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>105</v>
       </c>
       <c r="B106" s="1">
         <v>3</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="C106" s="5" t="s">
         <v>637</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -5238,24 +5244,24 @@
       <c r="E106" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F106" s="1" t="s">
+      <c r="F106" t="s">
         <v>622</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="H106" s="1" t="s">
+      <c r="H106" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>106</v>
       </c>
       <c r="B107" s="1">
         <v>13</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C107" s="5" t="s">
         <v>391</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -5264,24 +5270,24 @@
       <c r="E107" s="1">
         <v>603</v>
       </c>
-      <c r="F107" s="1" t="s">
+      <c r="F107" t="s">
         <v>640</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>641</v>
       </c>
-      <c r="H107" s="1" t="s">
+      <c r="H107" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="360" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>107</v>
       </c>
       <c r="B108" s="1">
         <v>48</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C108" s="5" t="s">
         <v>393</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -5290,24 +5296,24 @@
       <c r="E108" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F108" s="1" t="s">
+      <c r="F108" t="s">
         <v>625</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>643</v>
       </c>
-      <c r="H108" s="1" t="s">
+      <c r="H108" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" ht="330" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>108</v>
       </c>
       <c r="B109" s="1">
         <v>48</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C109" s="5" t="s">
         <v>395</v>
       </c>
       <c r="D109" s="1" t="s">
@@ -5316,24 +5322,24 @@
       <c r="E109" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F109" s="1" t="s">
+      <c r="F109" t="s">
         <v>622</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="H109" s="1" t="s">
+      <c r="H109" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>109</v>
       </c>
       <c r="B110" s="1">
         <v>25</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="C110" s="5" t="s">
         <v>397</v>
       </c>
       <c r="D110" s="1" t="s">
@@ -5342,13 +5348,13 @@
       <c r="E110" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F110" s="1" t="s">
+      <c r="F110" t="s">
         <v>625</v>
       </c>
       <c r="G110" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="H110" s="1" t="s">
+      <c r="H110" t="s">
         <v>648</v>
       </c>
     </row>
@@ -5359,7 +5365,7 @@
       <c r="B111" s="1">
         <v>1</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C111" s="5" t="s">
         <v>401</v>
       </c>
       <c r="D111" s="1" t="s">
@@ -5368,24 +5374,24 @@
       <c r="E111" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F111" s="1" t="s">
+      <c r="F111" t="s">
         <v>622</v>
       </c>
       <c r="G111" s="1" t="s">
         <v>649</v>
       </c>
-      <c r="H111" s="1" t="s">
+      <c r="H111" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>111</v>
       </c>
       <c r="B112" s="1">
         <v>7</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C112" s="5" t="s">
         <v>403</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -5394,13 +5400,13 @@
       <c r="E112" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F112" s="1" t="s">
+      <c r="F112" t="s">
         <v>622</v>
       </c>
       <c r="G112" s="1" t="s">
         <v>651</v>
       </c>
-      <c r="H112" s="1" t="s">
+      <c r="H112" t="s">
         <v>652</v>
       </c>
     </row>
@@ -5411,7 +5417,7 @@
       <c r="B113" s="1">
         <v>2</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C113" s="5" t="s">
         <v>405</v>
       </c>
       <c r="D113" s="1" t="s">
@@ -5420,13 +5426,13 @@
       <c r="E113" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F113" s="1" t="s">
+      <c r="F113" t="s">
         <v>625</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>653</v>
       </c>
-      <c r="H113" s="1" t="s">
+      <c r="H113" t="s">
         <v>654</v>
       </c>
     </row>
@@ -5437,7 +5443,7 @@
       <c r="B114" s="1">
         <v>1</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C114" s="5" t="s">
         <v>407</v>
       </c>
       <c r="D114" s="1" t="s">
@@ -5446,24 +5452,24 @@
       <c r="E114" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F114" s="1" t="s">
+      <c r="F114" t="s">
         <v>625</v>
       </c>
       <c r="G114" s="1" t="s">
         <v>655</v>
       </c>
-      <c r="H114" s="1" t="s">
+      <c r="H114" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>114</v>
       </c>
       <c r="B115" s="1">
         <v>24</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C115" s="5" t="s">
         <v>409</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -5472,24 +5478,24 @@
       <c r="E115" s="1">
         <v>603</v>
       </c>
-      <c r="F115" s="1" t="s">
+      <c r="F115" t="s">
         <v>657</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>658</v>
       </c>
-      <c r="H115" s="1" t="s">
+      <c r="H115" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>115</v>
       </c>
       <c r="B116" s="1">
         <v>26</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C116" s="5" t="s">
         <v>660</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -5498,13 +5504,13 @@
       <c r="E116" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F116" s="1" t="s">
+      <c r="F116" t="s">
         <v>622</v>
       </c>
       <c r="G116" s="1" t="s">
         <v>661</v>
       </c>
-      <c r="H116" s="1" t="s">
+      <c r="H116" t="s">
         <v>662</v>
       </c>
     </row>
@@ -5515,7 +5521,7 @@
       <c r="B117" s="1">
         <v>1</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C117" s="5" t="s">
         <v>612</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -5524,24 +5530,24 @@
       <c r="E117" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F117" s="1" t="s">
+      <c r="F117" t="s">
         <v>663</v>
       </c>
       <c r="G117" s="1" t="s">
         <v>664</v>
       </c>
-      <c r="H117" s="1" t="s">
+      <c r="H117" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>117</v>
       </c>
       <c r="B118" s="1">
         <v>8</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C118" s="5" t="s">
         <v>413</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -5550,13 +5556,13 @@
       <c r="E118" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F118" s="1" t="s">
+      <c r="F118" t="s">
         <v>622</v>
       </c>
       <c r="G118" s="1" t="s">
         <v>666</v>
       </c>
-      <c r="H118" s="1" t="s">
+      <c r="H118" t="s">
         <v>667</v>
       </c>
     </row>
@@ -5567,7 +5573,7 @@
       <c r="B119" s="1">
         <v>2</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C119" s="5" t="s">
         <v>677</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -5576,13 +5582,13 @@
       <c r="E119" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F119" s="1" t="s">
+      <c r="F119" t="s">
         <v>625</v>
       </c>
       <c r="G119" s="1" t="s">
         <v>668</v>
       </c>
-      <c r="H119" s="1" t="s">
+      <c r="H119" t="s">
         <v>669</v>
       </c>
     </row>
@@ -5593,7 +5599,7 @@
       <c r="B120" s="1">
         <v>1</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C120" s="5" t="s">
         <v>416</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -5602,13 +5608,13 @@
       <c r="E120" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F120" s="1" t="s">
+      <c r="F120" t="s">
         <v>622</v>
       </c>
       <c r="G120" s="1" t="s">
         <v>670</v>
       </c>
-      <c r="H120" s="1" t="s">
+      <c r="H120" t="s">
         <v>671</v>
       </c>
     </row>
@@ -5619,7 +5625,7 @@
       <c r="B121" s="1">
         <v>24</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="C121" s="5" t="s">
         <v>399</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -5628,24 +5634,24 @@
       <c r="E121" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="F121" s="1" t="s">
+      <c r="F121" t="s">
         <v>622</v>
       </c>
       <c r="G121" s="1" t="s">
         <v>670</v>
       </c>
-      <c r="H121" s="1" t="s">
+      <c r="H121" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" ht="375" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>121</v>
       </c>
       <c r="B122" s="1">
         <v>102</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="C122" s="5" t="s">
         <v>672</v>
       </c>
       <c r="D122" s="1" t="s">
@@ -5654,13 +5660,13 @@
       <c r="E122" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F122" s="1" t="s">
+      <c r="F122" t="s">
         <v>622</v>
       </c>
       <c r="G122" s="1" t="s">
         <v>673</v>
       </c>
-      <c r="H122" s="1" t="s">
+      <c r="H122" t="s">
         <v>674</v>
       </c>
     </row>
@@ -5671,7 +5677,7 @@
       <c r="B123" s="1">
         <v>1</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="C123" s="5" t="s">
         <v>419</v>
       </c>
       <c r="D123" s="1" t="s">
@@ -5680,13 +5686,13 @@
       <c r="E123" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F123" s="1" t="s">
+      <c r="F123" t="s">
         <v>625</v>
       </c>
       <c r="G123" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="H123" s="1" t="s">
+      <c r="H123" t="s">
         <v>679</v>
       </c>
     </row>
@@ -5697,7 +5703,7 @@
       <c r="B124" s="1">
         <v>1</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="C124" s="5" t="s">
         <v>421</v>
       </c>
       <c r="D124" s="1" t="s">
@@ -5706,24 +5712,24 @@
       <c r="E124" s="1">
         <v>603</v>
       </c>
-      <c r="F124" s="1" t="s">
+      <c r="F124" t="s">
         <v>657</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>680</v>
       </c>
-      <c r="H124" s="1" t="s">
+      <c r="H124" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" ht="315" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>124</v>
       </c>
       <c r="B125" s="1">
         <v>55</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C125" s="5" t="s">
         <v>423</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -5732,24 +5738,24 @@
       <c r="E125" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F125" s="1" t="s">
+      <c r="F125" t="s">
         <v>622</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>682</v>
       </c>
-      <c r="H125" s="1" t="s">
+      <c r="H125" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>125</v>
       </c>
       <c r="B126" s="1">
         <v>25</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="C126" s="5" t="s">
         <v>684</v>
       </c>
       <c r="D126" s="1" t="s">
@@ -5758,24 +5764,24 @@
       <c r="E126" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="F126" s="1" t="s">
+      <c r="F126" t="s">
         <v>625</v>
       </c>
       <c r="G126" s="1" t="s">
         <v>686</v>
       </c>
-      <c r="H126" s="1" t="s">
+      <c r="H126" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>126</v>
       </c>
       <c r="B127" s="1">
         <v>9</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="C127" s="5" t="s">
         <v>707</v>
       </c>
       <c r="D127" s="1" t="s">
@@ -5784,13 +5790,13 @@
       <c r="E127" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F127" s="1" t="s">
+      <c r="F127" t="s">
         <v>622</v>
       </c>
       <c r="G127" s="1" t="s">
         <v>688</v>
       </c>
-      <c r="H127" s="1" t="s">
+      <c r="H127" t="s">
         <v>689</v>
       </c>
     </row>
@@ -5801,7 +5807,7 @@
       <c r="B128" s="1">
         <v>1</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="C128" s="5" t="s">
         <v>613</v>
       </c>
       <c r="D128" s="1" t="s">
@@ -5810,13 +5816,13 @@
       <c r="E128" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F128" s="1" t="s">
+      <c r="F128" t="s">
         <v>622</v>
       </c>
       <c r="G128" s="1" t="s">
         <v>690</v>
       </c>
-      <c r="H128" s="1" t="s">
+      <c r="H128" t="s">
         <v>691</v>
       </c>
     </row>
@@ -5827,7 +5833,7 @@
       <c r="B129" s="1">
         <v>2</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="C129" s="5" t="s">
         <v>426</v>
       </c>
       <c r="D129" s="1" t="s">
@@ -5836,13 +5842,13 @@
       <c r="E129" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F129" s="1" t="s">
+      <c r="F129" t="s">
         <v>625</v>
       </c>
       <c r="G129" s="1" t="s">
         <v>690</v>
       </c>
-      <c r="H129" s="1" t="s">
+      <c r="H129" t="s">
         <v>691</v>
       </c>
     </row>
@@ -5853,7 +5859,7 @@
       <c r="B130" s="1">
         <v>1</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="C130" s="5" t="s">
         <v>428</v>
       </c>
       <c r="D130" s="1" t="s">
@@ -5862,13 +5868,13 @@
       <c r="E130" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F130" s="1" t="s">
+      <c r="F130" t="s">
         <v>625</v>
       </c>
       <c r="G130" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="H130" s="1" t="s">
+      <c r="H130" t="s">
         <v>693</v>
       </c>
     </row>
@@ -5879,7 +5885,7 @@
       <c r="B131" s="1">
         <v>2</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="C131" s="5" t="s">
         <v>430</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -5888,13 +5894,13 @@
       <c r="E131" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F131" s="1" t="s">
+      <c r="F131" t="s">
         <v>625</v>
       </c>
       <c r="G131" s="1" t="s">
         <v>694</v>
       </c>
-      <c r="H131" s="1" t="s">
+      <c r="H131" t="s">
         <v>695</v>
       </c>
     </row>
@@ -5905,7 +5911,7 @@
       <c r="B132" s="1">
         <v>1</v>
       </c>
-      <c r="C132" s="1" t="s">
+      <c r="C132" s="5" t="s">
         <v>432</v>
       </c>
       <c r="D132" s="1" t="s">
@@ -5914,24 +5920,24 @@
       <c r="E132" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F132" s="1" t="s">
+      <c r="F132" t="s">
         <v>625</v>
       </c>
       <c r="G132" s="1" t="s">
         <v>696</v>
       </c>
-      <c r="H132" s="1" t="s">
+      <c r="H132" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>132</v>
       </c>
       <c r="B133" s="1">
         <v>89</v>
       </c>
-      <c r="C133" s="1" t="s">
+      <c r="C133" s="5" t="s">
         <v>615</v>
       </c>
       <c r="D133" s="1" t="s">
@@ -5940,21 +5946,21 @@
       <c r="E133" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F133" s="1" t="s">
+      <c r="F133" t="s">
         <v>200</v>
       </c>
       <c r="G133" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" ht="315" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>133</v>
       </c>
       <c r="B134" s="1">
         <v>48</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="C134" s="5" t="s">
         <v>435</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -5963,13 +5969,13 @@
       <c r="E134" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="F134" s="1" t="s">
+      <c r="F134" t="s">
         <v>438</v>
       </c>
       <c r="G134" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="H134" s="1" t="s">
+      <c r="H134" t="s">
         <v>440</v>
       </c>
     </row>
@@ -5980,7 +5986,7 @@
       <c r="B135" s="1">
         <v>66</v>
       </c>
-      <c r="C135" s="1" t="s">
+      <c r="C135" s="5" t="s">
         <v>441</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -5989,13 +5995,13 @@
       <c r="E135" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="F135" s="1" t="s">
+      <c r="F135" t="s">
         <v>444</v>
       </c>
       <c r="G135" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="H135" s="1" t="s">
+      <c r="H135" t="s">
         <v>446</v>
       </c>
     </row>
@@ -6006,7 +6012,7 @@
       <c r="B136" s="1">
         <v>1</v>
       </c>
-      <c r="C136" s="1" t="s">
+      <c r="C136" s="5" t="s">
         <v>447</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -6015,13 +6021,13 @@
       <c r="E136" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="F136" s="1" t="s">
+      <c r="F136" t="s">
         <v>450</v>
       </c>
       <c r="G136" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="H136" s="1" t="s">
+      <c r="H136" t="s">
         <v>452</v>
       </c>
     </row>
@@ -6032,7 +6038,7 @@
       <c r="B137" s="1">
         <v>6</v>
       </c>
-      <c r="C137" s="1" t="s">
+      <c r="C137" s="5" t="s">
         <v>453</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -6041,13 +6047,13 @@
       <c r="E137" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="F137" s="1" t="s">
+      <c r="F137" t="s">
         <v>456</v>
       </c>
       <c r="G137" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="H137" s="1" t="s">
+      <c r="H137" t="s">
         <v>457</v>
       </c>
     </row>
@@ -6058,7 +6064,7 @@
       <c r="B138" s="1">
         <v>1</v>
       </c>
-      <c r="C138" s="1" t="s">
+      <c r="C138" s="5" t="s">
         <v>458</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -6067,13 +6073,13 @@
       <c r="E138" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="F138" s="1" t="s">
+      <c r="F138" t="s">
         <v>461</v>
       </c>
       <c r="G138" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="H138" s="1" t="s">
+      <c r="H138" t="s">
         <v>463</v>
       </c>
     </row>
@@ -6084,7 +6090,7 @@
       <c r="B139" s="1">
         <v>2</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="C139" s="5" t="s">
         <v>464</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -6093,21 +6099,21 @@
       <c r="E139" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="F139" s="1" t="s">
+      <c r="F139" t="s">
         <v>466</v>
       </c>
       <c r="G139" s="1" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>139</v>
       </c>
       <c r="B140" s="1">
         <v>30</v>
       </c>
-      <c r="C140" s="1" t="s">
+      <c r="C140" s="5" t="s">
         <v>468</v>
       </c>
       <c r="D140" s="1" t="s">
@@ -6116,24 +6122,24 @@
       <c r="E140" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="F140" s="1" t="s">
+      <c r="F140" t="s">
         <v>471</v>
       </c>
       <c r="G140" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="H140" s="1" t="s">
+      <c r="H140" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>140</v>
       </c>
       <c r="B141" s="1">
         <v>24</v>
       </c>
-      <c r="C141" s="1" t="s">
+      <c r="C141" s="5" t="s">
         <v>473</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -6142,24 +6148,24 @@
       <c r="E141" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="F141" s="1" t="s">
+      <c r="F141" t="s">
         <v>471</v>
       </c>
       <c r="G141" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="H141" s="1" t="s">
+      <c r="H141" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>141</v>
       </c>
       <c r="B142" s="1">
         <v>23</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="C142" s="5" t="s">
         <v>478</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -6168,24 +6174,24 @@
       <c r="E142" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="F142" s="1" t="s">
+      <c r="F142" t="s">
         <v>481</v>
       </c>
       <c r="G142" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="H142" s="1" t="s">
+      <c r="H142" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>142</v>
       </c>
       <c r="B143" s="1">
         <v>7</v>
       </c>
-      <c r="C143" s="1" t="s">
+      <c r="C143" s="5" t="s">
         <v>484</v>
       </c>
       <c r="D143" s="1" t="s">
@@ -6194,13 +6200,13 @@
       <c r="E143" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="F143" s="1" t="s">
+      <c r="F143" t="s">
         <v>444</v>
       </c>
       <c r="G143" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="H143" s="1" t="s">
+      <c r="H143" t="s">
         <v>487</v>
       </c>
     </row>
@@ -6211,7 +6217,7 @@
       <c r="B144" s="1">
         <v>1</v>
       </c>
-      <c r="C144" s="1" t="s">
+      <c r="C144" s="5" t="s">
         <v>488</v>
       </c>
       <c r="D144" s="1" t="s">
@@ -6220,13 +6226,13 @@
       <c r="E144" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="F144" s="1" t="s">
+      <c r="F144" t="s">
         <v>491</v>
       </c>
       <c r="G144" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="H144" s="1" t="s">
+      <c r="H144" t="s">
         <v>493</v>
       </c>
     </row>
@@ -6237,7 +6243,7 @@
       <c r="B145" s="1">
         <v>2</v>
       </c>
-      <c r="C145" s="1" t="s">
+      <c r="C145" s="5" t="s">
         <v>494</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -6246,24 +6252,24 @@
       <c r="E145" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="F145" s="1" t="s">
+      <c r="F145" t="s">
         <v>200</v>
       </c>
       <c r="G145" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H145" s="1" t="s">
+      <c r="H145" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>145</v>
       </c>
       <c r="B146" s="1">
         <v>24</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="C146" s="5" t="s">
         <v>497</v>
       </c>
       <c r="D146" s="1" t="s">
@@ -6272,13 +6278,13 @@
       <c r="E146" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="F146" s="1" t="s">
+      <c r="F146" t="s">
         <v>456</v>
       </c>
-      <c r="G146" t="s">
+      <c r="G146" s="1" t="s">
         <v>710</v>
       </c>
-      <c r="H146" s="1" t="s">
+      <c r="H146" t="s">
         <v>500</v>
       </c>
     </row>
@@ -6289,7 +6295,7 @@
       <c r="B147" s="1">
         <v>1</v>
       </c>
-      <c r="C147" s="1" t="s">
+      <c r="C147" s="5" t="s">
         <v>501</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -6298,24 +6304,24 @@
       <c r="E147" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="F147" s="1" t="s">
+      <c r="F147" t="s">
         <v>456</v>
       </c>
       <c r="G147" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="H147" s="1" t="s">
+      <c r="H147" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>147</v>
       </c>
       <c r="B148" s="1">
         <v>24</v>
       </c>
-      <c r="C148" s="1" t="s">
+      <c r="C148" s="5" t="s">
         <v>504</v>
       </c>
       <c r="D148" s="1" t="s">
@@ -6324,24 +6330,24 @@
       <c r="E148" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="F148" s="1" t="s">
+      <c r="F148" t="s">
         <v>111</v>
       </c>
       <c r="G148" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="H148" s="1" t="s">
+      <c r="H148" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>148</v>
       </c>
       <c r="B149" s="1">
         <v>125</v>
       </c>
-      <c r="C149" s="1" t="s">
+      <c r="C149" s="5" t="s">
         <v>508</v>
       </c>
       <c r="D149" s="1" t="s">
@@ -6350,13 +6356,13 @@
       <c r="E149" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="F149" s="1" t="s">
+      <c r="F149" t="s">
         <v>200</v>
       </c>
       <c r="G149" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H149" s="1" t="s">
+      <c r="H149" t="s">
         <v>708</v>
       </c>
     </row>
@@ -6367,7 +6373,7 @@
       <c r="B150" s="1">
         <v>1</v>
       </c>
-      <c r="C150" s="1" t="s">
+      <c r="C150" s="5" t="s">
         <v>511</v>
       </c>
       <c r="D150" s="1" t="s">
@@ -6376,13 +6382,13 @@
       <c r="E150" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="F150" s="1" t="s">
+      <c r="F150" t="s">
         <v>188</v>
       </c>
       <c r="G150" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="H150" s="1" t="s">
+      <c r="H150" t="s">
         <v>514</v>
       </c>
     </row>
@@ -6393,7 +6399,7 @@
       <c r="B151" s="1">
         <v>1</v>
       </c>
-      <c r="C151" s="1" t="s">
+      <c r="C151" s="5" t="s">
         <v>515</v>
       </c>
       <c r="D151" s="1" t="s">
@@ -6402,13 +6408,13 @@
       <c r="E151" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="F151" s="1" t="s">
+      <c r="F151" t="s">
         <v>188</v>
       </c>
       <c r="G151" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="H151" s="1" t="s">
+      <c r="H151" t="s">
         <v>518</v>
       </c>
     </row>
@@ -6419,7 +6425,7 @@
       <c r="B152" s="1">
         <v>1</v>
       </c>
-      <c r="C152" s="1" t="s">
+      <c r="C152" s="5" t="s">
         <v>519</v>
       </c>
       <c r="D152" s="1" t="s">
@@ -6428,13 +6434,13 @@
       <c r="E152" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="F152" s="1" t="s">
+      <c r="F152" t="s">
         <v>188</v>
       </c>
       <c r="G152" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="H152" s="1" t="s">
+      <c r="H152" t="s">
         <v>518</v>
       </c>
     </row>
@@ -6445,7 +6451,7 @@
       <c r="B153" s="1">
         <v>1</v>
       </c>
-      <c r="C153" s="1" t="s">
+      <c r="C153" s="5" t="s">
         <v>521</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -6454,13 +6460,13 @@
       <c r="E153" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="F153" s="1" t="s">
+      <c r="F153" t="s">
         <v>188</v>
       </c>
       <c r="G153" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="H153" s="1" t="s">
+      <c r="H153" t="s">
         <v>524</v>
       </c>
     </row>
@@ -6471,7 +6477,7 @@
       <c r="B154" s="1">
         <v>1</v>
       </c>
-      <c r="C154" s="1" t="s">
+      <c r="C154" s="5" t="s">
         <v>525</v>
       </c>
       <c r="D154" s="1" t="s">
@@ -6480,13 +6486,13 @@
       <c r="E154" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="F154" s="1" t="s">
+      <c r="F154" t="s">
         <v>188</v>
       </c>
       <c r="G154" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="H154" s="1" t="s">
+      <c r="H154" t="s">
         <v>528</v>
       </c>
     </row>
@@ -6497,7 +6503,7 @@
       <c r="B155" s="1">
         <v>1</v>
       </c>
-      <c r="C155" s="1" t="s">
+      <c r="C155" s="5" t="s">
         <v>529</v>
       </c>
       <c r="D155" s="1" t="s">
@@ -6506,13 +6512,13 @@
       <c r="E155" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="F155" s="1" t="s">
+      <c r="F155" t="s">
         <v>188</v>
       </c>
       <c r="G155" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="H155" s="1" t="s">
+      <c r="H155" t="s">
         <v>532</v>
       </c>
     </row>
@@ -6523,7 +6529,7 @@
       <c r="B156" s="1">
         <v>1</v>
       </c>
-      <c r="C156" s="1" t="s">
+      <c r="C156" s="5" t="s">
         <v>533</v>
       </c>
       <c r="D156" s="1" t="s">
@@ -6532,13 +6538,13 @@
       <c r="E156" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="F156" s="1" t="s">
+      <c r="F156" t="s">
         <v>188</v>
       </c>
       <c r="G156" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="H156" s="1" t="s">
+      <c r="H156" t="s">
         <v>536</v>
       </c>
     </row>
@@ -6549,7 +6555,7 @@
       <c r="B157" s="1">
         <v>1</v>
       </c>
-      <c r="C157" s="1" t="s">
+      <c r="C157" s="5" t="s">
         <v>537</v>
       </c>
       <c r="D157" s="1" t="s">
@@ -6558,13 +6564,13 @@
       <c r="E157" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="F157" s="1" t="s">
+      <c r="F157" t="s">
         <v>540</v>
       </c>
       <c r="G157" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="H157" s="1" t="s">
+      <c r="H157" t="s">
         <v>542</v>
       </c>
     </row>
@@ -6575,7 +6581,7 @@
       <c r="B158" s="1">
         <v>1</v>
       </c>
-      <c r="C158" s="1" t="s">
+      <c r="C158" s="5" t="s">
         <v>543</v>
       </c>
       <c r="D158" s="1" t="s">
@@ -6584,13 +6590,13 @@
       <c r="E158" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="F158" s="1" t="s">
+      <c r="F158" t="s">
         <v>546</v>
       </c>
       <c r="G158" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="H158" s="1" t="s">
+      <c r="H158" t="s">
         <v>548</v>
       </c>
     </row>
@@ -6601,7 +6607,7 @@
       <c r="B159" s="1">
         <v>1</v>
       </c>
-      <c r="C159" s="1" t="s">
+      <c r="C159" s="5" t="s">
         <v>549</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -6610,24 +6616,24 @@
       <c r="E159" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="F159" s="1" t="s">
+      <c r="F159" t="s">
         <v>352</v>
       </c>
       <c r="G159" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="H159" s="1" t="s">
+      <c r="H159" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>159</v>
       </c>
       <c r="B160" s="1">
         <v>7</v>
       </c>
-      <c r="C160" s="1" t="s">
+      <c r="C160" s="5" t="s">
         <v>553</v>
       </c>
       <c r="D160" s="1" t="s">
@@ -6636,13 +6642,13 @@
       <c r="E160" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="F160" s="1" t="s">
+      <c r="F160" t="s">
         <v>188</v>
       </c>
       <c r="G160" s="1" t="s">
         <v>636</v>
       </c>
-      <c r="H160" s="1" t="s">
+      <c r="H160" t="s">
         <v>556</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update inductor to larger size/correct value, fix BOM for 3.3V regulator
</commit_message>
<xml_diff>
--- a/radiant_bom.xlsx
+++ b/radiant_bom.xlsx
@@ -633,18 +633,9 @@
     <t>L18</t>
   </si>
   <si>
-    <t>DFE201612E-2R2M=P2</t>
-  </si>
-  <si>
-    <t>INDC2016X120N</t>
-  </si>
-  <si>
     <t>Murata Electronics</t>
   </si>
   <si>
-    <t>Fixed Inductors 0806 2.2uH 20% 2.4A</t>
-  </si>
-  <si>
     <t>D1-24 D27 D30-53</t>
   </si>
   <si>
@@ -1629,15 +1620,9 @@
     <t>U23</t>
   </si>
   <si>
-    <t>TPS627451DSST</t>
-  </si>
-  <si>
     <t>SON50P200X300X80-13N</t>
   </si>
   <si>
-    <t>TEXAS INSTRUMENTS - TPS627451DSST - DC/DC CONV, SYNC BUCK, 2.5MHZ, WSON-12</t>
-  </si>
-  <si>
     <t>V57</t>
   </si>
   <si>
@@ -2164,6 +2149,21 @@
   </si>
   <si>
     <t>Conn Shrouded Header (4 Sides) HDR 14 POS 2mm Solder ST Top Entry SMD Milli-Grid™ Tube</t>
+  </si>
+  <si>
+    <t>TPS62745DSST</t>
+  </si>
+  <si>
+    <t>TEXAS INSTRUMENTS - TPS62745DSST - DC/DC CONV, SYNC BUCK, 2.5MHZ, WSON-12</t>
+  </si>
+  <si>
+    <t>DFE322520FD-4R7M=P2</t>
+  </si>
+  <si>
+    <t>FIXED IND 4.7UH 3400MA INFOTNMNT</t>
+  </si>
+  <si>
+    <t>1210</t>
   </si>
 </sst>
 </file>
@@ -2509,8 +2509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,10 +3117,10 @@
         <v>117</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="H23" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -3195,10 +3195,10 @@
         <v>93</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="H26" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -3221,10 +3221,10 @@
         <v>93</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="H27" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="150" x14ac:dyDescent="0.25">
@@ -3244,13 +3244,13 @@
         <v>92</v>
       </c>
       <c r="F28" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="H28" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="405" x14ac:dyDescent="0.25">
@@ -3270,13 +3270,13 @@
         <v>92</v>
       </c>
       <c r="F29" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="H29" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -3296,13 +3296,13 @@
         <v>92</v>
       </c>
       <c r="F30" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="H30" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3313,7 +3313,7 @@
         <v>10</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>137</v>
@@ -3325,10 +3325,10 @@
         <v>93</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="H31" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3351,10 +3351,10 @@
         <v>93</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="H32" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3377,10 +3377,10 @@
         <v>93</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="H33" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -3403,10 +3403,10 @@
         <v>93</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="H34" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3429,10 +3429,10 @@
         <v>87</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="H35" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="270" x14ac:dyDescent="0.25">
@@ -3452,13 +3452,13 @@
         <v>92</v>
       </c>
       <c r="F36" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="H36" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3469,7 +3469,7 @@
         <v>7</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>148</v>
@@ -3481,10 +3481,10 @@
         <v>93</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="H37" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3504,13 +3504,13 @@
         <v>92</v>
       </c>
       <c r="F38" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="H38" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -3533,10 +3533,10 @@
         <v>93</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="H39" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3556,13 +3556,13 @@
         <v>92</v>
       </c>
       <c r="F40" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="H40" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -3585,10 +3585,10 @@
         <v>93</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="H41" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="195" x14ac:dyDescent="0.25">
@@ -3611,10 +3611,10 @@
         <v>120</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="H42" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3628,7 +3628,7 @@
         <v>165</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>116</v>
@@ -3637,10 +3637,10 @@
         <v>87</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="H43" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3663,10 +3663,10 @@
         <v>111</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="H44" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3689,10 +3689,10 @@
         <v>87</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="H45" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3712,13 +3712,13 @@
         <v>92</v>
       </c>
       <c r="F46" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="H46" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3738,13 +3738,13 @@
         <v>168</v>
       </c>
       <c r="F47" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="H47" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3767,10 +3767,10 @@
         <v>120</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="H48" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -3793,10 +3793,10 @@
         <v>111</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="H49" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -3819,10 +3819,10 @@
         <v>93</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="H50" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -3842,13 +3842,13 @@
         <v>92</v>
       </c>
       <c r="F51" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="H51" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -3871,10 +3871,10 @@
         <v>93</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="H52" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -4018,19 +4018,19 @@
         <v>201</v>
       </c>
       <c r="D58" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="F58" t="s">
         <v>202</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F58" t="s">
-        <v>204</v>
-      </c>
       <c r="G58" s="1" t="s">
-        <v>202</v>
+        <v>710</v>
       </c>
       <c r="H58" t="s">
-        <v>205</v>
+        <v>711</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4041,19 +4041,19 @@
         <v>49</v>
       </c>
       <c r="C59" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F59" t="s">
         <v>206</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="G59" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F59" t="s">
-        <v>209</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -4064,19 +4064,19 @@
         <v>1</v>
       </c>
       <c r="C60" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F60" t="s">
         <v>211</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="G60" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="F60" t="s">
-        <v>214</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -4087,22 +4087,22 @@
         <v>1</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F61" t="s">
         <v>69</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H61" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4113,22 +4113,22 @@
         <v>4</v>
       </c>
       <c r="C62" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F62" t="s">
+        <v>211</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="H62" t="s">
         <v>221</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F62" t="s">
-        <v>214</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="H62" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -4139,19 +4139,19 @@
         <v>6</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E63" s="1">
         <v>402</v>
       </c>
       <c r="F63" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -4162,13 +4162,13 @@
         <v>2</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F64" t="s">
         <v>200</v>
@@ -4188,19 +4188,19 @@
         <v>102</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E65" s="1">
         <v>603</v>
       </c>
       <c r="F65" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="240" x14ac:dyDescent="0.25">
@@ -4211,10 +4211,10 @@
         <v>48</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E66" s="1">
         <v>603</v>
@@ -4234,10 +4234,10 @@
         <v>24</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E67" s="1">
         <v>805</v>
@@ -4246,7 +4246,7 @@
         <v>87</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -4257,22 +4257,22 @@
         <v>1</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E68" s="1">
         <v>805</v>
       </c>
       <c r="F68" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H68" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -4283,22 +4283,22 @@
         <v>1</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E69" s="1">
         <v>805</v>
       </c>
       <c r="F69" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="H69" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -4309,22 +4309,22 @@
         <v>1</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E70" s="1">
         <v>805</v>
       </c>
       <c r="F70" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H70" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="240" x14ac:dyDescent="0.25">
@@ -4335,22 +4335,22 @@
         <v>48</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E71" s="1">
         <v>805</v>
       </c>
       <c r="F71" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H71" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -4361,22 +4361,22 @@
         <v>1</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E72" s="1">
         <v>805</v>
       </c>
       <c r="F72" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H72" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -4387,10 +4387,10 @@
         <v>1</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E73" s="1">
         <v>878321422</v>
@@ -4399,10 +4399,10 @@
         <v>13</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="H73" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -4413,22 +4413,22 @@
         <v>24</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F74" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="H74" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -4439,22 +4439,22 @@
         <v>2</v>
       </c>
       <c r="C75" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F75" t="s">
         <v>264</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="G75" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="H75" t="s">
         <v>266</v>
-      </c>
-      <c r="F75" t="s">
-        <v>267</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="H75" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -4465,22 +4465,22 @@
         <v>1</v>
       </c>
       <c r="C76" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F76" t="s">
         <v>270</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="G76" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="H76" t="s">
         <v>272</v>
-      </c>
-      <c r="F76" t="s">
-        <v>273</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="H76" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -4491,22 +4491,22 @@
         <v>1</v>
       </c>
       <c r="C77" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F77" t="s">
         <v>276</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="G77" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="H77" t="s">
         <v>278</v>
-      </c>
-      <c r="F77" t="s">
-        <v>279</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="H77" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4517,22 +4517,22 @@
         <v>6</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F78" t="s">
         <v>69</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="H78" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -4543,22 +4543,22 @@
         <v>2</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F79" t="s">
         <v>69</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="H79" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -4569,22 +4569,22 @@
         <v>24</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F80" t="s">
         <v>69</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="H80" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -4595,19 +4595,19 @@
         <v>24</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G81" s="1">
         <v>733660061</v>
       </c>
       <c r="H81" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -4618,22 +4618,22 @@
         <v>1</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="F82" t="s">
         <v>69</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="H82" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -4644,22 +4644,22 @@
         <v>1</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="F83" t="s">
         <v>69</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="H83" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -4670,22 +4670,22 @@
         <v>24</v>
       </c>
       <c r="C84" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F84" t="s">
         <v>311</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="G84" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="H84" t="s">
         <v>313</v>
-      </c>
-      <c r="F84" t="s">
-        <v>314</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="H84" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -4696,22 +4696,22 @@
         <v>24</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F85" t="s">
         <v>69</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="H85" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -4722,13 +4722,13 @@
         <v>1</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="F86" t="s">
         <v>13</v>
@@ -4737,7 +4737,7 @@
         <v>1050270001</v>
       </c>
       <c r="H86" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -4748,19 +4748,19 @@
         <v>1</v>
       </c>
       <c r="C87" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="F87" t="s">
         <v>324</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="G87" s="1" t="s">
         <v>325</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="F87" t="s">
-        <v>327</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -4771,22 +4771,22 @@
         <v>74</v>
       </c>
       <c r="C88" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F88" t="s">
+        <v>224</v>
+      </c>
+      <c r="G88" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="H88" t="s">
         <v>330</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="F88" t="s">
-        <v>227</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="H88" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4797,22 +4797,22 @@
         <v>6</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="F89" t="s">
         <v>81</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="H89" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -4823,22 +4823,22 @@
         <v>2</v>
       </c>
       <c r="C90" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="F90" t="s">
         <v>338</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="G90" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="H90" t="s">
         <v>339</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="F90" t="s">
-        <v>341</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="H90" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4849,22 +4849,22 @@
         <v>24</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="F91" t="s">
+        <v>338</v>
+      </c>
+      <c r="G91" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="G91" s="1" t="s">
-        <v>344</v>
-      </c>
       <c r="H91" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -4875,22 +4875,22 @@
         <v>4</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F92" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="H92" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -4901,22 +4901,22 @@
         <v>1</v>
       </c>
       <c r="C93" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="F93" t="s">
         <v>349</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="G93" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="H93" t="s">
         <v>350</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="F93" t="s">
-        <v>352</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="H93" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4927,13 +4927,13 @@
         <v>18</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F94" t="s">
         <v>200</v>
@@ -4953,22 +4953,22 @@
         <v>2</v>
       </c>
       <c r="C95" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="F95" t="s">
+        <v>224</v>
+      </c>
+      <c r="G95" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="H95" t="s">
         <v>358</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="F95" t="s">
-        <v>227</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="H95" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -4979,22 +4979,22 @@
         <v>1</v>
       </c>
       <c r="C96" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="F96" t="s">
         <v>362</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="G96" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="H96" t="s">
         <v>363</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="F96" t="s">
-        <v>365</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="H96" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -5005,19 +5005,19 @@
         <v>1</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="F97" t="s">
         <v>69</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="165" x14ac:dyDescent="0.25">
@@ -5028,22 +5028,22 @@
         <v>24</v>
       </c>
       <c r="C98" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="F98" t="s">
+        <v>370</v>
+      </c>
+      <c r="G98" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="H98" t="s">
         <v>372</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="F98" t="s">
-        <v>373</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="H98" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -5054,22 +5054,22 @@
         <v>49</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F99" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="H99" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5080,22 +5080,22 @@
         <v>6</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F100" t="s">
         <v>182</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="H100" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="345" x14ac:dyDescent="0.25">
@@ -5106,22 +5106,22 @@
         <v>73</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F101" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="H101" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5132,10 +5132,10 @@
         <v>6</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="E102" s="1">
         <v>603</v>
@@ -5144,10 +5144,10 @@
         <v>19</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="H102" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -5158,22 +5158,22 @@
         <v>51</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F103" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="H103" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -5184,22 +5184,22 @@
         <v>247</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F104" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="H104" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="180" x14ac:dyDescent="0.25">
@@ -5210,22 +5210,22 @@
         <v>24</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F105" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="H105" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5236,22 +5236,22 @@
         <v>3</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F106" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="H106" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -5262,22 +5262,22 @@
         <v>13</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="E107" s="1">
         <v>603</v>
       </c>
       <c r="F107" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="H107" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -5288,22 +5288,22 @@
         <v>48</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F108" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="H108" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="330" x14ac:dyDescent="0.25">
@@ -5314,22 +5314,22 @@
         <v>48</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F109" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="H109" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="180" x14ac:dyDescent="0.25">
@@ -5340,22 +5340,22 @@
         <v>25</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F110" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="H110" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -5366,22 +5366,22 @@
         <v>1</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F111" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="H111" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5392,22 +5392,22 @@
         <v>7</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F112" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="H112" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -5418,22 +5418,22 @@
         <v>2</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F113" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="H113" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -5444,22 +5444,22 @@
         <v>1</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F114" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="H114" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -5470,22 +5470,22 @@
         <v>24</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E115" s="1">
         <v>603</v>
       </c>
       <c r="F115" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="H115" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="150" x14ac:dyDescent="0.25">
@@ -5496,22 +5496,22 @@
         <v>26</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F116" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="H116" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -5522,22 +5522,22 @@
         <v>1</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F117" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="H117" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5548,22 +5548,22 @@
         <v>8</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F118" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="H118" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -5574,22 +5574,22 @@
         <v>2</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F119" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="H119" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -5600,22 +5600,22 @@
         <v>1</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F120" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="H120" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -5626,22 +5626,22 @@
         <v>24</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F121" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="H121" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="375" x14ac:dyDescent="0.25">
@@ -5652,22 +5652,22 @@
         <v>102</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F122" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="H122" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -5678,22 +5678,22 @@
         <v>1</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F123" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="H123" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -5704,22 +5704,22 @@
         <v>1</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="E124" s="1">
         <v>603</v>
       </c>
       <c r="F124" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="H124" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="315" x14ac:dyDescent="0.25">
@@ -5730,22 +5730,22 @@
         <v>55</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F125" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="H125" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5756,22 +5756,22 @@
         <v>25</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F126" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="H126" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -5782,22 +5782,22 @@
         <v>9</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F127" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="H127" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -5808,22 +5808,22 @@
         <v>1</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F128" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="H128" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -5834,22 +5834,22 @@
         <v>2</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F129" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="H129" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -5860,22 +5860,22 @@
         <v>1</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F130" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="H130" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -5886,22 +5886,22 @@
         <v>2</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F131" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="H131" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -5912,22 +5912,22 @@
         <v>1</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F132" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="H132" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -5938,13 +5938,13 @@
         <v>89</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F133" t="s">
         <v>200</v>
@@ -5961,22 +5961,22 @@
         <v>48</v>
       </c>
       <c r="C134" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="F134" t="s">
         <v>435</v>
       </c>
-      <c r="D134" s="1" t="s">
+      <c r="G134" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="E134" s="1" t="s">
+      <c r="H134" t="s">
         <v>437</v>
-      </c>
-      <c r="F134" t="s">
-        <v>438</v>
-      </c>
-      <c r="G134" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="H134" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -5987,22 +5987,22 @@
         <v>66</v>
       </c>
       <c r="C135" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="F135" t="s">
         <v>441</v>
       </c>
-      <c r="D135" s="1" t="s">
+      <c r="G135" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="E135" s="1" t="s">
+      <c r="H135" t="s">
         <v>443</v>
-      </c>
-      <c r="F135" t="s">
-        <v>444</v>
-      </c>
-      <c r="G135" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="H135" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -6013,22 +6013,22 @@
         <v>1</v>
       </c>
       <c r="C136" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="F136" t="s">
         <v>447</v>
       </c>
-      <c r="D136" s="1" t="s">
+      <c r="G136" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="E136" s="1" t="s">
+      <c r="H136" t="s">
         <v>449</v>
-      </c>
-      <c r="F136" t="s">
-        <v>450</v>
-      </c>
-      <c r="G136" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="H136" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -6039,22 +6039,22 @@
         <v>6</v>
       </c>
       <c r="C137" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="F137" t="s">
         <v>453</v>
       </c>
-      <c r="D137" s="1" t="s">
+      <c r="G137" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="H137" t="s">
         <v>454</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="F137" t="s">
-        <v>456</v>
-      </c>
-      <c r="G137" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="H137" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -6065,22 +6065,22 @@
         <v>1</v>
       </c>
       <c r="C138" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="F138" t="s">
         <v>458</v>
       </c>
-      <c r="D138" s="1" t="s">
+      <c r="G138" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="E138" s="1" t="s">
+      <c r="H138" t="s">
         <v>460</v>
-      </c>
-      <c r="F138" t="s">
-        <v>461</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="H138" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -6091,19 +6091,19 @@
         <v>2</v>
       </c>
       <c r="C139" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="F139" t="s">
+        <v>463</v>
+      </c>
+      <c r="G139" s="1" t="s">
         <v>464</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="F139" t="s">
-        <v>466</v>
-      </c>
-      <c r="G139" s="1" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -6114,22 +6114,22 @@
         <v>30</v>
       </c>
       <c r="C140" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="F140" t="s">
         <v>468</v>
       </c>
-      <c r="D140" s="1" t="s">
+      <c r="G140" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="H140" t="s">
         <v>469</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="F140" t="s">
-        <v>471</v>
-      </c>
-      <c r="G140" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="H140" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="141" spans="1:8" ht="165" x14ac:dyDescent="0.25">
@@ -6140,22 +6140,22 @@
         <v>24</v>
       </c>
       <c r="C141" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="F141" t="s">
+        <v>468</v>
+      </c>
+      <c r="G141" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="D141" s="1" t="s">
+      <c r="H141" t="s">
         <v>474</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="F141" t="s">
-        <v>471</v>
-      </c>
-      <c r="G141" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="H141" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="142" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -6166,22 +6166,22 @@
         <v>23</v>
       </c>
       <c r="C142" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="F142" t="s">
         <v>478</v>
       </c>
-      <c r="D142" s="1" t="s">
+      <c r="G142" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="E142" s="1" t="s">
+      <c r="H142" t="s">
         <v>480</v>
-      </c>
-      <c r="F142" t="s">
-        <v>481</v>
-      </c>
-      <c r="G142" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="H142" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="143" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -6192,22 +6192,22 @@
         <v>7</v>
       </c>
       <c r="C143" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="F143" t="s">
+        <v>441</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="H143" t="s">
         <v>484</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="F143" t="s">
-        <v>444</v>
-      </c>
-      <c r="G143" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="H143" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -6218,22 +6218,22 @@
         <v>1</v>
       </c>
       <c r="C144" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="F144" t="s">
         <v>488</v>
       </c>
-      <c r="D144" s="1" t="s">
+      <c r="G144" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="E144" s="1" t="s">
+      <c r="H144" t="s">
         <v>490</v>
-      </c>
-      <c r="F144" t="s">
-        <v>491</v>
-      </c>
-      <c r="G144" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="H144" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -6244,13 +6244,13 @@
         <v>2</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="F145" t="s">
         <v>200</v>
@@ -6259,7 +6259,7 @@
         <v>200</v>
       </c>
       <c r="H145" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="146" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -6270,22 +6270,22 @@
         <v>24</v>
       </c>
       <c r="C146" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="F146" t="s">
+        <v>453</v>
+      </c>
+      <c r="G146" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="H146" t="s">
         <v>497</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="F146" t="s">
-        <v>456</v>
-      </c>
-      <c r="G146" s="1" t="s">
-        <v>710</v>
-      </c>
-      <c r="H146" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -6296,22 +6296,22 @@
         <v>1</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="E147" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="F147" t="s">
+        <v>453</v>
+      </c>
+      <c r="G147" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="F147" t="s">
-        <v>456</v>
-      </c>
-      <c r="G147" s="1" t="s">
-        <v>502</v>
-      </c>
       <c r="H147" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -6322,22 +6322,22 @@
         <v>24</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="F148" t="s">
         <v>111</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="H148" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="149" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -6348,13 +6348,13 @@
         <v>125</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="F149" t="s">
         <v>200</v>
@@ -6363,7 +6363,7 @@
         <v>200</v>
       </c>
       <c r="H149" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -6374,22 +6374,22 @@
         <v>1</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="F150" t="s">
         <v>188</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="H150" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -6400,22 +6400,22 @@
         <v>1</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="F151" t="s">
         <v>188</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="H151" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -6426,22 +6426,22 @@
         <v>1</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="F152" t="s">
         <v>188</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="H152" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -6452,22 +6452,22 @@
         <v>1</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="F153" t="s">
         <v>188</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="H153" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -6478,22 +6478,22 @@
         <v>1</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="F154" t="s">
         <v>188</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="H154" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -6504,22 +6504,22 @@
         <v>1</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="F155" t="s">
         <v>188</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="H155" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -6530,22 +6530,22 @@
         <v>1</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>534</v>
+        <v>708</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="F156" t="s">
         <v>188</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>534</v>
+        <v>708</v>
       </c>
       <c r="H156" t="s">
-        <v>536</v>
+        <v>709</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
@@ -6556,22 +6556,22 @@
         <v>1</v>
       </c>
       <c r="C157" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="F157" t="s">
+        <v>535</v>
+      </c>
+      <c r="G157" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="H157" t="s">
         <v>537</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="F157" t="s">
-        <v>540</v>
-      </c>
-      <c r="G157" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="H157" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -6582,22 +6582,22 @@
         <v>1</v>
       </c>
       <c r="C158" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="F158" t="s">
+        <v>541</v>
+      </c>
+      <c r="G158" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="H158" t="s">
         <v>543</v>
-      </c>
-      <c r="D158" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="F158" t="s">
-        <v>546</v>
-      </c>
-      <c r="G158" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="H158" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -6608,22 +6608,22 @@
         <v>1</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="F159" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="H159" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
     </row>
     <row r="160" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -6634,22 +6634,22 @@
         <v>7</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="F160" t="s">
         <v>188</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="H160" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>
@@ -6670,31 +6670,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>693</v>
+      </c>
+      <c r="B1" t="s">
+        <v>694</v>
+      </c>
+      <c r="C1" t="s">
+        <v>695</v>
+      </c>
+      <c r="D1" t="s">
+        <v>696</v>
+      </c>
+      <c r="E1" t="s">
+        <v>697</v>
+      </c>
+      <c r="F1" t="s">
         <v>698</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>699</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>700</v>
       </c>
-      <c r="D1" t="s">
-        <v>701</v>
-      </c>
-      <c r="E1" t="s">
-        <v>702</v>
-      </c>
-      <c r="F1" t="s">
-        <v>703</v>
-      </c>
-      <c r="G1" t="s">
-        <v>704</v>
-      </c>
-      <c r="H1" t="s">
-        <v>705</v>
-      </c>
       <c r="I1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed line items 44, 120, 128 (wrong p/n). line item 150 was a duplicate, deleted
</commit_message>
<xml_diff>
--- a/radiant_bom.xlsx
+++ b/radiant_bom.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="726">
   <si>
     <t>Item</t>
   </si>
@@ -1557,9 +1557,6 @@
     <t>Texas Instruments 15A, 3m? eFuse with Accurate Current Monitor and Configurable Retry Timers 24-VQFN -40 to 125</t>
   </si>
   <si>
-    <t>U21</t>
-  </si>
-  <si>
     <t>TPS54225PWPR</t>
   </si>
   <si>
@@ -1569,12 +1566,6 @@
     <t>4.5 V to 18 V input, 2 A synchronous step-down converter in HTSSOP package</t>
   </si>
   <si>
-    <t>U22</t>
-  </si>
-  <si>
-    <t>SOP65P640X120-15NA</t>
-  </si>
-  <si>
     <t>U19</t>
   </si>
   <si>
@@ -1704,9 +1695,6 @@
     <t>CAP CER MLCC - SMD/SMT 1.0UF 16V 10% 0402</t>
   </si>
   <si>
-    <t>Walsin</t>
-  </si>
-  <si>
     <t>04025A2R2KAT2A</t>
   </si>
   <si>
@@ -1863,12 +1851,6 @@
     <t>CAP CER MLCC - SMD/SMT 0402 100V 470pF 5% SOFT C0G AEC-Q200</t>
   </si>
   <si>
-    <t>HMK105B7472KV-F</t>
-  </si>
-  <si>
-    <t>CAP CER MLCC - SMD/SMT 0402 100V 4700pF 5% C0G</t>
-  </si>
-  <si>
     <t>Stackpole</t>
   </si>
   <si>
@@ -2176,6 +2158,51 @@
   </si>
   <si>
     <t>RADIANTv1 Bill of Materials</t>
+  </si>
+  <si>
+    <t>U21-22</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>157</t>
+  </si>
+  <si>
+    <t>158</t>
+  </si>
+  <si>
+    <t>RC0402FR-076K04L</t>
+  </si>
+  <si>
+    <t>RES SMD 6.04K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RMCF0201FT4K70</t>
+  </si>
+  <si>
+    <t>RES 4.7K OHM 1% 1/20W 0201</t>
+  </si>
+  <si>
+    <t>CC0402KRX7R6BB473</t>
+  </si>
+  <si>
+    <t>CAP CER 0.047UF 10V X7R 0402</t>
   </si>
 </sst>
 </file>
@@ -2326,9 +2353,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2338,10 +2362,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2622,9 +2649,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H162"/>
+  <dimension ref="A1:H161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2639,20 +2668,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>716</v>
+      <c r="A1" s="17" t="s">
+        <v>710</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="8" t="s">
-        <v>714</v>
-      </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="18" t="s">
-        <v>715</v>
-      </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="D2" s="18" t="s">
+        <v>708</v>
+      </c>
+      <c r="E2" s="18"/>
+      <c r="F2" s="19" t="s">
+        <v>709</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -2665,18 +2694,18 @@
         <v>2</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>713</v>
+        <v>707</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2696,13 +2725,13 @@
       <c r="E4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="12">
         <v>744071039</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="13" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2722,13 +2751,13 @@
       <c r="E5" s="6">
         <v>21471100001</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2748,13 +2777,13 @@
       <c r="E6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="13" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2774,13 +2803,13 @@
       <c r="E7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="13" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2800,13 +2829,13 @@
       <c r="E8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="13" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2826,13 +2855,13 @@
       <c r="E9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="13" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2852,13 +2881,13 @@
       <c r="E10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="12">
         <v>39281043</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="13" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2878,13 +2907,13 @@
       <c r="E11" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="13" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2904,13 +2933,13 @@
       <c r="E12" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="13" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2930,13 +2959,13 @@
       <c r="E13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="13" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2956,13 +2985,13 @@
       <c r="E14" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="13" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2982,13 +3011,13 @@
       <c r="E15" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="13" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3008,13 +3037,13 @@
       <c r="E16" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="13" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3034,13 +3063,13 @@
       <c r="E17" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="13" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3060,13 +3089,13 @@
       <c r="E18" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="13" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3086,13 +3115,13 @@
       <c r="E19" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="13" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3112,13 +3141,13 @@
       <c r="E20" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="13" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3138,13 +3167,13 @@
       <c r="E21" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="H21" s="14" t="s">
+      <c r="H21" s="13" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3164,13 +3193,13 @@
       <c r="E22" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="G22" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="H22" s="13" t="s">
         <v>102</v>
       </c>
     </row>
@@ -3190,13 +3219,13 @@
       <c r="E23" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G23" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="13" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3216,13 +3245,13 @@
       <c r="E24" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="13" t="s">
         <v>112</v>
       </c>
     </row>
@@ -3242,14 +3271,14 @@
       <c r="E25" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="G25" s="13" t="s">
-        <v>549</v>
-      </c>
-      <c r="H25" s="14" t="s">
-        <v>550</v>
+      <c r="G25" s="12" t="s">
+        <v>546</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -3268,13 +3297,13 @@
       <c r="E26" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="G26" s="13" t="s">
+      <c r="G26" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="H26" s="14" t="s">
+      <c r="H26" s="13" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3294,13 +3323,13 @@
       <c r="E27" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="13" t="s">
         <v>125</v>
       </c>
     </row>
@@ -3320,14 +3349,14 @@
       <c r="E28" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G28" s="13" t="s">
-        <v>551</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>552</v>
+      <c r="G28" s="12" t="s">
+        <v>548</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -3346,14 +3375,14 @@
       <c r="E29" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="F29" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G29" s="13" t="s">
-        <v>553</v>
-      </c>
-      <c r="H29" s="14" t="s">
-        <v>554</v>
+      <c r="G29" s="12" t="s">
+        <v>550</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="150" x14ac:dyDescent="0.25">
@@ -3372,14 +3401,14 @@
       <c r="E30" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="G30" s="13" t="s">
-        <v>555</v>
-      </c>
-      <c r="H30" s="14" t="s">
-        <v>556</v>
+      <c r="G30" s="12" t="s">
+        <v>552</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="405" x14ac:dyDescent="0.25">
@@ -3398,14 +3427,14 @@
       <c r="E31" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="G31" s="13" t="s">
-        <v>557</v>
-      </c>
-      <c r="H31" s="14" t="s">
-        <v>558</v>
+      <c r="G31" s="12" t="s">
+        <v>554</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -3424,14 +3453,14 @@
       <c r="E32" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F32" s="12" t="s">
-        <v>559</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>560</v>
-      </c>
-      <c r="H32" s="14" t="s">
-        <v>561</v>
+      <c r="F32" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>556</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3442,7 +3471,7 @@
         <v>10</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>136</v>
@@ -3450,14 +3479,14 @@
       <c r="E33" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F33" s="12" t="s">
+      <c r="F33" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G33" s="13" t="s">
-        <v>562</v>
-      </c>
-      <c r="H33" s="14" t="s">
-        <v>563</v>
+      <c r="G33" s="12" t="s">
+        <v>558</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3476,14 +3505,14 @@
       <c r="E34" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="F34" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G34" s="13" t="s">
-        <v>564</v>
-      </c>
-      <c r="H34" s="14" t="s">
-        <v>565</v>
+      <c r="G34" s="12" t="s">
+        <v>560</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3502,14 +3531,14 @@
       <c r="E35" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F35" s="12" t="s">
+      <c r="F35" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G35" s="13" t="s">
-        <v>566</v>
-      </c>
-      <c r="H35" s="14" t="s">
-        <v>567</v>
+      <c r="G35" s="12" t="s">
+        <v>562</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -3528,14 +3557,14 @@
       <c r="E36" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F36" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G36" s="13" t="s">
-        <v>569</v>
-      </c>
-      <c r="H36" s="14" t="s">
-        <v>570</v>
+      <c r="G36" s="12" t="s">
+        <v>565</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3554,14 +3583,14 @@
       <c r="E37" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="F37" s="12" t="s">
+      <c r="F37" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="G37" s="13" t="s">
-        <v>571</v>
-      </c>
-      <c r="H37" s="14" t="s">
-        <v>572</v>
+      <c r="G37" s="12" t="s">
+        <v>567</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="270" x14ac:dyDescent="0.25">
@@ -3580,14 +3609,14 @@
       <c r="E38" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F38" s="12" t="s">
+      <c r="F38" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="G38" s="13" t="s">
-        <v>573</v>
-      </c>
-      <c r="H38" s="14" t="s">
-        <v>574</v>
+      <c r="G38" s="12" t="s">
+        <v>569</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3598,7 +3627,7 @@
         <v>7</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>147</v>
@@ -3606,14 +3635,14 @@
       <c r="E39" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F39" s="12" t="s">
+      <c r="F39" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G39" s="13" t="s">
-        <v>576</v>
-      </c>
-      <c r="H39" s="14" t="s">
-        <v>577</v>
+      <c r="G39" s="12" t="s">
+        <v>572</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3632,14 +3661,14 @@
       <c r="E40" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F40" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="G40" s="13" t="s">
-        <v>578</v>
-      </c>
-      <c r="H40" s="14" t="s">
-        <v>579</v>
+      <c r="G40" s="12" t="s">
+        <v>574</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -3658,14 +3687,14 @@
       <c r="E41" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="F41" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G41" s="13" t="s">
-        <v>580</v>
-      </c>
-      <c r="H41" s="14" t="s">
-        <v>581</v>
+      <c r="G41" s="12" t="s">
+        <v>576</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3684,14 +3713,14 @@
       <c r="E42" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F42" s="12" t="s">
+      <c r="F42" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="G42" s="13" t="s">
-        <v>582</v>
-      </c>
-      <c r="H42" s="14" t="s">
-        <v>583</v>
+      <c r="G42" s="12" t="s">
+        <v>578</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -3710,14 +3739,14 @@
       <c r="E43" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F43" s="12" t="s">
+      <c r="F43" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G43" s="13" t="s">
-        <v>584</v>
-      </c>
-      <c r="H43" s="14" t="s">
-        <v>585</v>
+      <c r="G43" s="12" t="s">
+        <v>580</v>
+      </c>
+      <c r="H43" s="13" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="195" x14ac:dyDescent="0.25">
@@ -3736,14 +3765,14 @@
       <c r="E44" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F44" s="12" t="s">
+      <c r="F44" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="G44" s="13" t="s">
-        <v>608</v>
-      </c>
-      <c r="H44" s="14" t="s">
-        <v>609</v>
+      <c r="G44" s="12" t="s">
+        <v>604</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>605</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3757,19 +3786,19 @@
         <v>164</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="F45" s="12" t="s">
+      <c r="F45" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="G45" s="13" t="s">
-        <v>587</v>
-      </c>
-      <c r="H45" s="14" t="s">
-        <v>588</v>
+      <c r="G45" s="12" t="s">
+        <v>583</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3788,14 +3817,14 @@
       <c r="E46" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F46" s="12" t="s">
+      <c r="F46" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="G46" s="13" t="s">
-        <v>610</v>
-      </c>
-      <c r="H46" s="14" t="s">
-        <v>611</v>
+      <c r="G46" s="12" t="s">
+        <v>606</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3814,14 +3843,14 @@
       <c r="E47" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F47" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="G47" s="13" t="s">
-        <v>612</v>
-      </c>
-      <c r="H47" s="14" t="s">
-        <v>613</v>
+      <c r="F47" s="11" t="s">
+        <v>611</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>724</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>725</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3840,14 +3869,14 @@
       <c r="E48" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F48" s="12" t="s">
+      <c r="F48" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="G48" s="13" t="s">
-        <v>589</v>
-      </c>
-      <c r="H48" s="14" t="s">
-        <v>590</v>
+      <c r="G48" s="12" t="s">
+        <v>585</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3866,14 +3895,14 @@
       <c r="E49" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="F49" s="12" t="s">
+      <c r="F49" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="G49" s="13" t="s">
-        <v>591</v>
-      </c>
-      <c r="H49" s="14" t="s">
-        <v>592</v>
+      <c r="G49" s="12" t="s">
+        <v>587</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -3892,14 +3921,14 @@
       <c r="E50" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F50" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="G50" s="13" t="s">
-        <v>593</v>
-      </c>
-      <c r="H50" s="14" t="s">
-        <v>594</v>
+      <c r="G50" s="12" t="s">
+        <v>589</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -3918,14 +3947,14 @@
       <c r="E51" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F51" s="12" t="s">
+      <c r="F51" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="G51" s="13" t="s">
-        <v>595</v>
-      </c>
-      <c r="H51" s="14" t="s">
-        <v>596</v>
+      <c r="G51" s="12" t="s">
+        <v>591</v>
+      </c>
+      <c r="H51" s="13" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -3944,14 +3973,14 @@
       <c r="E52" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F52" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G52" s="13" t="s">
-        <v>597</v>
-      </c>
-      <c r="H52" s="14" t="s">
-        <v>598</v>
+      <c r="G52" s="12" t="s">
+        <v>593</v>
+      </c>
+      <c r="H52" s="13" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -3970,14 +3999,14 @@
       <c r="E53" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="F53" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="G53" s="13" t="s">
-        <v>599</v>
-      </c>
-      <c r="H53" s="14" t="s">
-        <v>600</v>
+      <c r="G53" s="12" t="s">
+        <v>595</v>
+      </c>
+      <c r="H53" s="13" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -3996,14 +4025,14 @@
       <c r="E54" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F54" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G54" s="13" t="s">
-        <v>601</v>
-      </c>
-      <c r="H54" s="14" t="s">
-        <v>602</v>
+      <c r="G54" s="12" t="s">
+        <v>597</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -4022,13 +4051,13 @@
       <c r="E55" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="F55" s="12" t="s">
+      <c r="F55" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="G55" s="13" t="s">
+      <c r="G55" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="H55" s="14" t="s">
+      <c r="H55" s="13" t="s">
         <v>183</v>
       </c>
     </row>
@@ -4048,13 +4077,13 @@
       <c r="E56" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="F56" s="12" t="s">
+      <c r="F56" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="G56" s="13" t="s">
+      <c r="G56" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="H56" s="14" t="s">
+      <c r="H56" s="13" t="s">
         <v>188</v>
       </c>
     </row>
@@ -4074,13 +4103,13 @@
       <c r="E57" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="F57" s="12" t="s">
+      <c r="F57" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="G57" s="13" t="s">
+      <c r="G57" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="H57" s="14" t="s">
+      <c r="H57" s="13" t="s">
         <v>192</v>
       </c>
     </row>
@@ -4100,13 +4129,13 @@
       <c r="E58" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="F58" s="12" t="s">
+      <c r="F58" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="G58" s="13" t="s">
+      <c r="G58" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="H58" s="14" t="s">
+      <c r="H58" s="13" t="s">
         <v>199</v>
       </c>
     </row>
@@ -4126,13 +4155,13 @@
       <c r="E59" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="F59" s="12" t="s">
+      <c r="F59" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="G59" s="13" t="s">
+      <c r="G59" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="H59" s="14" t="s">
+      <c r="H59" s="13" t="s">
         <v>199</v>
       </c>
     </row>
@@ -4147,19 +4176,19 @@
         <v>200</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>708</v>
+        <v>702</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>707</v>
-      </c>
-      <c r="F60" s="12" t="s">
+        <v>701</v>
+      </c>
+      <c r="F60" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="G60" s="13" t="s">
-        <v>709</v>
-      </c>
-      <c r="H60" s="14" t="s">
-        <v>710</v>
+      <c r="G60" s="12" t="s">
+        <v>703</v>
+      </c>
+      <c r="H60" s="13" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4178,13 +4207,13 @@
       <c r="E61" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="F61" s="12" t="s">
+      <c r="F61" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="G61" s="13" t="s">
+      <c r="G61" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="H61" s="14"/>
+      <c r="H61" s="13"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
@@ -4202,13 +4231,13 @@
       <c r="E62" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="F62" s="12" t="s">
+      <c r="F62" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="G62" s="13" t="s">
+      <c r="G62" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="H62" s="14"/>
+      <c r="H62" s="13"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
@@ -4226,13 +4255,13 @@
       <c r="E63" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="F63" s="12" t="s">
+      <c r="F63" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G63" s="13" t="s">
+      <c r="G63" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="H63" s="14" t="s">
+      <c r="H63" s="13" t="s">
         <v>215</v>
       </c>
     </row>
@@ -4252,13 +4281,13 @@
       <c r="E64" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="F64" s="12" t="s">
+      <c r="F64" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="G64" s="13" t="s">
+      <c r="G64" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="H64" s="14" t="s">
+      <c r="H64" s="13" t="s">
         <v>219</v>
       </c>
     </row>
@@ -4278,13 +4307,13 @@
       <c r="E65" s="6">
         <v>402</v>
       </c>
-      <c r="F65" s="12" t="s">
+      <c r="F65" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="G65" s="13" t="s">
+      <c r="G65" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="H65" s="14"/>
+      <c r="H65" s="13"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
@@ -4294,7 +4323,7 @@
         <v>2</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>225</v>
@@ -4302,13 +4331,13 @@
       <c r="E66" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="F66" s="12" t="s">
+      <c r="F66" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="G66" s="13" t="s">
+      <c r="G66" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="H66" s="14" t="s">
+      <c r="H66" s="13" t="s">
         <v>199</v>
       </c>
     </row>
@@ -4328,13 +4357,13 @@
       <c r="E67" s="6">
         <v>603</v>
       </c>
-      <c r="F67" s="12" t="s">
+      <c r="F67" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="G67" s="13" t="s">
+      <c r="G67" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="H67" s="14"/>
+      <c r="H67" s="13"/>
     </row>
     <row r="68" spans="1:8" ht="240" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
@@ -4352,13 +4381,13 @@
       <c r="E68" s="6">
         <v>603</v>
       </c>
-      <c r="F68" s="12" t="s">
+      <c r="F68" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G68" s="13">
+      <c r="G68" s="12">
         <v>744917215</v>
       </c>
-      <c r="H68" s="14"/>
+      <c r="H68" s="13"/>
     </row>
     <row r="69" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
@@ -4376,13 +4405,13 @@
       <c r="E69" s="6">
         <v>805</v>
       </c>
-      <c r="F69" s="12" t="s">
+      <c r="F69" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="G69" s="13" t="s">
+      <c r="G69" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="H69" s="14"/>
+      <c r="H69" s="13"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
@@ -4400,13 +4429,13 @@
       <c r="E70" s="6">
         <v>805</v>
       </c>
-      <c r="F70" s="12" t="s">
+      <c r="F70" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="G70" s="13" t="s">
+      <c r="G70" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="H70" s="14" t="s">
+      <c r="H70" s="13" t="s">
         <v>238</v>
       </c>
     </row>
@@ -4426,13 +4455,13 @@
       <c r="E71" s="6">
         <v>805</v>
       </c>
-      <c r="F71" s="12" t="s">
+      <c r="F71" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="G71" s="13" t="s">
+      <c r="G71" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="H71" s="14" t="s">
+      <c r="H71" s="13" t="s">
         <v>242</v>
       </c>
     </row>
@@ -4452,13 +4481,13 @@
       <c r="E72" s="6">
         <v>805</v>
       </c>
-      <c r="F72" s="12" t="s">
+      <c r="F72" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="G72" s="13" t="s">
+      <c r="G72" s="12" t="s">
         <v>245</v>
       </c>
-      <c r="H72" s="14" t="s">
+      <c r="H72" s="13" t="s">
         <v>246</v>
       </c>
     </row>
@@ -4478,13 +4507,13 @@
       <c r="E73" s="6">
         <v>805</v>
       </c>
-      <c r="F73" s="12" t="s">
+      <c r="F73" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="G73" s="13" t="s">
+      <c r="G73" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="H73" s="14" t="s">
+      <c r="H73" s="13" t="s">
         <v>250</v>
       </c>
     </row>
@@ -4504,13 +4533,13 @@
       <c r="E74" s="6">
         <v>805</v>
       </c>
-      <c r="F74" s="12" t="s">
+      <c r="F74" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="G74" s="13" t="s">
+      <c r="G74" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="H74" s="14" t="s">
+      <c r="H74" s="13" t="s">
         <v>254</v>
       </c>
     </row>
@@ -4530,14 +4559,14 @@
       <c r="E75" s="6">
         <v>878321422</v>
       </c>
-      <c r="F75" s="12" t="s">
+      <c r="F75" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G75" s="13" t="s">
-        <v>703</v>
-      </c>
-      <c r="H75" s="14" t="s">
-        <v>704</v>
+      <c r="G75" s="12" t="s">
+        <v>697</v>
+      </c>
+      <c r="H75" s="13" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -4556,14 +4585,14 @@
       <c r="E76" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="F76" s="12" t="s">
-        <v>701</v>
-      </c>
-      <c r="G76" s="13" t="s">
-        <v>701</v>
-      </c>
-      <c r="H76" s="14" t="s">
-        <v>701</v>
+      <c r="F76" s="11" t="s">
+        <v>695</v>
+      </c>
+      <c r="G76" s="12" t="s">
+        <v>695</v>
+      </c>
+      <c r="H76" s="13" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -4582,13 +4611,13 @@
       <c r="E77" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="F77" s="12" t="s">
+      <c r="F77" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="G77" s="13" t="s">
+      <c r="G77" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="H77" s="14" t="s">
+      <c r="H77" s="13" t="s">
         <v>264</v>
       </c>
     </row>
@@ -4608,13 +4637,13 @@
       <c r="E78" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="F78" s="12" t="s">
+      <c r="F78" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="G78" s="13" t="s">
+      <c r="G78" s="12" t="s">
         <v>269</v>
       </c>
-      <c r="H78" s="14" t="s">
+      <c r="H78" s="13" t="s">
         <v>270</v>
       </c>
     </row>
@@ -4634,13 +4663,13 @@
       <c r="E79" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="F79" s="12" t="s">
+      <c r="F79" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="G79" s="13" t="s">
+      <c r="G79" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="H79" s="14" t="s">
+      <c r="H79" s="13" t="s">
         <v>276</v>
       </c>
     </row>
@@ -4660,13 +4689,13 @@
       <c r="E80" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="F80" s="12" t="s">
+      <c r="F80" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G80" s="13" t="s">
+      <c r="G80" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="H80" s="14" t="s">
+      <c r="H80" s="13" t="s">
         <v>281</v>
       </c>
     </row>
@@ -4686,13 +4715,13 @@
       <c r="E81" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="F81" s="12" t="s">
+      <c r="F81" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G81" s="13" t="s">
+      <c r="G81" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="H81" s="14" t="s">
+      <c r="H81" s="13" t="s">
         <v>286</v>
       </c>
     </row>
@@ -4712,13 +4741,13 @@
       <c r="E82" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="F82" s="12" t="s">
+      <c r="F82" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G82" s="13" t="s">
+      <c r="G82" s="12" t="s">
         <v>290</v>
       </c>
-      <c r="H82" s="14" t="s">
+      <c r="H82" s="13" t="s">
         <v>291</v>
       </c>
     </row>
@@ -4738,11 +4767,11 @@
       <c r="E83" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="F83" s="12"/>
-      <c r="G83" s="13">
+      <c r="F83" s="11"/>
+      <c r="G83" s="12">
         <v>733660061</v>
       </c>
-      <c r="H83" s="14" t="s">
+      <c r="H83" s="13" t="s">
         <v>295</v>
       </c>
     </row>
@@ -4762,13 +4791,13 @@
       <c r="E84" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="F84" s="12" t="s">
+      <c r="F84" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G84" s="13" t="s">
+      <c r="G84" s="12" t="s">
         <v>299</v>
       </c>
-      <c r="H84" s="14" t="s">
+      <c r="H84" s="13" t="s">
         <v>300</v>
       </c>
     </row>
@@ -4788,13 +4817,13 @@
       <c r="E85" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="F85" s="12" t="s">
+      <c r="F85" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G85" s="13" t="s">
+      <c r="G85" s="12" t="s">
         <v>304</v>
       </c>
-      <c r="H85" s="14" t="s">
+      <c r="H85" s="13" t="s">
         <v>305</v>
       </c>
     </row>
@@ -4814,13 +4843,13 @@
       <c r="E86" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="F86" s="12" t="s">
+      <c r="F86" s="11" t="s">
         <v>309</v>
       </c>
-      <c r="G86" s="13" t="s">
+      <c r="G86" s="12" t="s">
         <v>310</v>
       </c>
-      <c r="H86" s="14" t="s">
+      <c r="H86" s="13" t="s">
         <v>311</v>
       </c>
     </row>
@@ -4840,13 +4869,13 @@
       <c r="E87" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="F87" s="12" t="s">
+      <c r="F87" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G87" s="13" t="s">
+      <c r="G87" s="12" t="s">
         <v>313</v>
       </c>
-      <c r="H87" s="14" t="s">
+      <c r="H87" s="13" t="s">
         <v>315</v>
       </c>
     </row>
@@ -4866,13 +4895,13 @@
       <c r="E88" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="F88" s="12" t="s">
+      <c r="F88" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G88" s="13">
+      <c r="G88" s="12">
         <v>1050270001</v>
       </c>
-      <c r="H88" s="14" t="s">
+      <c r="H88" s="13" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4892,13 +4921,13 @@
       <c r="E89" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="F89" s="12" t="s">
+      <c r="F89" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="G89" s="13" t="s">
+      <c r="G89" s="12" t="s">
         <v>323</v>
       </c>
-      <c r="H89" s="14"/>
+      <c r="H89" s="13"/>
     </row>
     <row r="90" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
@@ -4916,13 +4945,13 @@
       <c r="E90" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="F90" s="12" t="s">
+      <c r="F90" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="G90" s="13" t="s">
+      <c r="G90" s="12" t="s">
         <v>327</v>
       </c>
-      <c r="H90" s="14" t="s">
+      <c r="H90" s="13" t="s">
         <v>328</v>
       </c>
     </row>
@@ -4942,13 +4971,13 @@
       <c r="E91" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="F91" s="12" t="s">
+      <c r="F91" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="G91" s="13" t="s">
+      <c r="G91" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="H91" s="14" t="s">
+      <c r="H91" s="13" t="s">
         <v>332</v>
       </c>
     </row>
@@ -4968,13 +4997,13 @@
       <c r="E92" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="F92" s="12" t="s">
+      <c r="F92" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="G92" s="13" t="s">
+      <c r="G92" s="12" t="s">
         <v>334</v>
       </c>
-      <c r="H92" s="14" t="s">
+      <c r="H92" s="13" t="s">
         <v>337</v>
       </c>
     </row>
@@ -4994,13 +5023,13 @@
       <c r="E93" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="F93" s="12" t="s">
+      <c r="F93" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="G93" s="13" t="s">
+      <c r="G93" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="H93" s="14" t="s">
+      <c r="H93" s="13" t="s">
         <v>340</v>
       </c>
     </row>
@@ -5020,13 +5049,13 @@
       <c r="E94" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="F94" s="12" t="s">
+      <c r="F94" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="G94" s="13" t="s">
+      <c r="G94" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="H94" s="14" t="s">
+      <c r="H94" s="13" t="s">
         <v>343</v>
       </c>
     </row>
@@ -5046,13 +5075,13 @@
       <c r="E95" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="F95" s="12" t="s">
+      <c r="F95" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="G95" s="13" t="s">
+      <c r="G95" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="H95" s="14" t="s">
+      <c r="H95" s="13" t="s">
         <v>348</v>
       </c>
     </row>
@@ -5072,13 +5101,13 @@
       <c r="E96" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="F96" s="12" t="s">
+      <c r="F96" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="G96" s="13" t="s">
+      <c r="G96" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="H96" s="14" t="s">
+      <c r="H96" s="13" t="s">
         <v>199</v>
       </c>
     </row>
@@ -5098,13 +5127,13 @@
       <c r="E97" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="F97" s="12" t="s">
+      <c r="F97" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="G97" s="13" t="s">
+      <c r="G97" s="12" t="s">
         <v>355</v>
       </c>
-      <c r="H97" s="14" t="s">
+      <c r="H97" s="13" t="s">
         <v>356</v>
       </c>
     </row>
@@ -5124,13 +5153,13 @@
       <c r="E98" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="F98" s="12" t="s">
+      <c r="F98" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="G98" s="13" t="s">
+      <c r="G98" s="12" t="s">
         <v>358</v>
       </c>
-      <c r="H98" s="14" t="s">
+      <c r="H98" s="13" t="s">
         <v>361</v>
       </c>
     </row>
@@ -5150,13 +5179,13 @@
       <c r="E99" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="F99" s="12" t="s">
+      <c r="F99" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G99" s="13" t="s">
+      <c r="G99" s="12" t="s">
         <v>365</v>
       </c>
-      <c r="H99" s="14"/>
+      <c r="H99" s="13"/>
     </row>
     <row r="100" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
@@ -5174,13 +5203,13 @@
       <c r="E100" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="F100" s="12" t="s">
+      <c r="F100" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="G100" s="13" t="s">
+      <c r="G100" s="12" t="s">
         <v>369</v>
       </c>
-      <c r="H100" s="14" t="s">
+      <c r="H100" s="13" t="s">
         <v>370</v>
       </c>
     </row>
@@ -5200,14 +5229,14 @@
       <c r="E101" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F101" s="12" t="s">
-        <v>614</v>
-      </c>
-      <c r="G101" s="13" t="s">
-        <v>615</v>
-      </c>
-      <c r="H101" s="14" t="s">
-        <v>616</v>
+      <c r="F101" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="G101" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="H101" s="13" t="s">
+        <v>610</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5226,13 +5255,13 @@
       <c r="E102" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F102" s="12" t="s">
+      <c r="F102" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="G102" s="13" t="s">
+      <c r="G102" s="12" t="s">
         <v>376</v>
       </c>
-      <c r="H102" s="14" t="s">
+      <c r="H102" s="13" t="s">
         <v>377</v>
       </c>
     </row>
@@ -5252,14 +5281,14 @@
       <c r="E103" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F103" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="G103" s="13" t="s">
-        <v>618</v>
-      </c>
-      <c r="H103" s="14" t="s">
-        <v>619</v>
+      <c r="F103" s="11" t="s">
+        <v>611</v>
+      </c>
+      <c r="G103" s="12" t="s">
+        <v>612</v>
+      </c>
+      <c r="H103" s="13" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5270,22 +5299,22 @@
         <v>6</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="E104" s="6">
         <v>603</v>
       </c>
-      <c r="F104" s="12" t="s">
+      <c r="F104" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G104" s="13" t="s">
-        <v>622</v>
-      </c>
-      <c r="H104" s="14" t="s">
-        <v>623</v>
+      <c r="G104" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="H104" s="13" t="s">
+        <v>617</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -5304,14 +5333,14 @@
       <c r="E105" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F105" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="G105" s="13" t="s">
-        <v>624</v>
-      </c>
-      <c r="H105" s="14" t="s">
-        <v>625</v>
+      <c r="F105" s="11" t="s">
+        <v>611</v>
+      </c>
+      <c r="G105" s="12" t="s">
+        <v>618</v>
+      </c>
+      <c r="H105" s="13" t="s">
+        <v>619</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -5322,7 +5351,7 @@
         <v>247</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>382</v>
@@ -5330,14 +5359,14 @@
       <c r="E106" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F106" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="G106" s="13" t="s">
-        <v>626</v>
-      </c>
-      <c r="H106" s="14" t="s">
-        <v>627</v>
+      <c r="F106" s="11" t="s">
+        <v>611</v>
+      </c>
+      <c r="G106" s="12" t="s">
+        <v>620</v>
+      </c>
+      <c r="H106" s="13" t="s">
+        <v>621</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="180" x14ac:dyDescent="0.25">
@@ -5356,14 +5385,14 @@
       <c r="E107" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F107" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="G107" s="13" t="s">
-        <v>667</v>
-      </c>
-      <c r="H107" s="14" t="s">
-        <v>668</v>
+      <c r="F107" s="11" t="s">
+        <v>611</v>
+      </c>
+      <c r="G107" s="12" t="s">
+        <v>661</v>
+      </c>
+      <c r="H107" s="13" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5374,7 +5403,7 @@
         <v>3</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>385</v>
@@ -5382,14 +5411,14 @@
       <c r="E108" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F108" s="12" t="s">
-        <v>614</v>
-      </c>
-      <c r="G108" s="13" t="s">
-        <v>630</v>
-      </c>
-      <c r="H108" s="14" t="s">
-        <v>631</v>
+      <c r="F108" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="G108" s="12" t="s">
+        <v>624</v>
+      </c>
+      <c r="H108" s="13" t="s">
+        <v>625</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -5408,14 +5437,14 @@
       <c r="E109" s="6">
         <v>603</v>
       </c>
-      <c r="F109" s="12" t="s">
-        <v>632</v>
-      </c>
-      <c r="G109" s="13" t="s">
-        <v>633</v>
-      </c>
-      <c r="H109" s="14" t="s">
-        <v>634</v>
+      <c r="F109" s="11" t="s">
+        <v>626</v>
+      </c>
+      <c r="G109" s="12" t="s">
+        <v>627</v>
+      </c>
+      <c r="H109" s="13" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -5434,14 +5463,14 @@
       <c r="E110" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F110" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="G110" s="13" t="s">
-        <v>635</v>
-      </c>
-      <c r="H110" s="14" t="s">
-        <v>636</v>
+      <c r="F110" s="11" t="s">
+        <v>611</v>
+      </c>
+      <c r="G110" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="H110" s="13" t="s">
+        <v>630</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="330" x14ac:dyDescent="0.25">
@@ -5460,14 +5489,14 @@
       <c r="E111" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F111" s="12" t="s">
-        <v>614</v>
-      </c>
-      <c r="G111" s="13" t="s">
-        <v>637</v>
-      </c>
-      <c r="H111" s="14" t="s">
-        <v>638</v>
+      <c r="F111" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="G111" s="12" t="s">
+        <v>631</v>
+      </c>
+      <c r="H111" s="13" t="s">
+        <v>632</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="180" x14ac:dyDescent="0.25">
@@ -5486,14 +5515,14 @@
       <c r="E112" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F112" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="G112" s="13" t="s">
-        <v>639</v>
-      </c>
-      <c r="H112" s="14" t="s">
-        <v>640</v>
+      <c r="F112" s="11" t="s">
+        <v>611</v>
+      </c>
+      <c r="G112" s="12" t="s">
+        <v>633</v>
+      </c>
+      <c r="H112" s="13" t="s">
+        <v>634</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -5512,14 +5541,14 @@
       <c r="E113" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F113" s="12" t="s">
-        <v>614</v>
-      </c>
-      <c r="G113" s="13" t="s">
-        <v>641</v>
-      </c>
-      <c r="H113" s="14" t="s">
-        <v>642</v>
+      <c r="F113" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="G113" s="12" t="s">
+        <v>635</v>
+      </c>
+      <c r="H113" s="13" t="s">
+        <v>636</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5538,14 +5567,14 @@
       <c r="E114" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F114" s="12" t="s">
-        <v>614</v>
-      </c>
-      <c r="G114" s="13" t="s">
-        <v>643</v>
-      </c>
-      <c r="H114" s="14" t="s">
-        <v>644</v>
+      <c r="F114" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="G114" s="12" t="s">
+        <v>637</v>
+      </c>
+      <c r="H114" s="13" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -5564,14 +5593,14 @@
       <c r="E115" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F115" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="G115" s="13" t="s">
-        <v>645</v>
-      </c>
-      <c r="H115" s="14" t="s">
-        <v>646</v>
+      <c r="F115" s="11" t="s">
+        <v>611</v>
+      </c>
+      <c r="G115" s="12" t="s">
+        <v>639</v>
+      </c>
+      <c r="H115" s="13" t="s">
+        <v>640</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -5590,14 +5619,14 @@
       <c r="E116" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F116" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="G116" s="13" t="s">
-        <v>647</v>
-      </c>
-      <c r="H116" s="14" t="s">
-        <v>648</v>
+      <c r="F116" s="11" t="s">
+        <v>611</v>
+      </c>
+      <c r="G116" s="12" t="s">
+        <v>641</v>
+      </c>
+      <c r="H116" s="13" t="s">
+        <v>642</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -5616,14 +5645,14 @@
       <c r="E117" s="6">
         <v>603</v>
       </c>
-      <c r="F117" s="12" t="s">
-        <v>649</v>
-      </c>
-      <c r="G117" s="13" t="s">
-        <v>650</v>
-      </c>
-      <c r="H117" s="14" t="s">
-        <v>651</v>
+      <c r="F117" s="11" t="s">
+        <v>643</v>
+      </c>
+      <c r="G117" s="12" t="s">
+        <v>644</v>
+      </c>
+      <c r="H117" s="13" t="s">
+        <v>645</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="150" x14ac:dyDescent="0.25">
@@ -5634,7 +5663,7 @@
         <v>26</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>406</v>
@@ -5642,14 +5671,14 @@
       <c r="E118" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F118" s="12" t="s">
-        <v>614</v>
-      </c>
-      <c r="G118" s="13" t="s">
-        <v>653</v>
-      </c>
-      <c r="H118" s="14" t="s">
-        <v>654</v>
+      <c r="F118" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="G118" s="12" t="s">
+        <v>647</v>
+      </c>
+      <c r="H118" s="13" t="s">
+        <v>648</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -5660,7 +5689,7 @@
         <v>1</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>407</v>
@@ -5668,14 +5697,14 @@
       <c r="E119" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F119" s="12" t="s">
-        <v>655</v>
-      </c>
-      <c r="G119" s="13" t="s">
-        <v>656</v>
-      </c>
-      <c r="H119" s="14" t="s">
-        <v>657</v>
+      <c r="F119" s="11" t="s">
+        <v>649</v>
+      </c>
+      <c r="G119" s="12" t="s">
+        <v>650</v>
+      </c>
+      <c r="H119" s="13" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5694,14 +5723,14 @@
       <c r="E120" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F120" s="12" t="s">
-        <v>614</v>
-      </c>
-      <c r="G120" s="13" t="s">
-        <v>658</v>
-      </c>
-      <c r="H120" s="14" t="s">
-        <v>659</v>
+      <c r="F120" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="G120" s="12" t="s">
+        <v>652</v>
+      </c>
+      <c r="H120" s="13" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -5712,7 +5741,7 @@
         <v>2</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="D121" s="6" t="s">
         <v>410</v>
@@ -5720,14 +5749,14 @@
       <c r="E121" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F121" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="G121" s="13" t="s">
-        <v>660</v>
-      </c>
-      <c r="H121" s="14" t="s">
-        <v>661</v>
+      <c r="F121" s="11" t="s">
+        <v>611</v>
+      </c>
+      <c r="G121" s="12" t="s">
+        <v>654</v>
+      </c>
+      <c r="H121" s="13" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -5746,14 +5775,14 @@
       <c r="E122" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F122" s="12" t="s">
-        <v>614</v>
-      </c>
-      <c r="G122" s="13" t="s">
-        <v>662</v>
-      </c>
-      <c r="H122" s="14" t="s">
-        <v>663</v>
+      <c r="F122" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="G122" s="12" t="s">
+        <v>656</v>
+      </c>
+      <c r="H122" s="13" t="s">
+        <v>657</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -5772,14 +5801,14 @@
       <c r="E123" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="F123" s="12" t="s">
-        <v>614</v>
-      </c>
-      <c r="G123" s="13" t="s">
-        <v>662</v>
-      </c>
-      <c r="H123" s="14" t="s">
-        <v>663</v>
+      <c r="F123" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="G123" s="12" t="s">
+        <v>722</v>
+      </c>
+      <c r="H123" s="13" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="375" x14ac:dyDescent="0.25">
@@ -5790,7 +5819,7 @@
         <v>102</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>413</v>
@@ -5798,14 +5827,14 @@
       <c r="E124" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F124" s="12" t="s">
-        <v>614</v>
-      </c>
-      <c r="G124" s="13" t="s">
-        <v>665</v>
-      </c>
-      <c r="H124" s="14" t="s">
-        <v>666</v>
+      <c r="F124" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="G124" s="12" t="s">
+        <v>659</v>
+      </c>
+      <c r="H124" s="13" t="s">
+        <v>660</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -5824,14 +5853,14 @@
       <c r="E125" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F125" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="G125" s="13" t="s">
-        <v>670</v>
-      </c>
-      <c r="H125" s="14" t="s">
-        <v>671</v>
+      <c r="F125" s="11" t="s">
+        <v>611</v>
+      </c>
+      <c r="G125" s="12" t="s">
+        <v>664</v>
+      </c>
+      <c r="H125" s="13" t="s">
+        <v>665</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -5850,14 +5879,14 @@
       <c r="E126" s="6">
         <v>603</v>
       </c>
-      <c r="F126" s="12" t="s">
-        <v>649</v>
-      </c>
-      <c r="G126" s="13" t="s">
-        <v>672</v>
-      </c>
-      <c r="H126" s="14" t="s">
-        <v>673</v>
+      <c r="F126" s="11" t="s">
+        <v>643</v>
+      </c>
+      <c r="G126" s="12" t="s">
+        <v>666</v>
+      </c>
+      <c r="H126" s="13" t="s">
+        <v>667</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="315" x14ac:dyDescent="0.25">
@@ -5876,14 +5905,14 @@
       <c r="E127" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F127" s="12" t="s">
-        <v>614</v>
-      </c>
-      <c r="G127" s="13" t="s">
-        <v>674</v>
-      </c>
-      <c r="H127" s="14" t="s">
-        <v>675</v>
+      <c r="F127" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="G127" s="12" t="s">
+        <v>668</v>
+      </c>
+      <c r="H127" s="13" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5894,22 +5923,22 @@
         <v>25</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="E128" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="F128" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="G128" s="13" t="s">
-        <v>678</v>
-      </c>
-      <c r="H128" s="14" t="s">
-        <v>679</v>
+      <c r="F128" s="11" t="s">
+        <v>611</v>
+      </c>
+      <c r="G128" s="12" t="s">
+        <v>672</v>
+      </c>
+      <c r="H128" s="13" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -5920,7 +5949,7 @@
         <v>9</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>699</v>
+        <v>693</v>
       </c>
       <c r="D129" s="6" t="s">
         <v>420</v>
@@ -5928,14 +5957,14 @@
       <c r="E129" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F129" s="12" t="s">
-        <v>614</v>
-      </c>
-      <c r="G129" s="13" t="s">
-        <v>680</v>
-      </c>
-      <c r="H129" s="14" t="s">
-        <v>681</v>
+      <c r="F129" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="G129" s="12" t="s">
+        <v>674</v>
+      </c>
+      <c r="H129" s="13" t="s">
+        <v>675</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -5946,22 +5975,22 @@
         <v>1</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="E130" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F130" s="12" t="s">
-        <v>614</v>
-      </c>
-      <c r="G130" s="13" t="s">
-        <v>682</v>
-      </c>
-      <c r="H130" s="14" t="s">
-        <v>683</v>
+      <c r="F130" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="G130" s="12" t="s">
+        <v>676</v>
+      </c>
+      <c r="H130" s="13" t="s">
+        <v>677</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -5980,14 +6009,14 @@
       <c r="E131" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F131" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="G131" s="13" t="s">
-        <v>682</v>
-      </c>
-      <c r="H131" s="14" t="s">
-        <v>683</v>
+      <c r="F131" s="11" t="s">
+        <v>611</v>
+      </c>
+      <c r="G131" s="12" t="s">
+        <v>720</v>
+      </c>
+      <c r="H131" s="13" t="s">
+        <v>721</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -6006,14 +6035,14 @@
       <c r="E132" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F132" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="G132" s="13" t="s">
-        <v>684</v>
-      </c>
-      <c r="H132" s="14" t="s">
-        <v>685</v>
+      <c r="F132" s="11" t="s">
+        <v>611</v>
+      </c>
+      <c r="G132" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H132" s="13" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -6032,14 +6061,14 @@
       <c r="E133" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F133" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="G133" s="13" t="s">
-        <v>686</v>
-      </c>
-      <c r="H133" s="14" t="s">
-        <v>687</v>
+      <c r="F133" s="11" t="s">
+        <v>611</v>
+      </c>
+      <c r="G133" s="12" t="s">
+        <v>680</v>
+      </c>
+      <c r="H133" s="13" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -6058,14 +6087,14 @@
       <c r="E134" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F134" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="G134" s="13" t="s">
-        <v>688</v>
-      </c>
-      <c r="H134" s="14" t="s">
-        <v>689</v>
+      <c r="F134" s="11" t="s">
+        <v>611</v>
+      </c>
+      <c r="G134" s="12" t="s">
+        <v>682</v>
+      </c>
+      <c r="H134" s="13" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -6076,7 +6105,7 @@
         <v>89</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="D135" s="6" t="s">
         <v>429</v>
@@ -6084,13 +6113,13 @@
       <c r="E135" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="F135" s="12" t="s">
+      <c r="F135" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="G135" s="13" t="s">
+      <c r="G135" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="H135" s="14"/>
+      <c r="H135" s="13"/>
     </row>
     <row r="136" spans="1:8" ht="315" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
@@ -6108,13 +6137,13 @@
       <c r="E136" s="6" t="s">
         <v>432</v>
       </c>
-      <c r="F136" s="12" t="s">
+      <c r="F136" s="11" t="s">
         <v>433</v>
       </c>
-      <c r="G136" s="13" t="s">
+      <c r="G136" s="12" t="s">
         <v>434</v>
       </c>
-      <c r="H136" s="14" t="s">
+      <c r="H136" s="13" t="s">
         <v>435</v>
       </c>
     </row>
@@ -6134,13 +6163,13 @@
       <c r="E137" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="F137" s="12" t="s">
+      <c r="F137" s="11" t="s">
         <v>439</v>
       </c>
-      <c r="G137" s="13" t="s">
+      <c r="G137" s="12" t="s">
         <v>440</v>
       </c>
-      <c r="H137" s="14" t="s">
+      <c r="H137" s="13" t="s">
         <v>441</v>
       </c>
     </row>
@@ -6160,13 +6189,13 @@
       <c r="E138" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="F138" s="12" t="s">
+      <c r="F138" s="11" t="s">
         <v>445</v>
       </c>
-      <c r="G138" s="13" t="s">
+      <c r="G138" s="12" t="s">
         <v>446</v>
       </c>
-      <c r="H138" s="14" t="s">
+      <c r="H138" s="13" t="s">
         <v>447</v>
       </c>
     </row>
@@ -6186,13 +6215,13 @@
       <c r="E139" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="F139" s="12" t="s">
+      <c r="F139" s="11" t="s">
         <v>451</v>
       </c>
-      <c r="G139" s="13" t="s">
+      <c r="G139" s="12" t="s">
         <v>449</v>
       </c>
-      <c r="H139" s="14" t="s">
+      <c r="H139" s="13" t="s">
         <v>452</v>
       </c>
     </row>
@@ -6212,13 +6241,13 @@
       <c r="E140" s="6" t="s">
         <v>455</v>
       </c>
-      <c r="F140" s="12" t="s">
+      <c r="F140" s="11" t="s">
         <v>456</v>
       </c>
-      <c r="G140" s="13" t="s">
+      <c r="G140" s="12" t="s">
         <v>457</v>
       </c>
-      <c r="H140" s="14" t="s">
+      <c r="H140" s="13" t="s">
         <v>458</v>
       </c>
     </row>
@@ -6238,13 +6267,13 @@
       <c r="E141" s="6" t="s">
         <v>432</v>
       </c>
-      <c r="F141" s="12" t="s">
+      <c r="F141" s="11" t="s">
         <v>461</v>
       </c>
-      <c r="G141" s="13" t="s">
+      <c r="G141" s="12" t="s">
         <v>462</v>
       </c>
-      <c r="H141" s="14"/>
+      <c r="H141" s="13"/>
     </row>
     <row r="142" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
@@ -6262,13 +6291,13 @@
       <c r="E142" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="F142" s="12" t="s">
+      <c r="F142" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="G142" s="13" t="s">
+      <c r="G142" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="H142" s="14" t="s">
+      <c r="H142" s="13" t="s">
         <v>467</v>
       </c>
     </row>
@@ -6288,13 +6317,13 @@
       <c r="E143" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="F143" s="12" t="s">
+      <c r="F143" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="G143" s="13" t="s">
+      <c r="G143" s="12" t="s">
         <v>471</v>
       </c>
-      <c r="H143" s="14" t="s">
+      <c r="H143" s="13" t="s">
         <v>472</v>
       </c>
     </row>
@@ -6314,13 +6343,13 @@
       <c r="E144" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="F144" s="12" t="s">
+      <c r="F144" s="11" t="s">
         <v>476</v>
       </c>
-      <c r="G144" s="13" t="s">
+      <c r="G144" s="12" t="s">
         <v>477</v>
       </c>
-      <c r="H144" s="14" t="s">
+      <c r="H144" s="13" t="s">
         <v>478</v>
       </c>
     </row>
@@ -6340,13 +6369,13 @@
       <c r="E145" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="F145" s="12" t="s">
+      <c r="F145" s="11" t="s">
         <v>439</v>
       </c>
-      <c r="G145" s="13" t="s">
+      <c r="G145" s="12" t="s">
         <v>481</v>
       </c>
-      <c r="H145" s="14" t="s">
+      <c r="H145" s="13" t="s">
         <v>482</v>
       </c>
     </row>
@@ -6366,13 +6395,13 @@
       <c r="E146" s="6" t="s">
         <v>485</v>
       </c>
-      <c r="F146" s="12" t="s">
+      <c r="F146" s="11" t="s">
         <v>486</v>
       </c>
-      <c r="G146" s="13" t="s">
+      <c r="G146" s="12" t="s">
         <v>487</v>
       </c>
-      <c r="H146" s="14" t="s">
+      <c r="H146" s="13" t="s">
         <v>488</v>
       </c>
     </row>
@@ -6392,13 +6421,13 @@
       <c r="E147" s="6" t="s">
         <v>490</v>
       </c>
-      <c r="F147" s="12" t="s">
+      <c r="F147" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="G147" s="13" t="s">
+      <c r="G147" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="H147" s="14" t="s">
+      <c r="H147" s="13" t="s">
         <v>491</v>
       </c>
     </row>
@@ -6418,13 +6447,13 @@
       <c r="E148" s="6" t="s">
         <v>494</v>
       </c>
-      <c r="F148" s="12" t="s">
+      <c r="F148" s="11" t="s">
         <v>451</v>
       </c>
-      <c r="G148" s="13" t="s">
-        <v>702</v>
-      </c>
-      <c r="H148" s="14" t="s">
+      <c r="G148" s="12" t="s">
+        <v>696</v>
+      </c>
+      <c r="H148" s="13" t="s">
         <v>495</v>
       </c>
     </row>
@@ -6444,13 +6473,13 @@
       <c r="E149" s="6" t="s">
         <v>494</v>
       </c>
-      <c r="F149" s="12" t="s">
+      <c r="F149" s="11" t="s">
         <v>451</v>
       </c>
-      <c r="G149" s="13" t="s">
+      <c r="G149" s="12" t="s">
         <v>497</v>
       </c>
-      <c r="H149" s="14" t="s">
+      <c r="H149" s="13" t="s">
         <v>498</v>
       </c>
     </row>
@@ -6470,13 +6499,13 @@
       <c r="E150" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="F150" s="12" t="s">
+      <c r="F150" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="G150" s="13" t="s">
+      <c r="G150" s="12" t="s">
         <v>501</v>
       </c>
-      <c r="H150" s="14" t="s">
+      <c r="H150" s="13" t="s">
         <v>502</v>
       </c>
     </row>
@@ -6496,14 +6525,14 @@
       <c r="E151" s="6" t="s">
         <v>505</v>
       </c>
-      <c r="F151" s="12" t="s">
+      <c r="F151" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="G151" s="13" t="s">
+      <c r="G151" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="H151" s="14" t="s">
-        <v>700</v>
+      <c r="H151" s="13" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -6522,13 +6551,13 @@
       <c r="E152" s="6" t="s">
         <v>508</v>
       </c>
-      <c r="F152" s="12" t="s">
+      <c r="F152" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="G152" s="13" t="s">
+      <c r="G152" s="12" t="s">
         <v>508</v>
       </c>
-      <c r="H152" s="14" t="s">
+      <c r="H152" s="13" t="s">
         <v>509</v>
       </c>
     </row>
@@ -6540,212 +6569,212 @@
         <v>1</v>
       </c>
       <c r="C153" s="5" t="s">
+        <v>711</v>
+      </c>
+      <c r="D153" s="6" t="s">
         <v>510</v>
       </c>
-      <c r="D153" s="6" t="s">
+      <c r="E153" s="6" t="s">
         <v>511</v>
       </c>
-      <c r="E153" s="6" t="s">
+      <c r="F153" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="G153" s="12" t="s">
+        <v>510</v>
+      </c>
+      <c r="H153" s="13" t="s">
         <v>512</v>
       </c>
-      <c r="F153" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="G153" s="13" t="s">
-        <v>511</v>
-      </c>
-      <c r="H153" s="14" t="s">
-        <v>513</v>
-      </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A154" s="1">
-        <v>151</v>
+      <c r="A154" s="1" t="s">
+        <v>712</v>
       </c>
       <c r="B154" s="1">
         <v>1</v>
       </c>
       <c r="C154" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="D154" s="6" t="s">
         <v>514</v>
-      </c>
-      <c r="D154" s="6" t="s">
-        <v>511</v>
       </c>
       <c r="E154" s="6" t="s">
         <v>515</v>
       </c>
-      <c r="F154" s="12" t="s">
+      <c r="F154" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="G154" s="13" t="s">
-        <v>511</v>
-      </c>
-      <c r="H154" s="14" t="s">
-        <v>513</v>
+      <c r="G154" s="12" t="s">
+        <v>514</v>
+      </c>
+      <c r="H154" s="13" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A155" s="1">
-        <v>152</v>
+      <c r="A155" s="1" t="s">
+        <v>713</v>
       </c>
       <c r="B155" s="1">
         <v>1</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="E155" s="6" t="s">
         <v>518</v>
       </c>
-      <c r="F155" s="12" t="s">
+      <c r="F155" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="G155" s="13" t="s">
-        <v>517</v>
-      </c>
-      <c r="H155" s="14" t="s">
+      <c r="G155" s="12" t="s">
         <v>519</v>
       </c>
+      <c r="H155" s="13" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A156" s="1">
-        <v>153</v>
+      <c r="A156" s="1" t="s">
+        <v>714</v>
       </c>
       <c r="B156" s="1">
         <v>1</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
       <c r="E156" s="6" t="s">
-        <v>521</v>
-      </c>
-      <c r="F156" s="12" t="s">
+        <v>523</v>
+      </c>
+      <c r="F156" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="G156" s="13" t="s">
+      <c r="G156" s="12" t="s">
         <v>522</v>
       </c>
-      <c r="H156" s="14" t="s">
-        <v>523</v>
+      <c r="H156" s="13" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A157" s="1">
-        <v>154</v>
+      <c r="A157" s="1" t="s">
+        <v>715</v>
       </c>
       <c r="B157" s="1">
         <v>1</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>525</v>
+        <v>699</v>
       </c>
       <c r="E157" s="6" t="s">
         <v>526</v>
       </c>
-      <c r="F157" s="12" t="s">
+      <c r="F157" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="G157" s="13" t="s">
-        <v>525</v>
-      </c>
-      <c r="H157" s="14" t="s">
-        <v>527</v>
+      <c r="G157" s="12" t="s">
+        <v>699</v>
+      </c>
+      <c r="H157" s="13" t="s">
+        <v>700</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A158" s="1">
-        <v>155</v>
+      <c r="A158" s="1" t="s">
+        <v>716</v>
       </c>
       <c r="B158" s="1">
         <v>1</v>
       </c>
       <c r="C158" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="D158" s="6" t="s">
         <v>528</v>
-      </c>
-      <c r="D158" s="6" t="s">
-        <v>705</v>
       </c>
       <c r="E158" s="6" t="s">
         <v>529</v>
       </c>
-      <c r="F158" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="G158" s="13" t="s">
-        <v>705</v>
-      </c>
-      <c r="H158" s="14" t="s">
-        <v>706</v>
+      <c r="F158" s="11" t="s">
+        <v>530</v>
+      </c>
+      <c r="G158" s="12" t="s">
+        <v>531</v>
+      </c>
+      <c r="H158" s="13" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A159" s="1">
-        <v>156</v>
+      <c r="A159" s="1" t="s">
+        <v>717</v>
       </c>
       <c r="B159" s="1">
         <v>1</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="E159" s="6" t="s">
-        <v>532</v>
-      </c>
-      <c r="F159" s="12" t="s">
-        <v>533</v>
-      </c>
-      <c r="G159" s="13" t="s">
-        <v>534</v>
-      </c>
-      <c r="H159" s="14" t="s">
         <v>535</v>
       </c>
+      <c r="F159" s="11" t="s">
+        <v>536</v>
+      </c>
+      <c r="G159" s="12" t="s">
+        <v>537</v>
+      </c>
+      <c r="H159" s="13" t="s">
+        <v>538</v>
+      </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A160" s="1">
-        <v>157</v>
+      <c r="A160" s="1" t="s">
+        <v>718</v>
       </c>
       <c r="B160" s="1">
         <v>1</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="D160" s="6" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="E160" s="6" t="s">
-        <v>538</v>
-      </c>
-      <c r="F160" s="12" t="s">
-        <v>539</v>
-      </c>
-      <c r="G160" s="13" t="s">
-        <v>540</v>
-      </c>
-      <c r="H160" s="14" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A161" s="1">
-        <v>158</v>
+      <c r="F160" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="G160" s="12" t="s">
+        <v>705</v>
+      </c>
+      <c r="H160" s="13" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="1" t="s">
+        <v>719</v>
       </c>
       <c r="B161" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C161" s="5" t="s">
         <v>542</v>
@@ -6756,40 +6785,14 @@
       <c r="E161" s="6" t="s">
         <v>544</v>
       </c>
-      <c r="F161" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="G161" s="13" t="s">
-        <v>711</v>
-      </c>
-      <c r="H161" s="14" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="1">
-        <v>159</v>
-      </c>
-      <c r="B162" s="1">
-        <v>7</v>
-      </c>
-      <c r="C162" s="5" t="s">
+      <c r="F161" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="G161" s="15" t="s">
+        <v>622</v>
+      </c>
+      <c r="H161" s="16" t="s">
         <v>545</v>
-      </c>
-      <c r="D162" s="6" t="s">
-        <v>546</v>
-      </c>
-      <c r="E162" s="6" t="s">
-        <v>547</v>
-      </c>
-      <c r="F162" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="G162" s="16" t="s">
-        <v>628</v>
-      </c>
-      <c r="H162" s="17" t="s">
-        <v>548</v>
       </c>
     </row>
   </sheetData>
@@ -6814,28 +6817,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>684</v>
+      </c>
+      <c r="B1" t="s">
+        <v>685</v>
+      </c>
+      <c r="C1" t="s">
+        <v>686</v>
+      </c>
+      <c r="D1" t="s">
+        <v>687</v>
+      </c>
+      <c r="E1" t="s">
+        <v>688</v>
+      </c>
+      <c r="F1" t="s">
+        <v>689</v>
+      </c>
+      <c r="G1" t="s">
         <v>690</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1" t="s">
         <v>691</v>
-      </c>
-      <c r="C1" t="s">
-        <v>692</v>
-      </c>
-      <c r="D1" t="s">
-        <v>693</v>
-      </c>
-      <c r="E1" t="s">
-        <v>694</v>
-      </c>
-      <c r="F1" t="s">
-        <v>695</v>
-      </c>
-      <c r="G1" t="s">
-        <v>696</v>
-      </c>
-      <c r="H1" t="s">
-        <v>697</v>
       </c>
       <c r="I1" t="s">
         <v>224</v>

</xml_diff>

<commit_message>
make sure BOM is updated
</commit_message>
<xml_diff>
--- a/radiant_bom.xlsx
+++ b/radiant_bom.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="725">
   <si>
     <t>Item</t>
   </si>
@@ -589,9 +589,6 @@
   </si>
   <si>
     <t>Texas Instruments</t>
-  </si>
-  <si>
-    <t>Low Jitter, 2-Input Selectable 1:12 Universal-to-LVDS Buffer</t>
   </si>
   <si>
     <t>L16-17</t>
@@ -2669,16 +2666,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" s="18" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E2" s="18"/>
       <c r="F2" s="19" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
@@ -2694,7 +2691,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>3</v>
@@ -3275,10 +3272,10 @@
         <v>116</v>
       </c>
       <c r="G25" s="12" t="s">
+        <v>545</v>
+      </c>
+      <c r="H25" s="13" t="s">
         <v>546</v>
-      </c>
-      <c r="H25" s="13" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -3353,10 +3350,10 @@
         <v>92</v>
       </c>
       <c r="G28" s="12" t="s">
+        <v>547</v>
+      </c>
+      <c r="H28" s="13" t="s">
         <v>548</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -3379,10 +3376,10 @@
         <v>92</v>
       </c>
       <c r="G29" s="12" t="s">
+        <v>549</v>
+      </c>
+      <c r="H29" s="13" t="s">
         <v>550</v>
-      </c>
-      <c r="H29" s="13" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="150" x14ac:dyDescent="0.25">
@@ -3402,13 +3399,13 @@
         <v>91</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G30" s="12" t="s">
+        <v>551</v>
+      </c>
+      <c r="H30" s="13" t="s">
         <v>552</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="405" x14ac:dyDescent="0.25">
@@ -3428,13 +3425,13 @@
         <v>91</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G31" s="12" t="s">
+        <v>553</v>
+      </c>
+      <c r="H31" s="13" t="s">
         <v>554</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -3457,10 +3454,10 @@
         <v>119</v>
       </c>
       <c r="G32" s="12" t="s">
+        <v>555</v>
+      </c>
+      <c r="H32" s="13" t="s">
         <v>556</v>
-      </c>
-      <c r="H32" s="13" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3471,7 +3468,7 @@
         <v>10</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>136</v>
@@ -3483,10 +3480,10 @@
         <v>92</v>
       </c>
       <c r="G33" s="12" t="s">
+        <v>557</v>
+      </c>
+      <c r="H33" s="13" t="s">
         <v>558</v>
-      </c>
-      <c r="H33" s="13" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3509,10 +3506,10 @@
         <v>92</v>
       </c>
       <c r="G34" s="12" t="s">
+        <v>559</v>
+      </c>
+      <c r="H34" s="13" t="s">
         <v>560</v>
-      </c>
-      <c r="H34" s="13" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3535,10 +3532,10 @@
         <v>92</v>
       </c>
       <c r="G35" s="12" t="s">
+        <v>561</v>
+      </c>
+      <c r="H35" s="13" t="s">
         <v>562</v>
-      </c>
-      <c r="H35" s="13" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -3561,10 +3558,10 @@
         <v>92</v>
       </c>
       <c r="G36" s="12" t="s">
+        <v>564</v>
+      </c>
+      <c r="H36" s="13" t="s">
         <v>565</v>
-      </c>
-      <c r="H36" s="13" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3587,10 +3584,10 @@
         <v>86</v>
       </c>
       <c r="G37" s="12" t="s">
+        <v>566</v>
+      </c>
+      <c r="H37" s="13" t="s">
         <v>567</v>
-      </c>
-      <c r="H37" s="13" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="270" x14ac:dyDescent="0.25">
@@ -3610,13 +3607,13 @@
         <v>91</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G38" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="H38" s="13" t="s">
         <v>569</v>
-      </c>
-      <c r="H38" s="13" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3627,7 +3624,7 @@
         <v>7</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>147</v>
@@ -3639,10 +3636,10 @@
         <v>92</v>
       </c>
       <c r="G39" s="12" t="s">
+        <v>571</v>
+      </c>
+      <c r="H39" s="13" t="s">
         <v>572</v>
-      </c>
-      <c r="H39" s="13" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3662,13 +3659,13 @@
         <v>91</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G40" s="12" t="s">
+        <v>573</v>
+      </c>
+      <c r="H40" s="13" t="s">
         <v>574</v>
-      </c>
-      <c r="H40" s="13" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -3691,10 +3688,10 @@
         <v>92</v>
       </c>
       <c r="G41" s="12" t="s">
+        <v>575</v>
+      </c>
+      <c r="H41" s="13" t="s">
         <v>576</v>
-      </c>
-      <c r="H41" s="13" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3714,13 +3711,13 @@
         <v>91</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G42" s="12" t="s">
+        <v>577</v>
+      </c>
+      <c r="H42" s="13" t="s">
         <v>578</v>
-      </c>
-      <c r="H42" s="13" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -3743,10 +3740,10 @@
         <v>92</v>
       </c>
       <c r="G43" s="12" t="s">
+        <v>579</v>
+      </c>
+      <c r="H43" s="13" t="s">
         <v>580</v>
-      </c>
-      <c r="H43" s="13" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="195" x14ac:dyDescent="0.25">
@@ -3769,10 +3766,10 @@
         <v>119</v>
       </c>
       <c r="G44" s="12" t="s">
+        <v>603</v>
+      </c>
+      <c r="H44" s="13" t="s">
         <v>604</v>
-      </c>
-      <c r="H44" s="13" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3786,7 +3783,7 @@
         <v>164</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>115</v>
@@ -3795,10 +3792,10 @@
         <v>86</v>
       </c>
       <c r="G45" s="12" t="s">
+        <v>582</v>
+      </c>
+      <c r="H45" s="13" t="s">
         <v>583</v>
-      </c>
-      <c r="H45" s="13" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3821,10 +3818,10 @@
         <v>110</v>
       </c>
       <c r="G46" s="12" t="s">
+        <v>605</v>
+      </c>
+      <c r="H46" s="13" t="s">
         <v>606</v>
-      </c>
-      <c r="H46" s="13" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3844,13 +3841,13 @@
         <v>91</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G47" s="12" t="s">
+        <v>723</v>
+      </c>
+      <c r="H47" s="13" t="s">
         <v>724</v>
-      </c>
-      <c r="H47" s="13" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3870,13 +3867,13 @@
         <v>91</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G48" s="12" t="s">
+        <v>584</v>
+      </c>
+      <c r="H48" s="13" t="s">
         <v>585</v>
-      </c>
-      <c r="H48" s="13" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3896,13 +3893,13 @@
         <v>167</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G49" s="12" t="s">
+        <v>586</v>
+      </c>
+      <c r="H49" s="13" t="s">
         <v>587</v>
-      </c>
-      <c r="H49" s="13" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -3925,10 +3922,10 @@
         <v>119</v>
       </c>
       <c r="G50" s="12" t="s">
+        <v>588</v>
+      </c>
+      <c r="H50" s="13" t="s">
         <v>589</v>
-      </c>
-      <c r="H50" s="13" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -3951,10 +3948,10 @@
         <v>110</v>
       </c>
       <c r="G51" s="12" t="s">
+        <v>590</v>
+      </c>
+      <c r="H51" s="13" t="s">
         <v>591</v>
-      </c>
-      <c r="H51" s="13" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -3977,10 +3974,10 @@
         <v>92</v>
       </c>
       <c r="G52" s="12" t="s">
+        <v>592</v>
+      </c>
+      <c r="H52" s="13" t="s">
         <v>593</v>
-      </c>
-      <c r="H52" s="13" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -4000,13 +3997,13 @@
         <v>91</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G53" s="12" t="s">
+        <v>594</v>
+      </c>
+      <c r="H53" s="13" t="s">
         <v>595</v>
-      </c>
-      <c r="H53" s="13" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -4029,10 +4026,10 @@
         <v>92</v>
       </c>
       <c r="G54" s="12" t="s">
+        <v>596</v>
+      </c>
+      <c r="H54" s="13" t="s">
         <v>597</v>
-      </c>
-      <c r="H54" s="13" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -4083,8 +4080,8 @@
       <c r="G56" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="H56" s="13" t="s">
-        <v>188</v>
+      <c r="H56" s="13">
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -4095,22 +4092,22 @@
         <v>2</v>
       </c>
       <c r="C57" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D57" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="E57" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>191</v>
       </c>
       <c r="F57" s="11" t="s">
         <v>110</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H57" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -4121,22 +4118,22 @@
         <v>2</v>
       </c>
       <c r="C58" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D58" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="D58" s="6" t="s">
+      <c r="E58" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="E58" s="6" t="s">
-        <v>195</v>
-      </c>
       <c r="F58" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H58" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -4147,22 +4144,22 @@
         <v>6</v>
       </c>
       <c r="C59" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D59" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="E59" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="F59" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="F59" s="11" t="s">
-        <v>199</v>
-      </c>
       <c r="G59" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H59" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -4173,22 +4170,22 @@
         <v>1</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="F60" s="11" t="s">
         <v>110</v>
       </c>
       <c r="G60" s="12" t="s">
+        <v>702</v>
+      </c>
+      <c r="H60" s="13" t="s">
         <v>703</v>
-      </c>
-      <c r="H60" s="13" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4199,19 +4196,19 @@
         <v>49</v>
       </c>
       <c r="C61" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D61" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="E61" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="E61" s="6" t="s">
+      <c r="F61" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="F61" s="11" t="s">
+      <c r="G61" s="12" t="s">
         <v>204</v>
-      </c>
-      <c r="G61" s="12" t="s">
-        <v>205</v>
       </c>
       <c r="H61" s="13"/>
     </row>
@@ -4223,19 +4220,19 @@
         <v>1</v>
       </c>
       <c r="C62" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D62" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="E62" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="E62" s="6" t="s">
+      <c r="F62" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="F62" s="11" t="s">
+      <c r="G62" s="12" t="s">
         <v>209</v>
-      </c>
-      <c r="G62" s="12" t="s">
-        <v>210</v>
       </c>
       <c r="H62" s="13"/>
     </row>
@@ -4247,22 +4244,22 @@
         <v>1</v>
       </c>
       <c r="C63" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D63" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="D63" s="6" t="s">
+      <c r="E63" s="6" t="s">
         <v>212</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>213</v>
       </c>
       <c r="F63" s="11" t="s">
         <v>68</v>
       </c>
       <c r="G63" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="H63" s="13" t="s">
         <v>214</v>
-      </c>
-      <c r="H63" s="13" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4273,22 +4270,22 @@
         <v>4</v>
       </c>
       <c r="C64" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="D64" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="D64" s="6" t="s">
+      <c r="E64" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="F64" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="G64" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="E64" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="F64" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="G64" s="12" t="s">
+      <c r="H64" s="13" t="s">
         <v>218</v>
-      </c>
-      <c r="H64" s="13" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -4299,19 +4296,19 @@
         <v>6</v>
       </c>
       <c r="C65" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D65" s="6" t="s">
         <v>220</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>221</v>
       </c>
       <c r="E65" s="6">
         <v>402</v>
       </c>
       <c r="F65" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="G65" s="12" t="s">
         <v>222</v>
-      </c>
-      <c r="G65" s="12" t="s">
-        <v>223</v>
       </c>
       <c r="H65" s="13"/>
     </row>
@@ -4323,22 +4320,22 @@
         <v>2</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D66" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E66" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="E66" s="6" t="s">
-        <v>226</v>
-      </c>
       <c r="F66" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G66" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -4349,19 +4346,19 @@
         <v>102</v>
       </c>
       <c r="C67" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="D67" s="6" t="s">
         <v>227</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>228</v>
       </c>
       <c r="E67" s="6">
         <v>603</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G67" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H67" s="13"/>
     </row>
@@ -4373,10 +4370,10 @@
         <v>48</v>
       </c>
       <c r="C68" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D68" s="6" t="s">
         <v>230</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>231</v>
       </c>
       <c r="E68" s="6">
         <v>603</v>
@@ -4397,10 +4394,10 @@
         <v>24</v>
       </c>
       <c r="C69" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D69" s="6" t="s">
         <v>232</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>233</v>
       </c>
       <c r="E69" s="6">
         <v>805</v>
@@ -4409,7 +4406,7 @@
         <v>86</v>
       </c>
       <c r="G69" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H69" s="13"/>
     </row>
@@ -4421,22 +4418,22 @@
         <v>1</v>
       </c>
       <c r="C70" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D70" s="6" t="s">
         <v>235</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>236</v>
       </c>
       <c r="E70" s="6">
         <v>805</v>
       </c>
       <c r="F70" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G70" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="H70" s="13" t="s">
         <v>237</v>
-      </c>
-      <c r="H70" s="13" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -4447,22 +4444,22 @@
         <v>1</v>
       </c>
       <c r="C71" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D71" s="6" t="s">
         <v>239</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>240</v>
       </c>
       <c r="E71" s="6">
         <v>805</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G71" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="H71" s="13" t="s">
         <v>241</v>
-      </c>
-      <c r="H71" s="13" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -4473,22 +4470,22 @@
         <v>1</v>
       </c>
       <c r="C72" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="D72" s="6" t="s">
         <v>243</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>244</v>
       </c>
       <c r="E72" s="6">
         <v>805</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G72" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="H72" s="13" t="s">
         <v>245</v>
-      </c>
-      <c r="H72" s="13" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="240" x14ac:dyDescent="0.25">
@@ -4499,22 +4496,22 @@
         <v>48</v>
       </c>
       <c r="C73" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D73" s="6" t="s">
         <v>247</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>248</v>
       </c>
       <c r="E73" s="6">
         <v>805</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G73" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="H73" s="13" t="s">
         <v>249</v>
-      </c>
-      <c r="H73" s="13" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -4525,22 +4522,22 @@
         <v>1</v>
       </c>
       <c r="C74" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="D74" s="6" t="s">
         <v>251</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>252</v>
       </c>
       <c r="E74" s="6">
         <v>805</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G74" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="H74" s="13" t="s">
         <v>253</v>
-      </c>
-      <c r="H74" s="13" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -4551,10 +4548,10 @@
         <v>1</v>
       </c>
       <c r="C75" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="D75" s="6" t="s">
         <v>255</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>256</v>
       </c>
       <c r="E75" s="6">
         <v>878321422</v>
@@ -4563,10 +4560,10 @@
         <v>12</v>
       </c>
       <c r="G75" s="12" t="s">
+        <v>696</v>
+      </c>
+      <c r="H75" s="13" t="s">
         <v>697</v>
-      </c>
-      <c r="H75" s="13" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -4577,22 +4574,22 @@
         <v>24</v>
       </c>
       <c r="C76" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="D76" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="D76" s="6" t="s">
-        <v>258</v>
-      </c>
       <c r="E76" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="G76" s="12" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -4603,22 +4600,22 @@
         <v>2</v>
       </c>
       <c r="C77" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="D77" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="D77" s="6" t="s">
+      <c r="E77" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="E77" s="6" t="s">
+      <c r="F77" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="F77" s="11" t="s">
+      <c r="G77" s="12" t="s">
         <v>262</v>
       </c>
-      <c r="G77" s="12" t="s">
+      <c r="H77" s="13" t="s">
         <v>263</v>
-      </c>
-      <c r="H77" s="13" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -4629,22 +4626,22 @@
         <v>1</v>
       </c>
       <c r="C78" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="D78" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="D78" s="6" t="s">
+      <c r="E78" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="E78" s="6" t="s">
+      <c r="F78" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="F78" s="11" t="s">
+      <c r="G78" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="G78" s="12" t="s">
+      <c r="H78" s="13" t="s">
         <v>269</v>
-      </c>
-      <c r="H78" s="13" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -4655,22 +4652,22 @@
         <v>1</v>
       </c>
       <c r="C79" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D79" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="D79" s="6" t="s">
+      <c r="E79" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="E79" s="6" t="s">
+      <c r="F79" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="F79" s="11" t="s">
+      <c r="G79" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="G79" s="12" t="s">
+      <c r="H79" s="13" t="s">
         <v>275</v>
-      </c>
-      <c r="H79" s="13" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4681,22 +4678,22 @@
         <v>6</v>
       </c>
       <c r="C80" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D80" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="D80" s="6" t="s">
+      <c r="E80" s="6" t="s">
         <v>278</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>279</v>
       </c>
       <c r="F80" s="11" t="s">
         <v>68</v>
       </c>
       <c r="G80" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="H80" s="13" t="s">
         <v>280</v>
-      </c>
-      <c r="H80" s="13" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -4707,22 +4704,22 @@
         <v>2</v>
       </c>
       <c r="C81" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="D81" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="D81" s="6" t="s">
+      <c r="E81" s="6" t="s">
         <v>283</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>284</v>
       </c>
       <c r="F81" s="11" t="s">
         <v>68</v>
       </c>
       <c r="G81" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="H81" s="13" t="s">
         <v>285</v>
-      </c>
-      <c r="H81" s="13" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -4733,22 +4730,22 @@
         <v>24</v>
       </c>
       <c r="C82" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="D82" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="D82" s="6" t="s">
+      <c r="E82" s="6" t="s">
         <v>288</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>289</v>
       </c>
       <c r="F82" s="11" t="s">
         <v>68</v>
       </c>
       <c r="G82" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="H82" s="13" t="s">
         <v>290</v>
-      </c>
-      <c r="H82" s="13" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -4759,20 +4756,20 @@
         <v>24</v>
       </c>
       <c r="C83" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="D83" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="D83" s="6" t="s">
+      <c r="E83" s="6" t="s">
         <v>293</v>
-      </c>
-      <c r="E83" s="6" t="s">
-        <v>294</v>
       </c>
       <c r="F83" s="11"/>
       <c r="G83" s="12">
         <v>733660061</v>
       </c>
       <c r="H83" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -4783,22 +4780,22 @@
         <v>1</v>
       </c>
       <c r="C84" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="D84" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="D84" s="6" t="s">
+      <c r="E84" s="6" t="s">
         <v>297</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>298</v>
       </c>
       <c r="F84" s="11" t="s">
         <v>68</v>
       </c>
       <c r="G84" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="H84" s="13" t="s">
         <v>299</v>
-      </c>
-      <c r="H84" s="13" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -4809,22 +4806,22 @@
         <v>1</v>
       </c>
       <c r="C85" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="D85" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="D85" s="6" t="s">
+      <c r="E85" s="6" t="s">
         <v>302</v>
-      </c>
-      <c r="E85" s="6" t="s">
-        <v>303</v>
       </c>
       <c r="F85" s="11" t="s">
         <v>68</v>
       </c>
       <c r="G85" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="H85" s="13" t="s">
         <v>304</v>
-      </c>
-      <c r="H85" s="13" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -4835,22 +4832,22 @@
         <v>24</v>
       </c>
       <c r="C86" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="D86" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="D86" s="6" t="s">
+      <c r="E86" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="E86" s="6" t="s">
+      <c r="F86" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="F86" s="11" t="s">
+      <c r="G86" s="12" t="s">
         <v>309</v>
       </c>
-      <c r="G86" s="12" t="s">
+      <c r="H86" s="13" t="s">
         <v>310</v>
-      </c>
-      <c r="H86" s="13" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -4861,22 +4858,22 @@
         <v>24</v>
       </c>
       <c r="C87" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D87" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="D87" s="6" t="s">
+      <c r="E87" s="6" t="s">
         <v>313</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>314</v>
       </c>
       <c r="F87" s="11" t="s">
         <v>68</v>
       </c>
       <c r="G87" s="12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -4887,13 +4884,13 @@
         <v>1</v>
       </c>
       <c r="C88" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="D88" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="D88" s="6" t="s">
-        <v>317</v>
-      </c>
       <c r="E88" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F88" s="11" t="s">
         <v>12</v>
@@ -4902,7 +4899,7 @@
         <v>1050270001</v>
       </c>
       <c r="H88" s="13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -4913,19 +4910,19 @@
         <v>1</v>
       </c>
       <c r="C89" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="D89" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="D89" s="6" t="s">
+      <c r="E89" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="E89" s="6" t="s">
+      <c r="F89" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="F89" s="11" t="s">
+      <c r="G89" s="12" t="s">
         <v>322</v>
-      </c>
-      <c r="G89" s="12" t="s">
-        <v>323</v>
       </c>
       <c r="H89" s="13"/>
     </row>
@@ -4937,22 +4934,22 @@
         <v>74</v>
       </c>
       <c r="C90" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="D90" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="D90" s="6" t="s">
+      <c r="E90" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="E90" s="6" t="s">
+      <c r="F90" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="G90" s="12" t="s">
         <v>326</v>
       </c>
-      <c r="F90" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="G90" s="12" t="s">
+      <c r="H90" s="13" t="s">
         <v>327</v>
-      </c>
-      <c r="H90" s="13" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4963,22 +4960,22 @@
         <v>6</v>
       </c>
       <c r="C91" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="D91" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="D91" s="6" t="s">
+      <c r="E91" s="6" t="s">
         <v>330</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>331</v>
       </c>
       <c r="F91" s="11" t="s">
         <v>80</v>
       </c>
       <c r="G91" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -4989,22 +4986,22 @@
         <v>2</v>
       </c>
       <c r="C92" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="D92" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="D92" s="6" t="s">
+      <c r="E92" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="E92" s="6" t="s">
+      <c r="F92" s="11" t="s">
         <v>335</v>
       </c>
-      <c r="F92" s="11" t="s">
+      <c r="G92" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="H92" s="13" t="s">
         <v>336</v>
-      </c>
-      <c r="G92" s="12" t="s">
-        <v>334</v>
-      </c>
-      <c r="H92" s="13" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5015,22 +5012,22 @@
         <v>24</v>
       </c>
       <c r="C93" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="D93" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="D93" s="6" t="s">
+      <c r="E93" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="F93" s="11" t="s">
+        <v>335</v>
+      </c>
+      <c r="G93" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="H93" s="13" t="s">
         <v>339</v>
-      </c>
-      <c r="E93" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="F93" s="11" t="s">
-        <v>336</v>
-      </c>
-      <c r="G93" s="12" t="s">
-        <v>339</v>
-      </c>
-      <c r="H93" s="13" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -5041,22 +5038,22 @@
         <v>4</v>
       </c>
       <c r="C94" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="D94" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="D94" s="6" t="s">
+      <c r="E94" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="F94" s="11" t="s">
+        <v>335</v>
+      </c>
+      <c r="G94" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="H94" s="13" t="s">
         <v>342</v>
-      </c>
-      <c r="E94" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="F94" s="11" t="s">
-        <v>336</v>
-      </c>
-      <c r="G94" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="H94" s="13" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -5067,22 +5064,22 @@
         <v>1</v>
       </c>
       <c r="C95" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="D95" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="D95" s="6" t="s">
+      <c r="E95" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="E95" s="6" t="s">
+      <c r="F95" s="11" t="s">
         <v>346</v>
       </c>
-      <c r="F95" s="11" t="s">
+      <c r="G95" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="H95" s="13" t="s">
         <v>347</v>
-      </c>
-      <c r="G95" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="H95" s="13" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5093,22 +5090,22 @@
         <v>18</v>
       </c>
       <c r="C96" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="D96" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="D96" s="6" t="s">
+      <c r="E96" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="E96" s="6" t="s">
-        <v>351</v>
-      </c>
       <c r="F96" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G96" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H96" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -5119,22 +5116,22 @@
         <v>2</v>
       </c>
       <c r="C97" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="D97" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="D97" s="6" t="s">
+      <c r="E97" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="E97" s="6" t="s">
+      <c r="F97" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="G97" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="F97" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="G97" s="12" t="s">
+      <c r="H97" s="13" t="s">
         <v>355</v>
-      </c>
-      <c r="H97" s="13" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -5145,22 +5142,22 @@
         <v>1</v>
       </c>
       <c r="C98" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="D98" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="D98" s="6" t="s">
+      <c r="E98" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="E98" s="6" t="s">
+      <c r="F98" s="11" t="s">
         <v>359</v>
       </c>
-      <c r="F98" s="11" t="s">
+      <c r="G98" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="H98" s="13" t="s">
         <v>360</v>
-      </c>
-      <c r="G98" s="12" t="s">
-        <v>358</v>
-      </c>
-      <c r="H98" s="13" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -5171,19 +5168,19 @@
         <v>1</v>
       </c>
       <c r="C99" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="D99" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="D99" s="6" t="s">
+      <c r="E99" s="6" t="s">
         <v>363</v>
-      </c>
-      <c r="E99" s="6" t="s">
-        <v>364</v>
       </c>
       <c r="F99" s="11" t="s">
         <v>68</v>
       </c>
       <c r="G99" s="12" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H99" s="13"/>
     </row>
@@ -5195,22 +5192,22 @@
         <v>24</v>
       </c>
       <c r="C100" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="D100" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="D100" s="6" t="s">
+      <c r="E100" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="F100" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="E100" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="F100" s="11" t="s">
+      <c r="G100" s="12" t="s">
         <v>368</v>
       </c>
-      <c r="G100" s="12" t="s">
+      <c r="H100" s="13" t="s">
         <v>369</v>
-      </c>
-      <c r="H100" s="13" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -5221,22 +5218,22 @@
         <v>49</v>
       </c>
       <c r="C101" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="D101" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="D101" s="6" t="s">
+      <c r="E101" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="E101" s="6" t="s">
-        <v>373</v>
-      </c>
       <c r="F101" s="11" t="s">
+        <v>607</v>
+      </c>
+      <c r="G101" s="12" t="s">
         <v>608</v>
       </c>
-      <c r="G101" s="12" t="s">
+      <c r="H101" s="13" t="s">
         <v>609</v>
-      </c>
-      <c r="H101" s="13" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5247,22 +5244,22 @@
         <v>6</v>
       </c>
       <c r="C102" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="D102" s="6" t="s">
         <v>374</v>
       </c>
-      <c r="D102" s="6" t="s">
-        <v>375</v>
-      </c>
       <c r="E102" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F102" s="11" t="s">
         <v>181</v>
       </c>
       <c r="G102" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="H102" s="13" t="s">
         <v>376</v>
-      </c>
-      <c r="H102" s="13" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="345" x14ac:dyDescent="0.25">
@@ -5273,22 +5270,22 @@
         <v>73</v>
       </c>
       <c r="C103" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="D103" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="D103" s="6" t="s">
-        <v>379</v>
-      </c>
       <c r="E103" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F103" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="G103" s="12" t="s">
         <v>611</v>
       </c>
-      <c r="G103" s="12" t="s">
+      <c r="H103" s="13" t="s">
         <v>612</v>
-      </c>
-      <c r="H103" s="13" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5299,10 +5296,10 @@
         <v>6</v>
       </c>
       <c r="C104" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="D104" s="6" t="s">
         <v>614</v>
-      </c>
-      <c r="D104" s="6" t="s">
-        <v>615</v>
       </c>
       <c r="E104" s="6">
         <v>603</v>
@@ -5311,10 +5308,10 @@
         <v>18</v>
       </c>
       <c r="G104" s="12" t="s">
+        <v>615</v>
+      </c>
+      <c r="H104" s="13" t="s">
         <v>616</v>
-      </c>
-      <c r="H104" s="13" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -5325,22 +5322,22 @@
         <v>51</v>
       </c>
       <c r="C105" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="D105" s="6" t="s">
         <v>380</v>
       </c>
-      <c r="D105" s="6" t="s">
-        <v>381</v>
-      </c>
       <c r="E105" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F105" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G105" s="12" t="s">
+        <v>617</v>
+      </c>
+      <c r="H105" s="13" t="s">
         <v>618</v>
-      </c>
-      <c r="H105" s="13" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -5351,22 +5348,22 @@
         <v>247</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F106" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G106" s="12" t="s">
+        <v>619</v>
+      </c>
+      <c r="H106" s="13" t="s">
         <v>620</v>
-      </c>
-      <c r="H106" s="13" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="180" x14ac:dyDescent="0.25">
@@ -5377,22 +5374,22 @@
         <v>24</v>
       </c>
       <c r="C107" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="D107" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="D107" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="E107" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F107" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G107" s="12" t="s">
+        <v>660</v>
+      </c>
+      <c r="H107" s="13" t="s">
         <v>661</v>
-      </c>
-      <c r="H107" s="13" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5403,22 +5400,22 @@
         <v>3</v>
       </c>
       <c r="C108" s="5" t="s">
+        <v>622</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="E108" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="F108" s="11" t="s">
+        <v>607</v>
+      </c>
+      <c r="G108" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="D108" s="6" t="s">
-        <v>385</v>
-      </c>
-      <c r="E108" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="F108" s="11" t="s">
-        <v>608</v>
-      </c>
-      <c r="G108" s="12" t="s">
+      <c r="H108" s="13" t="s">
         <v>624</v>
-      </c>
-      <c r="H108" s="13" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -5429,22 +5426,22 @@
         <v>13</v>
       </c>
       <c r="C109" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="D109" s="6" t="s">
         <v>386</v>
-      </c>
-      <c r="D109" s="6" t="s">
-        <v>387</v>
       </c>
       <c r="E109" s="6">
         <v>603</v>
       </c>
       <c r="F109" s="11" t="s">
+        <v>625</v>
+      </c>
+      <c r="G109" s="12" t="s">
         <v>626</v>
       </c>
-      <c r="G109" s="12" t="s">
+      <c r="H109" s="13" t="s">
         <v>627</v>
-      </c>
-      <c r="H109" s="13" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -5455,22 +5452,22 @@
         <v>48</v>
       </c>
       <c r="C110" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="D110" s="6" t="s">
         <v>388</v>
       </c>
-      <c r="D110" s="6" t="s">
-        <v>389</v>
-      </c>
       <c r="E110" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F110" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G110" s="12" t="s">
+        <v>628</v>
+      </c>
+      <c r="H110" s="13" t="s">
         <v>629</v>
-      </c>
-      <c r="H110" s="13" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="330" x14ac:dyDescent="0.25">
@@ -5481,22 +5478,22 @@
         <v>48</v>
       </c>
       <c r="C111" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="D111" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="D111" s="6" t="s">
-        <v>391</v>
-      </c>
       <c r="E111" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F111" s="11" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G111" s="12" t="s">
+        <v>630</v>
+      </c>
+      <c r="H111" s="13" t="s">
         <v>631</v>
-      </c>
-      <c r="H111" s="13" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="180" x14ac:dyDescent="0.25">
@@ -5507,22 +5504,22 @@
         <v>25</v>
       </c>
       <c r="C112" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="D112" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="D112" s="6" t="s">
-        <v>393</v>
-      </c>
       <c r="E112" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F112" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G112" s="12" t="s">
+        <v>632</v>
+      </c>
+      <c r="H112" s="13" t="s">
         <v>633</v>
-      </c>
-      <c r="H112" s="13" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -5533,22 +5530,22 @@
         <v>1</v>
       </c>
       <c r="C113" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="D113" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="D113" s="6" t="s">
-        <v>397</v>
-      </c>
       <c r="E113" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F113" s="11" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G113" s="12" t="s">
+        <v>634</v>
+      </c>
+      <c r="H113" s="13" t="s">
         <v>635</v>
-      </c>
-      <c r="H113" s="13" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5559,22 +5556,22 @@
         <v>7</v>
       </c>
       <c r="C114" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="D114" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="D114" s="6" t="s">
-        <v>399</v>
-      </c>
       <c r="E114" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F114" s="11" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G114" s="12" t="s">
+        <v>636</v>
+      </c>
+      <c r="H114" s="13" t="s">
         <v>637</v>
-      </c>
-      <c r="H114" s="13" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -5585,22 +5582,22 @@
         <v>2</v>
       </c>
       <c r="C115" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="D115" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="D115" s="6" t="s">
-        <v>401</v>
-      </c>
       <c r="E115" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F115" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G115" s="12" t="s">
+        <v>638</v>
+      </c>
+      <c r="H115" s="13" t="s">
         <v>639</v>
-      </c>
-      <c r="H115" s="13" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -5611,22 +5608,22 @@
         <v>1</v>
       </c>
       <c r="C116" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="D116" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="D116" s="6" t="s">
-        <v>403</v>
-      </c>
       <c r="E116" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F116" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G116" s="12" t="s">
+        <v>640</v>
+      </c>
+      <c r="H116" s="13" t="s">
         <v>641</v>
-      </c>
-      <c r="H116" s="13" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -5637,22 +5634,22 @@
         <v>24</v>
       </c>
       <c r="C117" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="D117" s="6" t="s">
         <v>404</v>
-      </c>
-      <c r="D117" s="6" t="s">
-        <v>405</v>
       </c>
       <c r="E117" s="6">
         <v>603</v>
       </c>
       <c r="F117" s="11" t="s">
+        <v>642</v>
+      </c>
+      <c r="G117" s="12" t="s">
         <v>643</v>
       </c>
-      <c r="G117" s="12" t="s">
+      <c r="H117" s="13" t="s">
         <v>644</v>
-      </c>
-      <c r="H117" s="13" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="150" x14ac:dyDescent="0.25">
@@ -5663,22 +5660,22 @@
         <v>26</v>
       </c>
       <c r="C118" s="5" t="s">
+        <v>645</v>
+      </c>
+      <c r="D118" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="E118" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="F118" s="11" t="s">
+        <v>607</v>
+      </c>
+      <c r="G118" s="12" t="s">
         <v>646</v>
       </c>
-      <c r="D118" s="6" t="s">
-        <v>406</v>
-      </c>
-      <c r="E118" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="F118" s="11" t="s">
-        <v>608</v>
-      </c>
-      <c r="G118" s="12" t="s">
+      <c r="H118" s="13" t="s">
         <v>647</v>
-      </c>
-      <c r="H118" s="13" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -5689,22 +5686,22 @@
         <v>1</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F119" s="11" t="s">
+        <v>648</v>
+      </c>
+      <c r="G119" s="12" t="s">
         <v>649</v>
       </c>
-      <c r="G119" s="12" t="s">
+      <c r="H119" s="13" t="s">
         <v>650</v>
-      </c>
-      <c r="H119" s="13" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5715,22 +5712,22 @@
         <v>8</v>
       </c>
       <c r="C120" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="D120" s="6" t="s">
         <v>408</v>
       </c>
-      <c r="D120" s="6" t="s">
-        <v>409</v>
-      </c>
       <c r="E120" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F120" s="11" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G120" s="12" t="s">
+        <v>651</v>
+      </c>
+      <c r="H120" s="13" t="s">
         <v>652</v>
-      </c>
-      <c r="H120" s="13" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -5741,22 +5738,22 @@
         <v>2</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F121" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G121" s="12" t="s">
+        <v>653</v>
+      </c>
+      <c r="H121" s="13" t="s">
         <v>654</v>
-      </c>
-      <c r="H121" s="13" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -5767,22 +5764,22 @@
         <v>1</v>
       </c>
       <c r="C122" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="D122" s="6" t="s">
         <v>411</v>
       </c>
-      <c r="D122" s="6" t="s">
-        <v>412</v>
-      </c>
       <c r="E122" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F122" s="11" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G122" s="12" t="s">
+        <v>655</v>
+      </c>
+      <c r="H122" s="13" t="s">
         <v>656</v>
-      </c>
-      <c r="H122" s="13" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -5793,22 +5790,22 @@
         <v>24</v>
       </c>
       <c r="C123" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="E123" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="D123" s="6" t="s">
-        <v>412</v>
-      </c>
-      <c r="E123" s="6" t="s">
-        <v>395</v>
-      </c>
       <c r="F123" s="11" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G123" s="12" t="s">
+        <v>721</v>
+      </c>
+      <c r="H123" s="13" t="s">
         <v>722</v>
-      </c>
-      <c r="H123" s="13" t="s">
-        <v>723</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="375" x14ac:dyDescent="0.25">
@@ -5819,22 +5816,22 @@
         <v>102</v>
       </c>
       <c r="C124" s="5" t="s">
+        <v>657</v>
+      </c>
+      <c r="D124" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="E124" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="F124" s="11" t="s">
+        <v>607</v>
+      </c>
+      <c r="G124" s="12" t="s">
         <v>658</v>
       </c>
-      <c r="D124" s="6" t="s">
-        <v>413</v>
-      </c>
-      <c r="E124" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="F124" s="11" t="s">
-        <v>608</v>
-      </c>
-      <c r="G124" s="12" t="s">
+      <c r="H124" s="13" t="s">
         <v>659</v>
-      </c>
-      <c r="H124" s="13" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -5845,22 +5842,22 @@
         <v>1</v>
       </c>
       <c r="C125" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="D125" s="6" t="s">
         <v>414</v>
       </c>
-      <c r="D125" s="6" t="s">
-        <v>415</v>
-      </c>
       <c r="E125" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F125" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G125" s="12" t="s">
+        <v>663</v>
+      </c>
+      <c r="H125" s="13" t="s">
         <v>664</v>
-      </c>
-      <c r="H125" s="13" t="s">
-        <v>665</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -5871,22 +5868,22 @@
         <v>1</v>
       </c>
       <c r="C126" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="D126" s="6" t="s">
         <v>416</v>
-      </c>
-      <c r="D126" s="6" t="s">
-        <v>417</v>
       </c>
       <c r="E126" s="6">
         <v>603</v>
       </c>
       <c r="F126" s="11" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G126" s="12" t="s">
+        <v>665</v>
+      </c>
+      <c r="H126" s="13" t="s">
         <v>666</v>
-      </c>
-      <c r="H126" s="13" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="315" x14ac:dyDescent="0.25">
@@ -5897,22 +5894,22 @@
         <v>55</v>
       </c>
       <c r="C127" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="D127" s="6" t="s">
         <v>418</v>
       </c>
-      <c r="D127" s="6" t="s">
-        <v>419</v>
-      </c>
       <c r="E127" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F127" s="11" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G127" s="12" t="s">
+        <v>667</v>
+      </c>
+      <c r="H127" s="13" t="s">
         <v>668</v>
-      </c>
-      <c r="H127" s="13" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5923,22 +5920,22 @@
         <v>25</v>
       </c>
       <c r="C128" s="5" t="s">
+        <v>669</v>
+      </c>
+      <c r="D128" s="6" t="s">
         <v>670</v>
       </c>
-      <c r="D128" s="6" t="s">
+      <c r="E128" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="F128" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="G128" s="12" t="s">
         <v>671</v>
       </c>
-      <c r="E128" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="F128" s="11" t="s">
-        <v>611</v>
-      </c>
-      <c r="G128" s="12" t="s">
+      <c r="H128" s="13" t="s">
         <v>672</v>
-      </c>
-      <c r="H128" s="13" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -5949,22 +5946,22 @@
         <v>9</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F129" s="11" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G129" s="12" t="s">
+        <v>673</v>
+      </c>
+      <c r="H129" s="13" t="s">
         <v>674</v>
-      </c>
-      <c r="H129" s="13" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -5975,22 +5972,22 @@
         <v>1</v>
       </c>
       <c r="C130" s="5" t="s">
+        <v>600</v>
+      </c>
+      <c r="D130" s="6" t="s">
         <v>601</v>
       </c>
-      <c r="D130" s="6" t="s">
-        <v>602</v>
-      </c>
       <c r="E130" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F130" s="11" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G130" s="12" t="s">
+        <v>675</v>
+      </c>
+      <c r="H130" s="13" t="s">
         <v>676</v>
-      </c>
-      <c r="H130" s="13" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -6001,22 +5998,22 @@
         <v>2</v>
       </c>
       <c r="C131" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="D131" s="6" t="s">
         <v>421</v>
       </c>
-      <c r="D131" s="6" t="s">
-        <v>422</v>
-      </c>
       <c r="E131" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F131" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G131" s="12" t="s">
+        <v>719</v>
+      </c>
+      <c r="H131" s="13" t="s">
         <v>720</v>
-      </c>
-      <c r="H131" s="13" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -6027,22 +6024,22 @@
         <v>1</v>
       </c>
       <c r="C132" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="D132" s="6" t="s">
         <v>423</v>
       </c>
-      <c r="D132" s="6" t="s">
-        <v>424</v>
-      </c>
       <c r="E132" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F132" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G132" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="H132" s="13" t="s">
         <v>678</v>
-      </c>
-      <c r="H132" s="13" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -6053,22 +6050,22 @@
         <v>2</v>
       </c>
       <c r="C133" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="D133" s="6" t="s">
         <v>425</v>
       </c>
-      <c r="D133" s="6" t="s">
-        <v>426</v>
-      </c>
       <c r="E133" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F133" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G133" s="12" t="s">
+        <v>679</v>
+      </c>
+      <c r="H133" s="13" t="s">
         <v>680</v>
-      </c>
-      <c r="H133" s="13" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -6079,22 +6076,22 @@
         <v>1</v>
       </c>
       <c r="C134" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="D134" s="6" t="s">
         <v>427</v>
       </c>
-      <c r="D134" s="6" t="s">
-        <v>428</v>
-      </c>
       <c r="E134" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F134" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G134" s="12" t="s">
+        <v>681</v>
+      </c>
+      <c r="H134" s="13" t="s">
         <v>682</v>
-      </c>
-      <c r="H134" s="13" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -6105,19 +6102,19 @@
         <v>89</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E135" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F135" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G135" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H135" s="13"/>
     </row>
@@ -6129,22 +6126,22 @@
         <v>48</v>
       </c>
       <c r="C136" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="D136" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="D136" s="6" t="s">
+      <c r="E136" s="6" t="s">
         <v>431</v>
       </c>
-      <c r="E136" s="6" t="s">
+      <c r="F136" s="11" t="s">
         <v>432</v>
       </c>
-      <c r="F136" s="11" t="s">
+      <c r="G136" s="12" t="s">
         <v>433</v>
       </c>
-      <c r="G136" s="12" t="s">
+      <c r="H136" s="13" t="s">
         <v>434</v>
-      </c>
-      <c r="H136" s="13" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -6155,22 +6152,22 @@
         <v>66</v>
       </c>
       <c r="C137" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="D137" s="6" t="s">
         <v>436</v>
       </c>
-      <c r="D137" s="6" t="s">
+      <c r="E137" s="6" t="s">
         <v>437</v>
       </c>
-      <c r="E137" s="6" t="s">
+      <c r="F137" s="11" t="s">
         <v>438</v>
       </c>
-      <c r="F137" s="11" t="s">
+      <c r="G137" s="12" t="s">
         <v>439</v>
       </c>
-      <c r="G137" s="12" t="s">
+      <c r="H137" s="13" t="s">
         <v>440</v>
-      </c>
-      <c r="H137" s="13" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -6181,22 +6178,22 @@
         <v>1</v>
       </c>
       <c r="C138" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="D138" s="6" t="s">
         <v>442</v>
       </c>
-      <c r="D138" s="6" t="s">
+      <c r="E138" s="6" t="s">
         <v>443</v>
       </c>
-      <c r="E138" s="6" t="s">
+      <c r="F138" s="11" t="s">
         <v>444</v>
       </c>
-      <c r="F138" s="11" t="s">
+      <c r="G138" s="12" t="s">
         <v>445</v>
       </c>
-      <c r="G138" s="12" t="s">
+      <c r="H138" s="13" t="s">
         <v>446</v>
-      </c>
-      <c r="H138" s="13" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -6207,22 +6204,22 @@
         <v>6</v>
       </c>
       <c r="C139" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="D139" s="6" t="s">
         <v>448</v>
       </c>
-      <c r="D139" s="6" t="s">
+      <c r="E139" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="E139" s="6" t="s">
+      <c r="F139" s="11" t="s">
         <v>450</v>
       </c>
-      <c r="F139" s="11" t="s">
+      <c r="G139" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="H139" s="13" t="s">
         <v>451</v>
-      </c>
-      <c r="G139" s="12" t="s">
-        <v>449</v>
-      </c>
-      <c r="H139" s="13" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -6233,22 +6230,22 @@
         <v>1</v>
       </c>
       <c r="C140" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="D140" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="D140" s="6" t="s">
+      <c r="E140" s="6" t="s">
         <v>454</v>
       </c>
-      <c r="E140" s="6" t="s">
+      <c r="F140" s="11" t="s">
         <v>455</v>
       </c>
-      <c r="F140" s="11" t="s">
+      <c r="G140" s="12" t="s">
         <v>456</v>
       </c>
-      <c r="G140" s="12" t="s">
+      <c r="H140" s="13" t="s">
         <v>457</v>
-      </c>
-      <c r="H140" s="13" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -6259,19 +6256,19 @@
         <v>2</v>
       </c>
       <c r="C141" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="D141" s="6" t="s">
         <v>459</v>
       </c>
-      <c r="D141" s="6" t="s">
+      <c r="E141" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="F141" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="E141" s="6" t="s">
-        <v>432</v>
-      </c>
-      <c r="F141" s="11" t="s">
+      <c r="G141" s="12" t="s">
         <v>461</v>
-      </c>
-      <c r="G141" s="12" t="s">
-        <v>462</v>
       </c>
       <c r="H141" s="13"/>
     </row>
@@ -6283,22 +6280,22 @@
         <v>30</v>
       </c>
       <c r="C142" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="D142" s="6" t="s">
         <v>463</v>
       </c>
-      <c r="D142" s="6" t="s">
+      <c r="E142" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="E142" s="6" t="s">
+      <c r="F142" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="F142" s="11" t="s">
+      <c r="G142" s="12" t="s">
+        <v>463</v>
+      </c>
+      <c r="H142" s="13" t="s">
         <v>466</v>
-      </c>
-      <c r="G142" s="12" t="s">
-        <v>464</v>
-      </c>
-      <c r="H142" s="13" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="143" spans="1:8" ht="165" x14ac:dyDescent="0.25">
@@ -6309,22 +6306,22 @@
         <v>24</v>
       </c>
       <c r="C143" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="D143" s="6" t="s">
         <v>468</v>
       </c>
-      <c r="D143" s="6" t="s">
+      <c r="E143" s="6" t="s">
         <v>469</v>
       </c>
-      <c r="E143" s="6" t="s">
+      <c r="F143" s="11" t="s">
+        <v>465</v>
+      </c>
+      <c r="G143" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="F143" s="11" t="s">
-        <v>466</v>
-      </c>
-      <c r="G143" s="12" t="s">
+      <c r="H143" s="13" t="s">
         <v>471</v>
-      </c>
-      <c r="H143" s="13" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="144" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -6335,22 +6332,22 @@
         <v>23</v>
       </c>
       <c r="C144" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="D144" s="6" t="s">
         <v>473</v>
       </c>
-      <c r="D144" s="6" t="s">
+      <c r="E144" s="6" t="s">
         <v>474</v>
       </c>
-      <c r="E144" s="6" t="s">
+      <c r="F144" s="11" t="s">
         <v>475</v>
       </c>
-      <c r="F144" s="11" t="s">
+      <c r="G144" s="12" t="s">
         <v>476</v>
       </c>
-      <c r="G144" s="12" t="s">
+      <c r="H144" s="13" t="s">
         <v>477</v>
-      </c>
-      <c r="H144" s="13" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="145" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -6361,22 +6358,22 @@
         <v>7</v>
       </c>
       <c r="C145" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="D145" s="6" t="s">
         <v>479</v>
       </c>
-      <c r="D145" s="6" t="s">
+      <c r="E145" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="F145" s="11" t="s">
+        <v>438</v>
+      </c>
+      <c r="G145" s="12" t="s">
         <v>480</v>
       </c>
-      <c r="E145" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="F145" s="11" t="s">
-        <v>439</v>
-      </c>
-      <c r="G145" s="12" t="s">
+      <c r="H145" s="13" t="s">
         <v>481</v>
-      </c>
-      <c r="H145" s="13" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
@@ -6387,22 +6384,22 @@
         <v>1</v>
       </c>
       <c r="C146" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="D146" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="D146" s="6" t="s">
+      <c r="E146" s="6" t="s">
         <v>484</v>
       </c>
-      <c r="E146" s="6" t="s">
+      <c r="F146" s="11" t="s">
         <v>485</v>
       </c>
-      <c r="F146" s="11" t="s">
+      <c r="G146" s="12" t="s">
         <v>486</v>
       </c>
-      <c r="G146" s="12" t="s">
+      <c r="H146" s="13" t="s">
         <v>487</v>
-      </c>
-      <c r="H146" s="13" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -6413,22 +6410,22 @@
         <v>2</v>
       </c>
       <c r="C147" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="D147" s="6" t="s">
         <v>489</v>
       </c>
-      <c r="D147" s="6" t="s">
+      <c r="E147" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="F147" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="G147" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="H147" s="13" t="s">
         <v>490</v>
-      </c>
-      <c r="E147" s="6" t="s">
-        <v>490</v>
-      </c>
-      <c r="F147" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="G147" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="H147" s="13" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -6439,22 +6436,22 @@
         <v>24</v>
       </c>
       <c r="C148" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="D148" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="D148" s="6" t="s">
+      <c r="E148" s="6" t="s">
         <v>493</v>
       </c>
-      <c r="E148" s="6" t="s">
+      <c r="F148" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="G148" s="12" t="s">
+        <v>695</v>
+      </c>
+      <c r="H148" s="13" t="s">
         <v>494</v>
-      </c>
-      <c r="F148" s="11" t="s">
-        <v>451</v>
-      </c>
-      <c r="G148" s="12" t="s">
-        <v>696</v>
-      </c>
-      <c r="H148" s="13" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -6465,22 +6462,22 @@
         <v>1</v>
       </c>
       <c r="C149" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="D149" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="D149" s="6" t="s">
+      <c r="E149" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="F149" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="G149" s="12" t="s">
+        <v>496</v>
+      </c>
+      <c r="H149" s="13" t="s">
         <v>497</v>
-      </c>
-      <c r="E149" s="6" t="s">
-        <v>494</v>
-      </c>
-      <c r="F149" s="11" t="s">
-        <v>451</v>
-      </c>
-      <c r="G149" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="H149" s="13" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="150" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -6491,22 +6488,22 @@
         <v>24</v>
       </c>
       <c r="C150" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="D150" s="6" t="s">
         <v>499</v>
       </c>
-      <c r="D150" s="6" t="s">
-        <v>500</v>
-      </c>
       <c r="E150" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F150" s="11" t="s">
         <v>110</v>
       </c>
       <c r="G150" s="12" t="s">
+        <v>500</v>
+      </c>
+      <c r="H150" s="13" t="s">
         <v>501</v>
-      </c>
-      <c r="H150" s="13" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="151" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -6517,22 +6514,22 @@
         <v>125</v>
       </c>
       <c r="C151" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="D151" s="6" t="s">
         <v>503</v>
       </c>
-      <c r="D151" s="6" t="s">
+      <c r="E151" s="6" t="s">
         <v>504</v>
       </c>
-      <c r="E151" s="6" t="s">
-        <v>505</v>
-      </c>
       <c r="F151" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G151" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H151" s="13" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -6543,22 +6540,22 @@
         <v>1</v>
       </c>
       <c r="C152" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="D152" s="6" t="s">
         <v>506</v>
       </c>
-      <c r="D152" s="6" t="s">
+      <c r="E152" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="E152" s="6" t="s">
-        <v>508</v>
       </c>
       <c r="F152" s="11" t="s">
         <v>187</v>
       </c>
       <c r="G152" s="12" t="s">
+        <v>507</v>
+      </c>
+      <c r="H152" s="13" t="s">
         <v>508</v>
-      </c>
-      <c r="H152" s="13" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -6569,230 +6566,230 @@
         <v>1</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D153" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="E153" s="6" t="s">
         <v>510</v>
-      </c>
-      <c r="E153" s="6" t="s">
-        <v>511</v>
       </c>
       <c r="F153" s="11" t="s">
         <v>187</v>
       </c>
       <c r="G153" s="12" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H153" s="13" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B154" s="1">
         <v>1</v>
       </c>
       <c r="C154" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="D154" s="6" t="s">
         <v>513</v>
       </c>
-      <c r="D154" s="6" t="s">
+      <c r="E154" s="6" t="s">
         <v>514</v>
-      </c>
-      <c r="E154" s="6" t="s">
-        <v>515</v>
       </c>
       <c r="F154" s="11" t="s">
         <v>187</v>
       </c>
       <c r="G154" s="12" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H154" s="13" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B155" s="1">
         <v>1</v>
       </c>
       <c r="C155" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="D155" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="E155" s="6" t="s">
         <v>517</v>
-      </c>
-      <c r="D155" s="6" t="s">
-        <v>514</v>
-      </c>
-      <c r="E155" s="6" t="s">
-        <v>518</v>
       </c>
       <c r="F155" s="11" t="s">
         <v>187</v>
       </c>
       <c r="G155" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="H155" s="13" t="s">
         <v>519</v>
-      </c>
-      <c r="H155" s="13" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B156" s="1">
         <v>1</v>
       </c>
       <c r="C156" s="5" t="s">
+        <v>520</v>
+      </c>
+      <c r="D156" s="6" t="s">
         <v>521</v>
       </c>
-      <c r="D156" s="6" t="s">
+      <c r="E156" s="6" t="s">
         <v>522</v>
-      </c>
-      <c r="E156" s="6" t="s">
-        <v>523</v>
       </c>
       <c r="F156" s="11" t="s">
         <v>187</v>
       </c>
       <c r="G156" s="12" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="H156" s="13" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B157" s="1">
         <v>1</v>
       </c>
       <c r="C157" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="D157" s="6" t="s">
+        <v>698</v>
+      </c>
+      <c r="E157" s="6" t="s">
         <v>525</v>
-      </c>
-      <c r="D157" s="6" t="s">
-        <v>699</v>
-      </c>
-      <c r="E157" s="6" t="s">
-        <v>526</v>
       </c>
       <c r="F157" s="11" t="s">
         <v>187</v>
       </c>
       <c r="G157" s="12" t="s">
+        <v>698</v>
+      </c>
+      <c r="H157" s="13" t="s">
         <v>699</v>
-      </c>
-      <c r="H157" s="13" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B158" s="1">
         <v>1</v>
       </c>
       <c r="C158" s="5" t="s">
+        <v>526</v>
+      </c>
+      <c r="D158" s="6" t="s">
         <v>527</v>
       </c>
-      <c r="D158" s="6" t="s">
+      <c r="E158" s="6" t="s">
         <v>528</v>
       </c>
-      <c r="E158" s="6" t="s">
+      <c r="F158" s="11" t="s">
         <v>529</v>
       </c>
-      <c r="F158" s="11" t="s">
+      <c r="G158" s="12" t="s">
         <v>530</v>
       </c>
-      <c r="G158" s="12" t="s">
+      <c r="H158" s="13" t="s">
         <v>531</v>
-      </c>
-      <c r="H158" s="13" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B159" s="1">
         <v>1</v>
       </c>
       <c r="C159" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="D159" s="6" t="s">
         <v>533</v>
       </c>
-      <c r="D159" s="6" t="s">
+      <c r="E159" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="E159" s="6" t="s">
+      <c r="F159" s="11" t="s">
         <v>535</v>
       </c>
-      <c r="F159" s="11" t="s">
+      <c r="G159" s="12" t="s">
         <v>536</v>
       </c>
-      <c r="G159" s="12" t="s">
+      <c r="H159" s="13" t="s">
         <v>537</v>
-      </c>
-      <c r="H159" s="13" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B160" s="1">
         <v>1</v>
       </c>
       <c r="C160" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="D160" s="6" t="s">
         <v>539</v>
       </c>
-      <c r="D160" s="6" t="s">
+      <c r="E160" s="6" t="s">
         <v>540</v>
       </c>
-      <c r="E160" s="6" t="s">
-        <v>541</v>
-      </c>
       <c r="F160" s="11" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G160" s="12" t="s">
+        <v>704</v>
+      </c>
+      <c r="H160" s="13" t="s">
         <v>705</v>
-      </c>
-      <c r="H160" s="13" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="161" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B161" s="1">
         <v>7</v>
       </c>
       <c r="C161" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="D161" s="6" t="s">
         <v>542</v>
       </c>
-      <c r="D161" s="6" t="s">
+      <c r="E161" s="6" t="s">
         <v>543</v>
-      </c>
-      <c r="E161" s="6" t="s">
-        <v>544</v>
       </c>
       <c r="F161" s="14" t="s">
         <v>187</v>
       </c>
       <c r="G161" s="15" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="H161" s="16" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
   </sheetData>
@@ -6817,31 +6814,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>683</v>
+      </c>
+      <c r="B1" t="s">
         <v>684</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>685</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>686</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>687</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>688</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>689</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>690</v>
       </c>
-      <c r="H1" t="s">
-        <v>691</v>
-      </c>
       <c r="I1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix line item 38
</commit_message>
<xml_diff>
--- a/radiant_bom.xlsx
+++ b/radiant_bom.xlsx
@@ -1752,9 +1752,6 @@
     <t>MLCC - SMD/SMT 0402 50VDC 27pF 1% AEC-Q200</t>
   </si>
   <si>
-    <t>C0402C360F5GACTU</t>
-  </si>
-  <si>
     <t>CAP CER MLCC - SMD/SMT 50V 36pF C0G 0402 1%</t>
   </si>
   <si>
@@ -2200,6 +2197,9 @@
   </si>
   <si>
     <t>CAP CER 0.047UF 10V X7R 0402</t>
+  </si>
+  <si>
+    <t>CBR04C360F5GAC</t>
   </si>
 </sst>
 </file>
@@ -2648,8 +2648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2666,16 +2666,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" s="18" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E2" s="18"/>
       <c r="F2" s="19" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
@@ -2691,7 +2691,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>3</v>
@@ -3688,10 +3688,10 @@
         <v>92</v>
       </c>
       <c r="G41" s="12" t="s">
+        <v>724</v>
+      </c>
+      <c r="H41" s="13" t="s">
         <v>575</v>
-      </c>
-      <c r="H41" s="13" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3714,10 +3714,10 @@
         <v>221</v>
       </c>
       <c r="G42" s="12" t="s">
+        <v>576</v>
+      </c>
+      <c r="H42" s="13" t="s">
         <v>577</v>
-      </c>
-      <c r="H42" s="13" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -3740,10 +3740,10 @@
         <v>92</v>
       </c>
       <c r="G43" s="12" t="s">
+        <v>578</v>
+      </c>
+      <c r="H43" s="13" t="s">
         <v>579</v>
-      </c>
-      <c r="H43" s="13" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="195" x14ac:dyDescent="0.25">
@@ -3766,10 +3766,10 @@
         <v>119</v>
       </c>
       <c r="G44" s="12" t="s">
+        <v>602</v>
+      </c>
+      <c r="H44" s="13" t="s">
         <v>603</v>
-      </c>
-      <c r="H44" s="13" t="s">
-        <v>604</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3783,7 +3783,7 @@
         <v>164</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>115</v>
@@ -3792,10 +3792,10 @@
         <v>86</v>
       </c>
       <c r="G45" s="12" t="s">
+        <v>581</v>
+      </c>
+      <c r="H45" s="13" t="s">
         <v>582</v>
-      </c>
-      <c r="H45" s="13" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3818,10 +3818,10 @@
         <v>110</v>
       </c>
       <c r="G46" s="12" t="s">
+        <v>604</v>
+      </c>
+      <c r="H46" s="13" t="s">
         <v>605</v>
-      </c>
-      <c r="H46" s="13" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3841,13 +3841,13 @@
         <v>91</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G47" s="12" t="s">
+        <v>722</v>
+      </c>
+      <c r="H47" s="13" t="s">
         <v>723</v>
-      </c>
-      <c r="H47" s="13" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3870,10 +3870,10 @@
         <v>221</v>
       </c>
       <c r="G48" s="12" t="s">
+        <v>583</v>
+      </c>
+      <c r="H48" s="13" t="s">
         <v>584</v>
-      </c>
-      <c r="H48" s="13" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3896,10 +3896,10 @@
         <v>221</v>
       </c>
       <c r="G49" s="12" t="s">
+        <v>585</v>
+      </c>
+      <c r="H49" s="13" t="s">
         <v>586</v>
-      </c>
-      <c r="H49" s="13" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -3922,10 +3922,10 @@
         <v>119</v>
       </c>
       <c r="G50" s="12" t="s">
+        <v>587</v>
+      </c>
+      <c r="H50" s="13" t="s">
         <v>588</v>
-      </c>
-      <c r="H50" s="13" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -3948,10 +3948,10 @@
         <v>110</v>
       </c>
       <c r="G51" s="12" t="s">
+        <v>589</v>
+      </c>
+      <c r="H51" s="13" t="s">
         <v>590</v>
-      </c>
-      <c r="H51" s="13" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -3974,10 +3974,10 @@
         <v>92</v>
       </c>
       <c r="G52" s="12" t="s">
+        <v>591</v>
+      </c>
+      <c r="H52" s="13" t="s">
         <v>592</v>
-      </c>
-      <c r="H52" s="13" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -4000,10 +4000,10 @@
         <v>221</v>
       </c>
       <c r="G53" s="12" t="s">
+        <v>593</v>
+      </c>
+      <c r="H53" s="13" t="s">
         <v>594</v>
-      </c>
-      <c r="H53" s="13" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -4026,10 +4026,10 @@
         <v>92</v>
       </c>
       <c r="G54" s="12" t="s">
+        <v>595</v>
+      </c>
+      <c r="H54" s="13" t="s">
         <v>596</v>
-      </c>
-      <c r="H54" s="13" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -4173,19 +4173,19 @@
         <v>199</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="F60" s="11" t="s">
         <v>110</v>
       </c>
       <c r="G60" s="12" t="s">
+        <v>701</v>
+      </c>
+      <c r="H60" s="13" t="s">
         <v>702</v>
-      </c>
-      <c r="H60" s="13" t="s">
-        <v>703</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4320,7 +4320,7 @@
         <v>2</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>224</v>
@@ -4560,10 +4560,10 @@
         <v>12</v>
       </c>
       <c r="G75" s="12" t="s">
+        <v>695</v>
+      </c>
+      <c r="H75" s="13" t="s">
         <v>696</v>
-      </c>
-      <c r="H75" s="13" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -4583,13 +4583,13 @@
         <v>257</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="G76" s="12" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -5227,13 +5227,13 @@
         <v>372</v>
       </c>
       <c r="F101" s="11" t="s">
+        <v>606</v>
+      </c>
+      <c r="G101" s="12" t="s">
         <v>607</v>
       </c>
-      <c r="G101" s="12" t="s">
+      <c r="H101" s="13" t="s">
         <v>608</v>
-      </c>
-      <c r="H101" s="13" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5279,13 +5279,13 @@
         <v>372</v>
       </c>
       <c r="F103" s="11" t="s">
+        <v>609</v>
+      </c>
+      <c r="G103" s="12" t="s">
         <v>610</v>
       </c>
-      <c r="G103" s="12" t="s">
+      <c r="H103" s="13" t="s">
         <v>611</v>
-      </c>
-      <c r="H103" s="13" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5296,10 +5296,10 @@
         <v>6</v>
       </c>
       <c r="C104" s="5" t="s">
+        <v>612</v>
+      </c>
+      <c r="D104" s="6" t="s">
         <v>613</v>
-      </c>
-      <c r="D104" s="6" t="s">
-        <v>614</v>
       </c>
       <c r="E104" s="6">
         <v>603</v>
@@ -5308,10 +5308,10 @@
         <v>18</v>
       </c>
       <c r="G104" s="12" t="s">
+        <v>614</v>
+      </c>
+      <c r="H104" s="13" t="s">
         <v>615</v>
-      </c>
-      <c r="H104" s="13" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -5331,13 +5331,13 @@
         <v>372</v>
       </c>
       <c r="F105" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G105" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="H105" s="13" t="s">
         <v>617</v>
-      </c>
-      <c r="H105" s="13" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -5348,7 +5348,7 @@
         <v>247</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>381</v>
@@ -5357,13 +5357,13 @@
         <v>372</v>
       </c>
       <c r="F106" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G106" s="12" t="s">
+        <v>618</v>
+      </c>
+      <c r="H106" s="13" t="s">
         <v>619</v>
-      </c>
-      <c r="H106" s="13" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="180" x14ac:dyDescent="0.25">
@@ -5383,13 +5383,13 @@
         <v>372</v>
       </c>
       <c r="F107" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G107" s="12" t="s">
+        <v>659</v>
+      </c>
+      <c r="H107" s="13" t="s">
         <v>660</v>
-      </c>
-      <c r="H107" s="13" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5400,7 +5400,7 @@
         <v>3</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>384</v>
@@ -5409,13 +5409,13 @@
         <v>372</v>
       </c>
       <c r="F108" s="11" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G108" s="12" t="s">
+        <v>622</v>
+      </c>
+      <c r="H108" s="13" t="s">
         <v>623</v>
-      </c>
-      <c r="H108" s="13" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -5435,13 +5435,13 @@
         <v>603</v>
       </c>
       <c r="F109" s="11" t="s">
+        <v>624</v>
+      </c>
+      <c r="G109" s="12" t="s">
         <v>625</v>
       </c>
-      <c r="G109" s="12" t="s">
+      <c r="H109" s="13" t="s">
         <v>626</v>
-      </c>
-      <c r="H109" s="13" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="360" x14ac:dyDescent="0.25">
@@ -5461,13 +5461,13 @@
         <v>372</v>
       </c>
       <c r="F110" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G110" s="12" t="s">
+        <v>627</v>
+      </c>
+      <c r="H110" s="13" t="s">
         <v>628</v>
-      </c>
-      <c r="H110" s="13" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="330" x14ac:dyDescent="0.25">
@@ -5487,13 +5487,13 @@
         <v>372</v>
       </c>
       <c r="F111" s="11" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G111" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="H111" s="13" t="s">
         <v>630</v>
-      </c>
-      <c r="H111" s="13" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="180" x14ac:dyDescent="0.25">
@@ -5513,13 +5513,13 @@
         <v>372</v>
       </c>
       <c r="F112" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G112" s="12" t="s">
+        <v>631</v>
+      </c>
+      <c r="H112" s="13" t="s">
         <v>632</v>
-      </c>
-      <c r="H112" s="13" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -5539,13 +5539,13 @@
         <v>372</v>
       </c>
       <c r="F113" s="11" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G113" s="12" t="s">
+        <v>633</v>
+      </c>
+      <c r="H113" s="13" t="s">
         <v>634</v>
-      </c>
-      <c r="H113" s="13" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5565,13 +5565,13 @@
         <v>372</v>
       </c>
       <c r="F114" s="11" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G114" s="12" t="s">
+        <v>635</v>
+      </c>
+      <c r="H114" s="13" t="s">
         <v>636</v>
-      </c>
-      <c r="H114" s="13" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -5591,13 +5591,13 @@
         <v>372</v>
       </c>
       <c r="F115" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G115" s="12" t="s">
+        <v>637</v>
+      </c>
+      <c r="H115" s="13" t="s">
         <v>638</v>
-      </c>
-      <c r="H115" s="13" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -5617,13 +5617,13 @@
         <v>372</v>
       </c>
       <c r="F116" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G116" s="12" t="s">
+        <v>639</v>
+      </c>
+      <c r="H116" s="13" t="s">
         <v>640</v>
-      </c>
-      <c r="H116" s="13" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -5643,13 +5643,13 @@
         <v>603</v>
       </c>
       <c r="F117" s="11" t="s">
+        <v>641</v>
+      </c>
+      <c r="G117" s="12" t="s">
         <v>642</v>
       </c>
-      <c r="G117" s="12" t="s">
+      <c r="H117" s="13" t="s">
         <v>643</v>
-      </c>
-      <c r="H117" s="13" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="150" x14ac:dyDescent="0.25">
@@ -5660,7 +5660,7 @@
         <v>26</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>405</v>
@@ -5669,13 +5669,13 @@
         <v>372</v>
       </c>
       <c r="F118" s="11" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G118" s="12" t="s">
+        <v>645</v>
+      </c>
+      <c r="H118" s="13" t="s">
         <v>646</v>
-      </c>
-      <c r="H118" s="13" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -5686,7 +5686,7 @@
         <v>1</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>406</v>
@@ -5695,13 +5695,13 @@
         <v>372</v>
       </c>
       <c r="F119" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="G119" s="12" t="s">
         <v>648</v>
       </c>
-      <c r="G119" s="12" t="s">
+      <c r="H119" s="13" t="s">
         <v>649</v>
-      </c>
-      <c r="H119" s="13" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5721,13 +5721,13 @@
         <v>372</v>
       </c>
       <c r="F120" s="11" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G120" s="12" t="s">
+        <v>650</v>
+      </c>
+      <c r="H120" s="13" t="s">
         <v>651</v>
-      </c>
-      <c r="H120" s="13" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -5738,7 +5738,7 @@
         <v>2</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D121" s="6" t="s">
         <v>409</v>
@@ -5747,13 +5747,13 @@
         <v>372</v>
       </c>
       <c r="F121" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G121" s="12" t="s">
+        <v>652</v>
+      </c>
+      <c r="H121" s="13" t="s">
         <v>653</v>
-      </c>
-      <c r="H121" s="13" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -5773,13 +5773,13 @@
         <v>372</v>
       </c>
       <c r="F122" s="11" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G122" s="12" t="s">
+        <v>654</v>
+      </c>
+      <c r="H122" s="13" t="s">
         <v>655</v>
-      </c>
-      <c r="H122" s="13" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -5799,13 +5799,13 @@
         <v>394</v>
       </c>
       <c r="F123" s="11" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G123" s="12" t="s">
+        <v>720</v>
+      </c>
+      <c r="H123" s="13" t="s">
         <v>721</v>
-      </c>
-      <c r="H123" s="13" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="375" x14ac:dyDescent="0.25">
@@ -5816,7 +5816,7 @@
         <v>102</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>412</v>
@@ -5825,13 +5825,13 @@
         <v>372</v>
       </c>
       <c r="F124" s="11" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G124" s="12" t="s">
+        <v>657</v>
+      </c>
+      <c r="H124" s="13" t="s">
         <v>658</v>
-      </c>
-      <c r="H124" s="13" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -5851,13 +5851,13 @@
         <v>372</v>
       </c>
       <c r="F125" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G125" s="12" t="s">
+        <v>662</v>
+      </c>
+      <c r="H125" s="13" t="s">
         <v>663</v>
-      </c>
-      <c r="H125" s="13" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -5877,13 +5877,13 @@
         <v>603</v>
       </c>
       <c r="F126" s="11" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="G126" s="12" t="s">
+        <v>664</v>
+      </c>
+      <c r="H126" s="13" t="s">
         <v>665</v>
-      </c>
-      <c r="H126" s="13" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="315" x14ac:dyDescent="0.25">
@@ -5903,13 +5903,13 @@
         <v>372</v>
       </c>
       <c r="F127" s="11" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G127" s="12" t="s">
+        <v>666</v>
+      </c>
+      <c r="H127" s="13" t="s">
         <v>667</v>
-      </c>
-      <c r="H127" s="13" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5920,22 +5920,22 @@
         <v>25</v>
       </c>
       <c r="C128" s="5" t="s">
+        <v>668</v>
+      </c>
+      <c r="D128" s="6" t="s">
         <v>669</v>
-      </c>
-      <c r="D128" s="6" t="s">
-        <v>670</v>
       </c>
       <c r="E128" s="6" t="s">
         <v>394</v>
       </c>
       <c r="F128" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G128" s="12" t="s">
+        <v>670</v>
+      </c>
+      <c r="H128" s="13" t="s">
         <v>671</v>
-      </c>
-      <c r="H128" s="13" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -5946,7 +5946,7 @@
         <v>9</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D129" s="6" t="s">
         <v>419</v>
@@ -5955,13 +5955,13 @@
         <v>372</v>
       </c>
       <c r="F129" s="11" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G129" s="12" t="s">
+        <v>672</v>
+      </c>
+      <c r="H129" s="13" t="s">
         <v>673</v>
-      </c>
-      <c r="H129" s="13" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -5972,22 +5972,22 @@
         <v>1</v>
       </c>
       <c r="C130" s="5" t="s">
+        <v>599</v>
+      </c>
+      <c r="D130" s="6" t="s">
         <v>600</v>
-      </c>
-      <c r="D130" s="6" t="s">
-        <v>601</v>
       </c>
       <c r="E130" s="6" t="s">
         <v>372</v>
       </c>
       <c r="F130" s="11" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G130" s="12" t="s">
+        <v>674</v>
+      </c>
+      <c r="H130" s="13" t="s">
         <v>675</v>
-      </c>
-      <c r="H130" s="13" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -6007,13 +6007,13 @@
         <v>372</v>
       </c>
       <c r="F131" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G131" s="12" t="s">
+        <v>718</v>
+      </c>
+      <c r="H131" s="13" t="s">
         <v>719</v>
-      </c>
-      <c r="H131" s="13" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -6033,13 +6033,13 @@
         <v>372</v>
       </c>
       <c r="F132" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G132" s="12" t="s">
+        <v>676</v>
+      </c>
+      <c r="H132" s="13" t="s">
         <v>677</v>
-      </c>
-      <c r="H132" s="13" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -6059,13 +6059,13 @@
         <v>372</v>
       </c>
       <c r="F133" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G133" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="H133" s="13" t="s">
         <v>679</v>
-      </c>
-      <c r="H133" s="13" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -6085,13 +6085,13 @@
         <v>372</v>
       </c>
       <c r="F134" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G134" s="12" t="s">
+        <v>680</v>
+      </c>
+      <c r="H134" s="13" t="s">
         <v>681</v>
-      </c>
-      <c r="H134" s="13" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -6102,7 +6102,7 @@
         <v>89</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D135" s="6" t="s">
         <v>428</v>
@@ -6448,7 +6448,7 @@
         <v>450</v>
       </c>
       <c r="G148" s="12" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="H148" s="13" t="s">
         <v>494</v>
@@ -6529,7 +6529,7 @@
         <v>198</v>
       </c>
       <c r="H151" s="13" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -6566,7 +6566,7 @@
         <v>1</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D153" s="6" t="s">
         <v>509</v>
@@ -6586,7 +6586,7 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B154" s="1">
         <v>1</v>
@@ -6612,7 +6612,7 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B155" s="1">
         <v>1</v>
@@ -6638,7 +6638,7 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B156" s="1">
         <v>1</v>
@@ -6664,7 +6664,7 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B157" s="1">
         <v>1</v>
@@ -6673,7 +6673,7 @@
         <v>524</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E157" s="6" t="s">
         <v>525</v>
@@ -6682,15 +6682,15 @@
         <v>187</v>
       </c>
       <c r="G157" s="12" t="s">
+        <v>697</v>
+      </c>
+      <c r="H157" s="13" t="s">
         <v>698</v>
-      </c>
-      <c r="H157" s="13" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B158" s="1">
         <v>1</v>
@@ -6716,7 +6716,7 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B159" s="1">
         <v>1</v>
@@ -6742,7 +6742,7 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B160" s="1">
         <v>1</v>
@@ -6760,15 +6760,15 @@
         <v>346</v>
       </c>
       <c r="G160" s="12" t="s">
+        <v>703</v>
+      </c>
+      <c r="H160" s="13" t="s">
         <v>704</v>
-      </c>
-      <c r="H160" s="13" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="161" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B161" s="1">
         <v>7</v>
@@ -6786,7 +6786,7 @@
         <v>187</v>
       </c>
       <c r="G161" s="15" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="H161" s="16" t="s">
         <v>544</v>
@@ -6814,28 +6814,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>682</v>
+      </c>
+      <c r="B1" t="s">
         <v>683</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>684</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>685</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>686</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>687</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>688</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>689</v>
-      </c>
-      <c r="H1" t="s">
-        <v>690</v>
       </c>
       <c r="I1" t="s">
         <v>223</v>

</xml_diff>

<commit_message>
fix part number for 12.7k resistor
</commit_message>
<xml_diff>
--- a/radiant_bom.xlsx
+++ b/radiant_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\radiant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FB19A74-7FE9-4102-B4D7-D0FFE6612164}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB80845-A8F4-4F98-AB48-677478ABF7AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="375" windowWidth="44625" windowHeight="16455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="746">
   <si>
     <t>Item</t>
   </si>
@@ -2283,6 +2283,9 @@
   </si>
   <si>
     <t>L10M L10N L10O L10P L10Q L10R L10S L10T L10U</t>
+  </si>
+  <si>
+    <t>RC0402FR-0712K7L</t>
   </si>
 </sst>
 </file>
@@ -2727,8 +2730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E55CFCB-55D4-4B99-A501-EF331A0E0C1E}">
   <dimension ref="A1:H168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="I114" sqref="I114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5647,7 +5650,7 @@
         <v>602</v>
       </c>
       <c r="G113" s="11" t="s">
-        <v>611</v>
+        <v>745</v>
       </c>
       <c r="H113" s="11" t="s">
         <v>612</v>

</xml_diff>

<commit_message>
update red LED part # for available type
</commit_message>
<xml_diff>
--- a/radiant_bom.xlsx
+++ b/radiant_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\radiant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB80845-A8F4-4F98-AB48-677478ABF7AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65B303E-D42D-4D68-82B8-8AF2712B5B82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="375" windowWidth="44625" windowHeight="16455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1472,9 +1472,6 @@
     <t>SM_LED,Red</t>
   </si>
   <si>
-    <t>SML-D12U1WT86</t>
-  </si>
-  <si>
     <t>LED RED DIFFUSED 1608 SMD</t>
   </si>
   <si>
@@ -2286,6 +2283,9 @@
   </si>
   <si>
     <t>RC0402FR-0712K7L</t>
+  </si>
+  <si>
+    <t>SML-D12V1WT86</t>
   </si>
 </sst>
 </file>
@@ -2730,8 +2730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E55CFCB-55D4-4B99-A501-EF331A0E0C1E}">
   <dimension ref="A1:H168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="I114" sqref="I114"/>
+    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
+      <selection activeCell="G153" sqref="G153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2748,7 +2748,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2761,11 +2761,11 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="12" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="10" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
@@ -2781,7 +2781,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>3</v>
@@ -2807,7 +2807,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>8</v>
@@ -2816,7 +2816,7 @@
         <v>9</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>10</v>
@@ -2833,10 +2833,10 @@
         <v>11</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>697</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>698</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>699</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>12</v>
@@ -2972,7 +2972,7 @@
         <v>12</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>34</v>
@@ -3142,22 +3142,22 @@
         <v>1</v>
       </c>
       <c r="C17" s="6" t="s">
+        <v>700</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>701</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>702</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="F17" s="11" t="s">
         <v>703</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="G17" s="11" t="s">
+        <v>730</v>
+      </c>
+      <c r="H17" s="11" t="s">
         <v>704</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>731</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3246,7 +3246,7 @@
         <v>443</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>89</v>
@@ -3388,10 +3388,10 @@
         <v>115</v>
       </c>
       <c r="G26" s="11" t="s">
+        <v>538</v>
+      </c>
+      <c r="H26" s="11" t="s">
         <v>539</v>
-      </c>
-      <c r="H26" s="11" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="150" x14ac:dyDescent="0.25">
@@ -3466,10 +3466,10 @@
         <v>91</v>
       </c>
       <c r="G29" s="11" t="s">
+        <v>540</v>
+      </c>
+      <c r="H29" s="11" t="s">
         <v>541</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3480,7 +3480,7 @@
         <v>19</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>127</v>
@@ -3492,10 +3492,10 @@
         <v>91</v>
       </c>
       <c r="G30" s="11" t="s">
+        <v>542</v>
+      </c>
+      <c r="H30" s="11" t="s">
         <v>543</v>
-      </c>
-      <c r="H30" s="11" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3518,10 +3518,10 @@
         <v>219</v>
       </c>
       <c r="G31" s="11" t="s">
+        <v>544</v>
+      </c>
+      <c r="H31" s="11" t="s">
         <v>545</v>
-      </c>
-      <c r="H31" s="11" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3544,10 +3544,10 @@
         <v>219</v>
       </c>
       <c r="G32" s="11" t="s">
+        <v>546</v>
+      </c>
+      <c r="H32" s="11" t="s">
         <v>547</v>
-      </c>
-      <c r="H32" s="11" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3558,7 +3558,7 @@
         <v>6</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>131</v>
@@ -3570,10 +3570,10 @@
         <v>91</v>
       </c>
       <c r="G33" s="11" t="s">
+        <v>564</v>
+      </c>
+      <c r="H33" s="11" t="s">
         <v>565</v>
-      </c>
-      <c r="H33" s="11" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3596,10 +3596,10 @@
         <v>118</v>
       </c>
       <c r="G34" s="11" t="s">
+        <v>548</v>
+      </c>
+      <c r="H34" s="11" t="s">
         <v>549</v>
-      </c>
-      <c r="H34" s="11" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3610,7 +3610,7 @@
         <v>10</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>134</v>
@@ -3622,10 +3622,10 @@
         <v>91</v>
       </c>
       <c r="G35" s="11" t="s">
+        <v>550</v>
+      </c>
+      <c r="H35" s="11" t="s">
         <v>551</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3648,10 +3648,10 @@
         <v>91</v>
       </c>
       <c r="G36" s="11" t="s">
+        <v>552</v>
+      </c>
+      <c r="H36" s="11" t="s">
         <v>553</v>
-      </c>
-      <c r="H36" s="11" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3674,10 +3674,10 @@
         <v>91</v>
       </c>
       <c r="G37" s="11" t="s">
+        <v>554</v>
+      </c>
+      <c r="H37" s="11" t="s">
         <v>555</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -3700,10 +3700,10 @@
         <v>91</v>
       </c>
       <c r="G38" s="11" t="s">
+        <v>557</v>
+      </c>
+      <c r="H38" s="11" t="s">
         <v>558</v>
-      </c>
-      <c r="H38" s="11" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3726,10 +3726,10 @@
         <v>86</v>
       </c>
       <c r="G39" s="11" t="s">
+        <v>559</v>
+      </c>
+      <c r="H39" s="11" t="s">
         <v>560</v>
-      </c>
-      <c r="H39" s="11" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3752,10 +3752,10 @@
         <v>219</v>
       </c>
       <c r="G40" s="11" t="s">
+        <v>561</v>
+      </c>
+      <c r="H40" s="11" t="s">
         <v>562</v>
-      </c>
-      <c r="H40" s="11" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -3766,7 +3766,7 @@
         <v>7</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>145</v>
@@ -3778,10 +3778,10 @@
         <v>91</v>
       </c>
       <c r="G41" s="11" t="s">
+        <v>564</v>
+      </c>
+      <c r="H41" s="11" t="s">
         <v>565</v>
-      </c>
-      <c r="H41" s="11" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3804,10 +3804,10 @@
         <v>219</v>
       </c>
       <c r="G42" s="11" t="s">
+        <v>566</v>
+      </c>
+      <c r="H42" s="11" t="s">
         <v>567</v>
-      </c>
-      <c r="H42" s="11" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3830,10 +3830,10 @@
         <v>91</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -3856,10 +3856,10 @@
         <v>219</v>
       </c>
       <c r="G44" s="11" t="s">
+        <v>569</v>
+      </c>
+      <c r="H44" s="11" t="s">
         <v>570</v>
-      </c>
-      <c r="H44" s="11" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3882,10 +3882,10 @@
         <v>91</v>
       </c>
       <c r="G45" s="11" t="s">
+        <v>571</v>
+      </c>
+      <c r="H45" s="11" t="s">
         <v>572</v>
-      </c>
-      <c r="H45" s="11" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3908,10 +3908,10 @@
         <v>118</v>
       </c>
       <c r="G46" s="11" t="s">
+        <v>594</v>
+      </c>
+      <c r="H46" s="11" t="s">
         <v>595</v>
-      </c>
-      <c r="H46" s="11" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3925,7 +3925,7 @@
         <v>162</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>114</v>
@@ -3934,10 +3934,10 @@
         <v>86</v>
       </c>
       <c r="G47" s="11" t="s">
+        <v>574</v>
+      </c>
+      <c r="H47" s="11" t="s">
         <v>575</v>
-      </c>
-      <c r="H47" s="11" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3960,10 +3960,10 @@
         <v>109</v>
       </c>
       <c r="G48" s="11" t="s">
+        <v>596</v>
+      </c>
+      <c r="H48" s="11" t="s">
         <v>597</v>
-      </c>
-      <c r="H48" s="11" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -3983,13 +3983,13 @@
         <v>90</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G49" s="11" t="s">
+        <v>693</v>
+      </c>
+      <c r="H49" s="11" t="s">
         <v>694</v>
-      </c>
-      <c r="H49" s="11" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -4012,10 +4012,10 @@
         <v>219</v>
       </c>
       <c r="G50" s="11" t="s">
+        <v>576</v>
+      </c>
+      <c r="H50" s="11" t="s">
         <v>577</v>
-      </c>
-      <c r="H50" s="11" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -4038,10 +4038,10 @@
         <v>219</v>
       </c>
       <c r="G51" s="11" t="s">
+        <v>578</v>
+      </c>
+      <c r="H51" s="11" t="s">
         <v>579</v>
-      </c>
-      <c r="H51" s="11" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -4064,10 +4064,10 @@
         <v>118</v>
       </c>
       <c r="G52" s="11" t="s">
+        <v>580</v>
+      </c>
+      <c r="H52" s="11" t="s">
         <v>581</v>
-      </c>
-      <c r="H52" s="11" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -4090,10 +4090,10 @@
         <v>109</v>
       </c>
       <c r="G53" s="11" t="s">
+        <v>582</v>
+      </c>
+      <c r="H53" s="11" t="s">
         <v>583</v>
-      </c>
-      <c r="H53" s="11" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -4116,10 +4116,10 @@
         <v>91</v>
       </c>
       <c r="G54" s="11" t="s">
+        <v>584</v>
+      </c>
+      <c r="H54" s="11" t="s">
         <v>585</v>
-      </c>
-      <c r="H54" s="11" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -4142,10 +4142,10 @@
         <v>219</v>
       </c>
       <c r="G55" s="11" t="s">
+        <v>586</v>
+      </c>
+      <c r="H55" s="11" t="s">
         <v>587</v>
-      </c>
-      <c r="H55" s="11" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -4168,10 +4168,10 @@
         <v>91</v>
       </c>
       <c r="G56" s="11" t="s">
+        <v>588</v>
+      </c>
+      <c r="H56" s="11" t="s">
         <v>589</v>
-      </c>
-      <c r="H56" s="11" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4182,10 +4182,10 @@
         <v>30</v>
       </c>
       <c r="C57" s="6" t="s">
+        <v>737</v>
+      </c>
+      <c r="D57" s="8" t="s">
         <v>738</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>739</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>90</v>
@@ -4249,7 +4249,7 @@
         <v>183</v>
       </c>
       <c r="H59" s="11" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -4353,7 +4353,7 @@
         <v>202</v>
       </c>
       <c r="H63" s="11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -4379,7 +4379,7 @@
         <v>207</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -4448,7 +4448,7 @@
         <v>218</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="F67" s="11" t="s">
         <v>219</v>
@@ -4457,7 +4457,7 @@
         <v>220</v>
       </c>
       <c r="H67" s="11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -4494,22 +4494,22 @@
         <v>1</v>
       </c>
       <c r="C69" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="D69" s="8" t="s">
         <v>709</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>710</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>223</v>
       </c>
       <c r="F69" s="11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G69" s="11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="H69" s="11" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -4520,22 +4520,22 @@
         <v>15</v>
       </c>
       <c r="C70" s="6" t="s">
+        <v>739</v>
+      </c>
+      <c r="D70" s="8" t="s">
         <v>740</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="E70" s="8" t="s">
+        <v>711</v>
+      </c>
+      <c r="F70" s="11" t="s">
+        <v>598</v>
+      </c>
+      <c r="G70" s="11" t="s">
         <v>741</v>
       </c>
-      <c r="E70" s="8" t="s">
-        <v>712</v>
-      </c>
-      <c r="F70" s="11" t="s">
-        <v>599</v>
-      </c>
-      <c r="G70" s="11" t="s">
+      <c r="H70" s="11" t="s">
         <v>742</v>
-      </c>
-      <c r="H70" s="11" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -4552,7 +4552,7 @@
         <v>225</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="F71" s="11" t="s">
         <v>219</v>
@@ -4561,7 +4561,7 @@
         <v>226</v>
       </c>
       <c r="H71" s="11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -4578,16 +4578,16 @@
         <v>228</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="F72" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="H72" s="11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4604,7 +4604,7 @@
         <v>230</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F73" s="11" t="s">
         <v>86</v>
@@ -4613,7 +4613,7 @@
         <v>231</v>
       </c>
       <c r="H73" s="11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -4630,7 +4630,7 @@
         <v>233</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F74" s="11" t="s">
         <v>219</v>
@@ -4656,7 +4656,7 @@
         <v>237</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F75" s="11" t="s">
         <v>219</v>
@@ -4676,22 +4676,22 @@
         <v>9</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="F76" s="11" t="s">
         <v>219</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="H76" s="11" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -4708,7 +4708,7 @@
         <v>241</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F77" s="11" t="s">
         <v>219</v>
@@ -4734,7 +4734,7 @@
         <v>245</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F78" s="11" t="s">
         <v>219</v>
@@ -4760,7 +4760,7 @@
         <v>249</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F79" s="11" t="s">
         <v>219</v>
@@ -4783,19 +4783,19 @@
         <v>197</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F80" s="11" t="s">
         <v>109</v>
       </c>
       <c r="G80" s="11" t="s">
+        <v>682</v>
+      </c>
+      <c r="H80" s="11" t="s">
         <v>683</v>
-      </c>
-      <c r="H80" s="11" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -4812,16 +4812,16 @@
         <v>253</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="F81" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G81" s="11" t="s">
+        <v>678</v>
+      </c>
+      <c r="H81" s="11" t="s">
         <v>679</v>
-      </c>
-      <c r="H81" s="11" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -4841,13 +4841,13 @@
         <v>255</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="G82" s="11" t="s">
         <v>255</v>
       </c>
       <c r="H82" s="11" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -5023,10 +5023,10 @@
         <v>291</v>
       </c>
       <c r="F89" s="11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="H89" s="11" t="s">
         <v>292</v>
@@ -5156,7 +5156,7 @@
         <v>12</v>
       </c>
       <c r="G94" s="11" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="H94" s="11" t="s">
         <v>315</v>
@@ -5185,7 +5185,7 @@
         <v>320</v>
       </c>
       <c r="H95" s="11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -5445,7 +5445,7 @@
         <v>362</v>
       </c>
       <c r="H105" s="11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5491,13 +5491,13 @@
         <v>370</v>
       </c>
       <c r="F107" s="11" t="s">
+        <v>598</v>
+      </c>
+      <c r="G107" s="11" t="s">
         <v>599</v>
       </c>
-      <c r="G107" s="11" t="s">
+      <c r="H107" s="11" t="s">
         <v>600</v>
-      </c>
-      <c r="H107" s="11" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -5543,13 +5543,13 @@
         <v>370</v>
       </c>
       <c r="F109" s="11" t="s">
+        <v>601</v>
+      </c>
+      <c r="G109" s="11" t="s">
         <v>602</v>
       </c>
-      <c r="G109" s="11" t="s">
+      <c r="H109" s="11" t="s">
         <v>603</v>
-      </c>
-      <c r="H109" s="11" t="s">
-        <v>604</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -5560,22 +5560,22 @@
         <v>6</v>
       </c>
       <c r="C110" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="D110" s="8" t="s">
         <v>605</v>
       </c>
-      <c r="D110" s="8" t="s">
-        <v>606</v>
-      </c>
       <c r="E110" s="8" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="F110" s="11" t="s">
         <v>18</v>
       </c>
       <c r="G110" s="11" t="s">
+        <v>606</v>
+      </c>
+      <c r="H110" s="11" t="s">
         <v>607</v>
-      </c>
-      <c r="H110" s="11" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5595,13 +5595,13 @@
         <v>370</v>
       </c>
       <c r="F111" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G111" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="H111" s="11" t="s">
         <v>609</v>
-      </c>
-      <c r="H111" s="11" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -5612,7 +5612,7 @@
         <v>224</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D112" s="8" t="s">
         <v>379</v>
@@ -5621,13 +5621,13 @@
         <v>370</v>
       </c>
       <c r="F112" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G112" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="H112" s="11" t="s">
         <v>611</v>
-      </c>
-      <c r="H112" s="11" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5638,22 +5638,22 @@
         <v>24</v>
       </c>
       <c r="C113" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="D113" s="8" t="s">
         <v>720</v>
-      </c>
-      <c r="D113" s="8" t="s">
-        <v>721</v>
       </c>
       <c r="E113" s="8" t="s">
         <v>370</v>
       </c>
       <c r="F113" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G113" s="11" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="H113" s="11" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5673,13 +5673,13 @@
         <v>370</v>
       </c>
       <c r="F114" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G114" s="11" t="s">
+        <v>651</v>
+      </c>
+      <c r="H114" s="11" t="s">
         <v>652</v>
-      </c>
-      <c r="H114" s="11" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -5690,7 +5690,7 @@
         <v>3</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D115" s="8" t="s">
         <v>382</v>
@@ -5699,13 +5699,13 @@
         <v>370</v>
       </c>
       <c r="F115" s="11" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G115" s="11" t="s">
+        <v>614</v>
+      </c>
+      <c r="H115" s="11" t="s">
         <v>615</v>
-      </c>
-      <c r="H115" s="11" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -5722,16 +5722,16 @@
         <v>384</v>
       </c>
       <c r="E116" s="8" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="F116" s="11" t="s">
+        <v>616</v>
+      </c>
+      <c r="G116" s="11" t="s">
         <v>617</v>
       </c>
-      <c r="G116" s="11" t="s">
+      <c r="H116" s="11" t="s">
         <v>618</v>
-      </c>
-      <c r="H116" s="11" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5751,13 +5751,13 @@
         <v>370</v>
       </c>
       <c r="F117" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G117" s="11" t="s">
+        <v>619</v>
+      </c>
+      <c r="H117" s="11" t="s">
         <v>620</v>
-      </c>
-      <c r="H117" s="11" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5777,13 +5777,13 @@
         <v>370</v>
       </c>
       <c r="F118" s="11" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G118" s="11" t="s">
+        <v>621</v>
+      </c>
+      <c r="H118" s="11" t="s">
         <v>622</v>
-      </c>
-      <c r="H118" s="11" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5803,13 +5803,13 @@
         <v>370</v>
       </c>
       <c r="F119" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G119" s="11" t="s">
+        <v>623</v>
+      </c>
+      <c r="H119" s="11" t="s">
         <v>624</v>
-      </c>
-      <c r="H119" s="11" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -5829,13 +5829,13 @@
         <v>370</v>
       </c>
       <c r="F120" s="11" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G120" s="11" t="s">
+        <v>625</v>
+      </c>
+      <c r="H120" s="11" t="s">
         <v>626</v>
-      </c>
-      <c r="H120" s="11" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -5846,7 +5846,7 @@
         <v>11</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D121" s="8" t="s">
         <v>395</v>
@@ -5855,13 +5855,13 @@
         <v>370</v>
       </c>
       <c r="F121" s="11" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G121" s="11" t="s">
+        <v>627</v>
+      </c>
+      <c r="H121" s="11" t="s">
         <v>628</v>
-      </c>
-      <c r="H121" s="11" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -5881,13 +5881,13 @@
         <v>370</v>
       </c>
       <c r="F122" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G122" s="11" t="s">
+        <v>629</v>
+      </c>
+      <c r="H122" s="11" t="s">
         <v>630</v>
-      </c>
-      <c r="H122" s="11" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -5907,13 +5907,13 @@
         <v>370</v>
       </c>
       <c r="F123" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G123" s="11" t="s">
+        <v>631</v>
+      </c>
+      <c r="H123" s="11" t="s">
         <v>632</v>
-      </c>
-      <c r="H123" s="11" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5930,16 +5930,16 @@
         <v>401</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="F124" s="11" t="s">
+        <v>633</v>
+      </c>
+      <c r="G124" s="11" t="s">
         <v>634</v>
       </c>
-      <c r="G124" s="11" t="s">
+      <c r="H124" s="11" t="s">
         <v>635</v>
-      </c>
-      <c r="H124" s="11" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5950,7 +5950,7 @@
         <v>26</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D125" s="8" t="s">
         <v>402</v>
@@ -5959,13 +5959,13 @@
         <v>370</v>
       </c>
       <c r="F125" s="11" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G125" s="11" t="s">
+        <v>637</v>
+      </c>
+      <c r="H125" s="11" t="s">
         <v>638</v>
-      </c>
-      <c r="H125" s="11" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -5976,7 +5976,7 @@
         <v>1</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D126" s="8" t="s">
         <v>403</v>
@@ -5985,13 +5985,13 @@
         <v>370</v>
       </c>
       <c r="F126" s="11" t="s">
+        <v>639</v>
+      </c>
+      <c r="G126" s="11" t="s">
         <v>640</v>
       </c>
-      <c r="G126" s="11" t="s">
+      <c r="H126" s="11" t="s">
         <v>641</v>
-      </c>
-      <c r="H126" s="11" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -6011,13 +6011,13 @@
         <v>370</v>
       </c>
       <c r="F127" s="11" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G127" s="11" t="s">
+        <v>642</v>
+      </c>
+      <c r="H127" s="11" t="s">
         <v>643</v>
-      </c>
-      <c r="H127" s="11" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -6028,7 +6028,7 @@
         <v>2</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D128" s="8" t="s">
         <v>406</v>
@@ -6037,13 +6037,13 @@
         <v>370</v>
       </c>
       <c r="F128" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G128" s="11" t="s">
+        <v>644</v>
+      </c>
+      <c r="H128" s="11" t="s">
         <v>645</v>
-      </c>
-      <c r="H128" s="11" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -6063,13 +6063,13 @@
         <v>392</v>
       </c>
       <c r="F129" s="11" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G129" s="11" t="s">
+        <v>691</v>
+      </c>
+      <c r="H129" s="11" t="s">
         <v>692</v>
-      </c>
-      <c r="H129" s="11" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -6083,19 +6083,19 @@
         <v>407</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E130" s="8" t="s">
         <v>370</v>
       </c>
       <c r="F130" s="11" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G130" s="11" t="s">
+        <v>646</v>
+      </c>
+      <c r="H130" s="11" t="s">
         <v>647</v>
-      </c>
-      <c r="H130" s="11" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -6106,7 +6106,7 @@
         <v>102</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D131" s="8" t="s">
         <v>409</v>
@@ -6115,13 +6115,13 @@
         <v>370</v>
       </c>
       <c r="F131" s="11" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G131" s="11" t="s">
+        <v>649</v>
+      </c>
+      <c r="H131" s="11" t="s">
         <v>650</v>
-      </c>
-      <c r="H131" s="11" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -6141,13 +6141,13 @@
         <v>370</v>
       </c>
       <c r="F132" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G132" s="11" t="s">
+        <v>654</v>
+      </c>
+      <c r="H132" s="11" t="s">
         <v>655</v>
-      </c>
-      <c r="H132" s="11" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -6164,16 +6164,16 @@
         <v>413</v>
       </c>
       <c r="E133" s="8" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="F133" s="11" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G133" s="11" t="s">
+        <v>656</v>
+      </c>
+      <c r="H133" s="11" t="s">
         <v>657</v>
-      </c>
-      <c r="H133" s="11" t="s">
-        <v>658</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -6193,13 +6193,13 @@
         <v>370</v>
       </c>
       <c r="F134" s="11" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G134" s="11" t="s">
+        <v>658</v>
+      </c>
+      <c r="H134" s="11" t="s">
         <v>659</v>
-      </c>
-      <c r="H134" s="11" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -6210,22 +6210,22 @@
         <v>25</v>
       </c>
       <c r="C135" s="6" t="s">
+        <v>660</v>
+      </c>
+      <c r="D135" s="8" t="s">
         <v>661</v>
-      </c>
-      <c r="D135" s="8" t="s">
-        <v>662</v>
       </c>
       <c r="E135" s="8" t="s">
         <v>392</v>
       </c>
       <c r="F135" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G135" s="11" t="s">
+        <v>662</v>
+      </c>
+      <c r="H135" s="11" t="s">
         <v>663</v>
-      </c>
-      <c r="H135" s="11" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -6236,7 +6236,7 @@
         <v>9</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D136" s="8" t="s">
         <v>416</v>
@@ -6245,13 +6245,13 @@
         <v>370</v>
       </c>
       <c r="F136" s="11" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G136" s="11" t="s">
+        <v>664</v>
+      </c>
+      <c r="H136" s="11" t="s">
         <v>665</v>
-      </c>
-      <c r="H136" s="11" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -6262,22 +6262,22 @@
         <v>1</v>
       </c>
       <c r="C137" s="6" t="s">
+        <v>591</v>
+      </c>
+      <c r="D137" s="8" t="s">
         <v>592</v>
-      </c>
-      <c r="D137" s="8" t="s">
-        <v>593</v>
       </c>
       <c r="E137" s="8" t="s">
         <v>370</v>
       </c>
       <c r="F137" s="11" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G137" s="11" t="s">
+        <v>666</v>
+      </c>
+      <c r="H137" s="11" t="s">
         <v>667</v>
-      </c>
-      <c r="H137" s="11" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -6297,13 +6297,13 @@
         <v>370</v>
       </c>
       <c r="F138" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G138" s="11" t="s">
+        <v>689</v>
+      </c>
+      <c r="H138" s="11" t="s">
         <v>690</v>
-      </c>
-      <c r="H138" s="11" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -6323,13 +6323,13 @@
         <v>370</v>
       </c>
       <c r="F139" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G139" s="11" t="s">
+        <v>668</v>
+      </c>
+      <c r="H139" s="11" t="s">
         <v>669</v>
-      </c>
-      <c r="H139" s="11" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -6349,13 +6349,13 @@
         <v>370</v>
       </c>
       <c r="F140" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G140" s="11" t="s">
+        <v>670</v>
+      </c>
+      <c r="H140" s="11" t="s">
         <v>671</v>
-      </c>
-      <c r="H140" s="11" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -6375,13 +6375,13 @@
         <v>370</v>
       </c>
       <c r="F141" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G141" s="11" t="s">
+        <v>672</v>
+      </c>
+      <c r="H141" s="11" t="s">
         <v>673</v>
-      </c>
-      <c r="H141" s="11" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="142" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -6392,7 +6392,7 @@
         <v>89</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D142" s="8" t="s">
         <v>425</v>
@@ -6407,7 +6407,7 @@
         <v>196</v>
       </c>
       <c r="H142" s="11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="143" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -6534,7 +6534,7 @@
         <v>452</v>
       </c>
       <c r="G147" s="11" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="H147" s="11" t="s">
         <v>453</v>
@@ -6563,7 +6563,7 @@
         <v>457</v>
       </c>
       <c r="H148" s="11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="149" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -6612,10 +6612,10 @@
         <v>461</v>
       </c>
       <c r="G150" s="11" t="s">
+        <v>731</v>
+      </c>
+      <c r="H150" s="11" t="s">
         <v>732</v>
-      </c>
-      <c r="H150" s="11" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -6664,10 +6664,10 @@
         <v>435</v>
       </c>
       <c r="G152" s="11" t="s">
+        <v>745</v>
+      </c>
+      <c r="H152" s="11" t="s">
         <v>474</v>
-      </c>
-      <c r="H152" s="11" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -6678,22 +6678,22 @@
         <v>1</v>
       </c>
       <c r="C153" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="D153" s="8" t="s">
         <v>476</v>
       </c>
-      <c r="D153" s="8" t="s">
+      <c r="E153" s="8" t="s">
         <v>477</v>
       </c>
-      <c r="E153" s="8" t="s">
+      <c r="F153" s="11" t="s">
         <v>478</v>
       </c>
-      <c r="F153" s="11" t="s">
+      <c r="G153" s="11" t="s">
         <v>479</v>
       </c>
-      <c r="G153" s="11" t="s">
+      <c r="H153" s="11" t="s">
         <v>480</v>
-      </c>
-      <c r="H153" s="11" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -6704,13 +6704,13 @@
         <v>2</v>
       </c>
       <c r="C154" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="D154" s="8" t="s">
         <v>482</v>
       </c>
-      <c r="D154" s="8" t="s">
-        <v>483</v>
-      </c>
       <c r="E154" s="8" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F154" s="11" t="s">
         <v>196</v>
@@ -6719,7 +6719,7 @@
         <v>196</v>
       </c>
       <c r="H154" s="11" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="155" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -6730,22 +6730,22 @@
         <v>24</v>
       </c>
       <c r="C155" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="D155" s="8" t="s">
         <v>485</v>
       </c>
-      <c r="D155" s="8" t="s">
+      <c r="E155" s="8" t="s">
         <v>486</v>
-      </c>
-      <c r="E155" s="8" t="s">
-        <v>487</v>
       </c>
       <c r="F155" s="11" t="s">
         <v>447</v>
       </c>
       <c r="G155" s="11" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H155" s="11" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -6756,22 +6756,22 @@
         <v>1</v>
       </c>
       <c r="C156" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="D156" s="8" t="s">
         <v>489</v>
       </c>
-      <c r="D156" s="8" t="s">
-        <v>490</v>
-      </c>
       <c r="E156" s="8" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F156" s="11" t="s">
         <v>447</v>
       </c>
       <c r="G156" s="11" t="s">
+        <v>489</v>
+      </c>
+      <c r="H156" s="11" t="s">
         <v>490</v>
-      </c>
-      <c r="H156" s="11" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="157" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -6782,22 +6782,22 @@
         <v>24</v>
       </c>
       <c r="C157" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="D157" s="8" t="s">
         <v>492</v>
       </c>
-      <c r="D157" s="8" t="s">
-        <v>493</v>
-      </c>
       <c r="E157" s="8" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F157" s="11" t="s">
         <v>109</v>
       </c>
       <c r="G157" s="11" t="s">
+        <v>493</v>
+      </c>
+      <c r="H157" s="11" t="s">
         <v>494</v>
-      </c>
-      <c r="H157" s="11" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -6808,13 +6808,13 @@
         <v>125</v>
       </c>
       <c r="C158" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="D158" s="8" t="s">
         <v>496</v>
       </c>
-      <c r="D158" s="8" t="s">
+      <c r="E158" s="8" t="s">
         <v>497</v>
-      </c>
-      <c r="E158" s="8" t="s">
-        <v>498</v>
       </c>
       <c r="F158" s="11" t="s">
         <v>196</v>
@@ -6823,7 +6823,7 @@
         <v>196</v>
       </c>
       <c r="H158" s="11" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -6834,22 +6834,22 @@
         <v>1</v>
       </c>
       <c r="C159" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="D159" s="8" t="s">
         <v>499</v>
       </c>
-      <c r="D159" s="8" t="s">
+      <c r="E159" s="8" t="s">
         <v>500</v>
-      </c>
-      <c r="E159" s="8" t="s">
-        <v>501</v>
       </c>
       <c r="F159" s="11" t="s">
         <v>185</v>
       </c>
       <c r="G159" s="11" t="s">
+        <v>500</v>
+      </c>
+      <c r="H159" s="11" t="s">
         <v>501</v>
-      </c>
-      <c r="H159" s="11" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -6860,22 +6860,22 @@
         <v>2</v>
       </c>
       <c r="C160" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D160" s="8" t="s">
+        <v>502</v>
+      </c>
+      <c r="E160" s="8" t="s">
         <v>503</v>
-      </c>
-      <c r="E160" s="8" t="s">
-        <v>504</v>
       </c>
       <c r="F160" s="11" t="s">
         <v>185</v>
       </c>
       <c r="G160" s="11" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="H160" s="11" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
@@ -6886,22 +6886,22 @@
         <v>1</v>
       </c>
       <c r="C161" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="D161" s="8" t="s">
         <v>506</v>
       </c>
-      <c r="D161" s="8" t="s">
+      <c r="E161" s="8" t="s">
         <v>507</v>
-      </c>
-      <c r="E161" s="8" t="s">
-        <v>508</v>
       </c>
       <c r="F161" s="11" t="s">
         <v>185</v>
       </c>
       <c r="G161" s="11" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="H161" s="11" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
@@ -6912,22 +6912,22 @@
         <v>1</v>
       </c>
       <c r="C162" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="D162" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="E162" s="8" t="s">
         <v>510</v>
-      </c>
-      <c r="D162" s="8" t="s">
-        <v>507</v>
-      </c>
-      <c r="E162" s="8" t="s">
-        <v>511</v>
       </c>
       <c r="F162" s="11" t="s">
         <v>185</v>
       </c>
       <c r="G162" s="11" t="s">
+        <v>511</v>
+      </c>
+      <c r="H162" s="11" t="s">
         <v>512</v>
-      </c>
-      <c r="H162" s="11" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
@@ -6938,22 +6938,22 @@
         <v>1</v>
       </c>
       <c r="C163" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="D163" s="8" t="s">
         <v>514</v>
       </c>
-      <c r="D163" s="8" t="s">
+      <c r="E163" s="8" t="s">
         <v>515</v>
-      </c>
-      <c r="E163" s="8" t="s">
-        <v>516</v>
       </c>
       <c r="F163" s="11" t="s">
         <v>185</v>
       </c>
       <c r="G163" s="11" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H163" s="11" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
@@ -6964,22 +6964,22 @@
         <v>1</v>
       </c>
       <c r="C164" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="D164" s="8" t="s">
+        <v>724</v>
+      </c>
+      <c r="E164" s="8" t="s">
         <v>518</v>
-      </c>
-      <c r="D164" s="8" t="s">
-        <v>725</v>
-      </c>
-      <c r="E164" s="8" t="s">
-        <v>519</v>
       </c>
       <c r="F164" s="11" t="s">
         <v>185</v>
       </c>
       <c r="G164" s="11" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="H164" s="11" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
@@ -6990,22 +6990,22 @@
         <v>1</v>
       </c>
       <c r="C165" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="D165" s="8" t="s">
         <v>520</v>
       </c>
-      <c r="D165" s="8" t="s">
+      <c r="E165" s="8" t="s">
         <v>521</v>
       </c>
-      <c r="E165" s="8" t="s">
+      <c r="F165" s="11" t="s">
         <v>522</v>
       </c>
-      <c r="F165" s="11" t="s">
+      <c r="G165" s="11" t="s">
         <v>523</v>
       </c>
-      <c r="G165" s="11" t="s">
+      <c r="H165" s="11" t="s">
         <v>524</v>
-      </c>
-      <c r="H165" s="11" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
@@ -7016,22 +7016,22 @@
         <v>1</v>
       </c>
       <c r="C166" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="D166" s="8" t="s">
         <v>526</v>
       </c>
-      <c r="D166" s="8" t="s">
+      <c r="E166" s="8" t="s">
         <v>527</v>
       </c>
-      <c r="E166" s="8" t="s">
+      <c r="F166" s="11" t="s">
         <v>528</v>
       </c>
-      <c r="F166" s="11" t="s">
+      <c r="G166" s="11" t="s">
         <v>529</v>
       </c>
-      <c r="G166" s="11" t="s">
+      <c r="H166" s="11" t="s">
         <v>530</v>
-      </c>
-      <c r="H166" s="11" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
@@ -7042,22 +7042,22 @@
         <v>1</v>
       </c>
       <c r="C167" s="6" t="s">
+        <v>531</v>
+      </c>
+      <c r="D167" s="8" t="s">
         <v>532</v>
       </c>
-      <c r="D167" s="8" t="s">
+      <c r="E167" s="8" t="s">
         <v>533</v>
-      </c>
-      <c r="E167" s="8" t="s">
-        <v>534</v>
       </c>
       <c r="F167" s="11" t="s">
         <v>344</v>
       </c>
       <c r="G167" s="11" t="s">
+        <v>684</v>
+      </c>
+      <c r="H167" s="11" t="s">
         <v>685</v>
-      </c>
-      <c r="H167" s="11" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
@@ -7068,22 +7068,22 @@
         <v>7</v>
       </c>
       <c r="C168" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="D168" s="8" t="s">
         <v>535</v>
       </c>
-      <c r="D168" s="8" t="s">
+      <c r="E168" s="8" t="s">
         <v>536</v>
-      </c>
-      <c r="E168" s="8" t="s">
-        <v>537</v>
       </c>
       <c r="F168" s="11" t="s">
         <v>185</v>
       </c>
       <c r="G168" s="11" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="H168" s="11" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update MIC94310 for more available package type
</commit_message>
<xml_diff>
--- a/radiant_bom.xlsx
+++ b/radiant_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\radiant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65B303E-D42D-4D68-82B8-8AF2712B5B82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8355B69F-E86B-478E-A6B4-BA2B4D6C43F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="375" windowWidth="44625" windowHeight="16455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -971,9 +971,6 @@
     <t>Micrel</t>
   </si>
   <si>
-    <t>MIC94310-PYMT-TR</t>
-  </si>
-  <si>
     <t>LDO Voltage Regulators 200mA Ripple Blocker, with Fixed Output Voltage Follower</t>
   </si>
   <si>
@@ -2286,6 +2283,9 @@
   </si>
   <si>
     <t>SML-D12V1WT86</t>
+  </si>
+  <si>
+    <t>MIC94310-PYMT-T5</t>
   </si>
 </sst>
 </file>
@@ -2730,8 +2730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E55CFCB-55D4-4B99-A501-EF331A0E0C1E}">
   <dimension ref="A1:H168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="G153" sqref="G153"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2748,7 +2748,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2761,11 +2761,11 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="12" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="10" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
@@ -2781,7 +2781,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>3</v>
@@ -2807,7 +2807,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>8</v>
@@ -2816,7 +2816,7 @@
         <v>9</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>10</v>
@@ -2833,10 +2833,10 @@
         <v>11</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>696</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>697</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>698</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>12</v>
@@ -2972,7 +2972,7 @@
         <v>12</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>34</v>
@@ -3142,22 +3142,22 @@
         <v>1</v>
       </c>
       <c r="C17" s="6" t="s">
+        <v>699</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>700</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>701</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="F17" s="11" t="s">
         <v>702</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="G17" s="11" t="s">
+        <v>729</v>
+      </c>
+      <c r="H17" s="11" t="s">
         <v>703</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>730</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3246,7 +3246,7 @@
         <v>443</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>89</v>
@@ -3388,10 +3388,10 @@
         <v>115</v>
       </c>
       <c r="G26" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="H26" s="11" t="s">
         <v>538</v>
-      </c>
-      <c r="H26" s="11" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="150" x14ac:dyDescent="0.25">
@@ -3466,10 +3466,10 @@
         <v>91</v>
       </c>
       <c r="G29" s="11" t="s">
+        <v>539</v>
+      </c>
+      <c r="H29" s="11" t="s">
         <v>540</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3480,7 +3480,7 @@
         <v>19</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>127</v>
@@ -3492,10 +3492,10 @@
         <v>91</v>
       </c>
       <c r="G30" s="11" t="s">
+        <v>541</v>
+      </c>
+      <c r="H30" s="11" t="s">
         <v>542</v>
-      </c>
-      <c r="H30" s="11" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3518,10 +3518,10 @@
         <v>219</v>
       </c>
       <c r="G31" s="11" t="s">
+        <v>543</v>
+      </c>
+      <c r="H31" s="11" t="s">
         <v>544</v>
-      </c>
-      <c r="H31" s="11" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3544,10 +3544,10 @@
         <v>219</v>
       </c>
       <c r="G32" s="11" t="s">
+        <v>545</v>
+      </c>
+      <c r="H32" s="11" t="s">
         <v>546</v>
-      </c>
-      <c r="H32" s="11" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3558,7 +3558,7 @@
         <v>6</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>131</v>
@@ -3570,10 +3570,10 @@
         <v>91</v>
       </c>
       <c r="G33" s="11" t="s">
+        <v>563</v>
+      </c>
+      <c r="H33" s="11" t="s">
         <v>564</v>
-      </c>
-      <c r="H33" s="11" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3596,10 +3596,10 @@
         <v>118</v>
       </c>
       <c r="G34" s="11" t="s">
+        <v>547</v>
+      </c>
+      <c r="H34" s="11" t="s">
         <v>548</v>
-      </c>
-      <c r="H34" s="11" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3610,7 +3610,7 @@
         <v>10</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>134</v>
@@ -3622,10 +3622,10 @@
         <v>91</v>
       </c>
       <c r="G35" s="11" t="s">
+        <v>549</v>
+      </c>
+      <c r="H35" s="11" t="s">
         <v>550</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3648,10 +3648,10 @@
         <v>91</v>
       </c>
       <c r="G36" s="11" t="s">
+        <v>551</v>
+      </c>
+      <c r="H36" s="11" t="s">
         <v>552</v>
-      </c>
-      <c r="H36" s="11" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3674,10 +3674,10 @@
         <v>91</v>
       </c>
       <c r="G37" s="11" t="s">
+        <v>553</v>
+      </c>
+      <c r="H37" s="11" t="s">
         <v>554</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -3700,10 +3700,10 @@
         <v>91</v>
       </c>
       <c r="G38" s="11" t="s">
+        <v>556</v>
+      </c>
+      <c r="H38" s="11" t="s">
         <v>557</v>
-      </c>
-      <c r="H38" s="11" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3726,10 +3726,10 @@
         <v>86</v>
       </c>
       <c r="G39" s="11" t="s">
+        <v>558</v>
+      </c>
+      <c r="H39" s="11" t="s">
         <v>559</v>
-      </c>
-      <c r="H39" s="11" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3752,10 +3752,10 @@
         <v>219</v>
       </c>
       <c r="G40" s="11" t="s">
+        <v>560</v>
+      </c>
+      <c r="H40" s="11" t="s">
         <v>561</v>
-      </c>
-      <c r="H40" s="11" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -3766,7 +3766,7 @@
         <v>7</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>145</v>
@@ -3778,10 +3778,10 @@
         <v>91</v>
       </c>
       <c r="G41" s="11" t="s">
+        <v>563</v>
+      </c>
+      <c r="H41" s="11" t="s">
         <v>564</v>
-      </c>
-      <c r="H41" s="11" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3804,10 +3804,10 @@
         <v>219</v>
       </c>
       <c r="G42" s="11" t="s">
+        <v>565</v>
+      </c>
+      <c r="H42" s="11" t="s">
         <v>566</v>
-      </c>
-      <c r="H42" s="11" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3830,10 +3830,10 @@
         <v>91</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -3856,10 +3856,10 @@
         <v>219</v>
       </c>
       <c r="G44" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="H44" s="11" t="s">
         <v>569</v>
-      </c>
-      <c r="H44" s="11" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3882,10 +3882,10 @@
         <v>91</v>
       </c>
       <c r="G45" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="H45" s="11" t="s">
         <v>571</v>
-      </c>
-      <c r="H45" s="11" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3908,10 +3908,10 @@
         <v>118</v>
       </c>
       <c r="G46" s="11" t="s">
+        <v>593</v>
+      </c>
+      <c r="H46" s="11" t="s">
         <v>594</v>
-      </c>
-      <c r="H46" s="11" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3925,7 +3925,7 @@
         <v>162</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>114</v>
@@ -3934,10 +3934,10 @@
         <v>86</v>
       </c>
       <c r="G47" s="11" t="s">
+        <v>573</v>
+      </c>
+      <c r="H47" s="11" t="s">
         <v>574</v>
-      </c>
-      <c r="H47" s="11" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3960,10 +3960,10 @@
         <v>109</v>
       </c>
       <c r="G48" s="11" t="s">
+        <v>595</v>
+      </c>
+      <c r="H48" s="11" t="s">
         <v>596</v>
-      </c>
-      <c r="H48" s="11" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -3983,13 +3983,13 @@
         <v>90</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G49" s="11" t="s">
+        <v>692</v>
+      </c>
+      <c r="H49" s="11" t="s">
         <v>693</v>
-      </c>
-      <c r="H49" s="11" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -4012,10 +4012,10 @@
         <v>219</v>
       </c>
       <c r="G50" s="11" t="s">
+        <v>575</v>
+      </c>
+      <c r="H50" s="11" t="s">
         <v>576</v>
-      </c>
-      <c r="H50" s="11" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -4038,10 +4038,10 @@
         <v>219</v>
       </c>
       <c r="G51" s="11" t="s">
+        <v>577</v>
+      </c>
+      <c r="H51" s="11" t="s">
         <v>578</v>
-      </c>
-      <c r="H51" s="11" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -4064,10 +4064,10 @@
         <v>118</v>
       </c>
       <c r="G52" s="11" t="s">
+        <v>579</v>
+      </c>
+      <c r="H52" s="11" t="s">
         <v>580</v>
-      </c>
-      <c r="H52" s="11" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -4090,10 +4090,10 @@
         <v>109</v>
       </c>
       <c r="G53" s="11" t="s">
+        <v>581</v>
+      </c>
+      <c r="H53" s="11" t="s">
         <v>582</v>
-      </c>
-      <c r="H53" s="11" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -4116,10 +4116,10 @@
         <v>91</v>
       </c>
       <c r="G54" s="11" t="s">
+        <v>583</v>
+      </c>
+      <c r="H54" s="11" t="s">
         <v>584</v>
-      </c>
-      <c r="H54" s="11" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -4142,10 +4142,10 @@
         <v>219</v>
       </c>
       <c r="G55" s="11" t="s">
+        <v>585</v>
+      </c>
+      <c r="H55" s="11" t="s">
         <v>586</v>
-      </c>
-      <c r="H55" s="11" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -4168,10 +4168,10 @@
         <v>91</v>
       </c>
       <c r="G56" s="11" t="s">
+        <v>587</v>
+      </c>
+      <c r="H56" s="11" t="s">
         <v>588</v>
-      </c>
-      <c r="H56" s="11" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4182,10 +4182,10 @@
         <v>30</v>
       </c>
       <c r="C57" s="6" t="s">
+        <v>736</v>
+      </c>
+      <c r="D57" s="8" t="s">
         <v>737</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>738</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>90</v>
@@ -4249,7 +4249,7 @@
         <v>183</v>
       </c>
       <c r="H59" s="11" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -4353,7 +4353,7 @@
         <v>202</v>
       </c>
       <c r="H63" s="11" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -4379,7 +4379,7 @@
         <v>207</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -4448,7 +4448,7 @@
         <v>218</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="F67" s="11" t="s">
         <v>219</v>
@@ -4457,7 +4457,7 @@
         <v>220</v>
       </c>
       <c r="H67" s="11" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -4494,22 +4494,22 @@
         <v>1</v>
       </c>
       <c r="C69" s="6" t="s">
+        <v>707</v>
+      </c>
+      <c r="D69" s="8" t="s">
         <v>708</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>709</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>223</v>
       </c>
       <c r="F69" s="11" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="G69" s="11" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="H69" s="11" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -4520,22 +4520,22 @@
         <v>15</v>
       </c>
       <c r="C70" s="6" t="s">
+        <v>738</v>
+      </c>
+      <c r="D70" s="8" t="s">
         <v>739</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="E70" s="8" t="s">
+        <v>710</v>
+      </c>
+      <c r="F70" s="11" t="s">
+        <v>597</v>
+      </c>
+      <c r="G70" s="11" t="s">
         <v>740</v>
       </c>
-      <c r="E70" s="8" t="s">
-        <v>711</v>
-      </c>
-      <c r="F70" s="11" t="s">
-        <v>598</v>
-      </c>
-      <c r="G70" s="11" t="s">
+      <c r="H70" s="11" t="s">
         <v>741</v>
-      </c>
-      <c r="H70" s="11" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -4552,7 +4552,7 @@
         <v>225</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="F71" s="11" t="s">
         <v>219</v>
@@ -4561,7 +4561,7 @@
         <v>226</v>
       </c>
       <c r="H71" s="11" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -4578,16 +4578,16 @@
         <v>228</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="F72" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="H72" s="11" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4604,7 +4604,7 @@
         <v>230</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F73" s="11" t="s">
         <v>86</v>
@@ -4613,7 +4613,7 @@
         <v>231</v>
       </c>
       <c r="H73" s="11" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -4630,7 +4630,7 @@
         <v>233</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F74" s="11" t="s">
         <v>219</v>
@@ -4656,7 +4656,7 @@
         <v>237</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F75" s="11" t="s">
         <v>219</v>
@@ -4676,22 +4676,22 @@
         <v>9</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="F76" s="11" t="s">
         <v>219</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="H76" s="11" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -4708,7 +4708,7 @@
         <v>241</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F77" s="11" t="s">
         <v>219</v>
@@ -4734,7 +4734,7 @@
         <v>245</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F78" s="11" t="s">
         <v>219</v>
@@ -4760,7 +4760,7 @@
         <v>249</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F79" s="11" t="s">
         <v>219</v>
@@ -4783,19 +4783,19 @@
         <v>197</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="F80" s="11" t="s">
         <v>109</v>
       </c>
       <c r="G80" s="11" t="s">
+        <v>681</v>
+      </c>
+      <c r="H80" s="11" t="s">
         <v>682</v>
-      </c>
-      <c r="H80" s="11" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -4812,16 +4812,16 @@
         <v>253</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="F81" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G81" s="11" t="s">
+        <v>677</v>
+      </c>
+      <c r="H81" s="11" t="s">
         <v>678</v>
-      </c>
-      <c r="H81" s="11" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -4841,13 +4841,13 @@
         <v>255</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G82" s="11" t="s">
         <v>255</v>
       </c>
       <c r="H82" s="11" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -5023,10 +5023,10 @@
         <v>291</v>
       </c>
       <c r="F89" s="11" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="H89" s="11" t="s">
         <v>292</v>
@@ -5104,10 +5104,10 @@
         <v>306</v>
       </c>
       <c r="G92" s="11" t="s">
+        <v>745</v>
+      </c>
+      <c r="H92" s="11" t="s">
         <v>307</v>
-      </c>
-      <c r="H92" s="11" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -5118,22 +5118,22 @@
         <v>24</v>
       </c>
       <c r="C93" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="D93" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="D93" s="8" t="s">
+      <c r="E93" s="8" t="s">
         <v>310</v>
-      </c>
-      <c r="E93" s="8" t="s">
-        <v>311</v>
       </c>
       <c r="F93" s="11" t="s">
         <v>68</v>
       </c>
       <c r="G93" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H93" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -5144,22 +5144,22 @@
         <v>1</v>
       </c>
       <c r="C94" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="D94" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="D94" s="8" t="s">
-        <v>314</v>
-      </c>
       <c r="E94" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F94" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G94" s="11" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="H94" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -5170,22 +5170,22 @@
         <v>1</v>
       </c>
       <c r="C95" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="D95" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="D95" s="8" t="s">
+      <c r="E95" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="E95" s="8" t="s">
+      <c r="F95" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="F95" s="11" t="s">
+      <c r="G95" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="G95" s="11" t="s">
-        <v>320</v>
-      </c>
       <c r="H95" s="11" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -5196,22 +5196,22 @@
         <v>74</v>
       </c>
       <c r="C96" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="D96" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="D96" s="8" t="s">
+      <c r="E96" s="8" t="s">
         <v>322</v>
-      </c>
-      <c r="E96" s="8" t="s">
-        <v>323</v>
       </c>
       <c r="F96" s="11" t="s">
         <v>219</v>
       </c>
       <c r="G96" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="H96" s="11" t="s">
         <v>324</v>
-      </c>
-      <c r="H96" s="11" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -5222,22 +5222,22 @@
         <v>6</v>
       </c>
       <c r="C97" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="D97" s="8" t="s">
         <v>326</v>
       </c>
-      <c r="D97" s="8" t="s">
+      <c r="E97" s="8" t="s">
         <v>327</v>
-      </c>
-      <c r="E97" s="8" t="s">
-        <v>328</v>
       </c>
       <c r="F97" s="11" t="s">
         <v>80</v>
       </c>
       <c r="G97" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H97" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -5248,22 +5248,22 @@
         <v>2</v>
       </c>
       <c r="C98" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="D98" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="D98" s="8" t="s">
+      <c r="E98" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="E98" s="8" t="s">
+      <c r="F98" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="F98" s="11" t="s">
+      <c r="G98" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="H98" s="11" t="s">
         <v>333</v>
-      </c>
-      <c r="G98" s="11" t="s">
-        <v>331</v>
-      </c>
-      <c r="H98" s="11" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -5274,22 +5274,22 @@
         <v>24</v>
       </c>
       <c r="C99" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="D99" s="8" t="s">
         <v>335</v>
       </c>
-      <c r="D99" s="8" t="s">
+      <c r="E99" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="F99" s="11" t="s">
+        <v>332</v>
+      </c>
+      <c r="G99" s="11" t="s">
+        <v>335</v>
+      </c>
+      <c r="H99" s="11" t="s">
         <v>336</v>
-      </c>
-      <c r="E99" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="F99" s="11" t="s">
-        <v>333</v>
-      </c>
-      <c r="G99" s="11" t="s">
-        <v>336</v>
-      </c>
-      <c r="H99" s="11" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -5300,22 +5300,22 @@
         <v>4</v>
       </c>
       <c r="C100" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="D100" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="D100" s="8" t="s">
+      <c r="E100" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="F100" s="11" t="s">
+        <v>332</v>
+      </c>
+      <c r="G100" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="H100" s="11" t="s">
         <v>339</v>
-      </c>
-      <c r="E100" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="F100" s="11" t="s">
-        <v>333</v>
-      </c>
-      <c r="G100" s="11" t="s">
-        <v>339</v>
-      </c>
-      <c r="H100" s="11" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -5326,22 +5326,22 @@
         <v>1</v>
       </c>
       <c r="C101" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="D101" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="D101" s="8" t="s">
+      <c r="E101" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="E101" s="8" t="s">
+      <c r="F101" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="F101" s="11" t="s">
+      <c r="G101" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="H101" s="11" t="s">
         <v>344</v>
-      </c>
-      <c r="G101" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="H101" s="11" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -5352,13 +5352,13 @@
         <v>18</v>
       </c>
       <c r="C102" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="D102" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="D102" s="8" t="s">
+      <c r="E102" s="8" t="s">
         <v>347</v>
-      </c>
-      <c r="E102" s="8" t="s">
-        <v>348</v>
       </c>
       <c r="F102" s="11" t="s">
         <v>196</v>
@@ -5378,22 +5378,22 @@
         <v>2</v>
       </c>
       <c r="C103" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="D103" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="D103" s="8" t="s">
+      <c r="E103" s="8" t="s">
         <v>350</v>
-      </c>
-      <c r="E103" s="8" t="s">
-        <v>351</v>
       </c>
       <c r="F103" s="11" t="s">
         <v>219</v>
       </c>
       <c r="G103" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="H103" s="11" t="s">
         <v>352</v>
-      </c>
-      <c r="H103" s="11" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -5404,22 +5404,22 @@
         <v>1</v>
       </c>
       <c r="C104" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="D104" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="D104" s="8" t="s">
+      <c r="E104" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="E104" s="8" t="s">
+      <c r="F104" s="11" t="s">
         <v>356</v>
       </c>
-      <c r="F104" s="11" t="s">
+      <c r="G104" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="H104" s="11" t="s">
         <v>357</v>
-      </c>
-      <c r="G104" s="11" t="s">
-        <v>355</v>
-      </c>
-      <c r="H104" s="11" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -5430,22 +5430,22 @@
         <v>1</v>
       </c>
       <c r="C105" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="D105" s="8" t="s">
         <v>359</v>
       </c>
-      <c r="D105" s="8" t="s">
+      <c r="E105" s="8" t="s">
         <v>360</v>
-      </c>
-      <c r="E105" s="8" t="s">
-        <v>361</v>
       </c>
       <c r="F105" s="11" t="s">
         <v>68</v>
       </c>
       <c r="G105" s="11" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H105" s="11" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5456,22 +5456,22 @@
         <v>24</v>
       </c>
       <c r="C106" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="D106" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="D106" s="8" t="s">
+      <c r="E106" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="F106" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="E106" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="F106" s="11" t="s">
+      <c r="G106" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="G106" s="11" t="s">
+      <c r="H106" s="11" t="s">
         <v>366</v>
-      </c>
-      <c r="H106" s="11" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5482,22 +5482,22 @@
         <v>49</v>
       </c>
       <c r="C107" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="D107" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="D107" s="8" t="s">
+      <c r="E107" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="E107" s="8" t="s">
-        <v>370</v>
-      </c>
       <c r="F107" s="11" t="s">
+        <v>597</v>
+      </c>
+      <c r="G107" s="11" t="s">
         <v>598</v>
       </c>
-      <c r="G107" s="11" t="s">
+      <c r="H107" s="11" t="s">
         <v>599</v>
-      </c>
-      <c r="H107" s="11" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -5508,22 +5508,22 @@
         <v>6</v>
       </c>
       <c r="C108" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="D108" s="8" t="s">
         <v>371</v>
       </c>
-      <c r="D108" s="8" t="s">
-        <v>372</v>
-      </c>
       <c r="E108" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F108" s="11" t="s">
         <v>179</v>
       </c>
       <c r="G108" s="11" t="s">
+        <v>372</v>
+      </c>
+      <c r="H108" s="11" t="s">
         <v>373</v>
-      </c>
-      <c r="H108" s="11" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5534,22 +5534,22 @@
         <v>73</v>
       </c>
       <c r="C109" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="D109" s="8" t="s">
         <v>375</v>
       </c>
-      <c r="D109" s="8" t="s">
-        <v>376</v>
-      </c>
       <c r="E109" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F109" s="11" t="s">
+        <v>600</v>
+      </c>
+      <c r="G109" s="11" t="s">
         <v>601</v>
       </c>
-      <c r="G109" s="11" t="s">
+      <c r="H109" s="11" t="s">
         <v>602</v>
-      </c>
-      <c r="H109" s="11" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -5560,22 +5560,22 @@
         <v>6</v>
       </c>
       <c r="C110" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="D110" s="8" t="s">
         <v>604</v>
       </c>
-      <c r="D110" s="8" t="s">
-        <v>605</v>
-      </c>
       <c r="E110" s="8" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="F110" s="11" t="s">
         <v>18</v>
       </c>
       <c r="G110" s="11" t="s">
+        <v>605</v>
+      </c>
+      <c r="H110" s="11" t="s">
         <v>606</v>
-      </c>
-      <c r="H110" s="11" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5586,22 +5586,22 @@
         <v>51</v>
       </c>
       <c r="C111" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="D111" s="8" t="s">
         <v>377</v>
       </c>
-      <c r="D111" s="8" t="s">
-        <v>378</v>
-      </c>
       <c r="E111" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F111" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G111" s="11" t="s">
+        <v>607</v>
+      </c>
+      <c r="H111" s="11" t="s">
         <v>608</v>
-      </c>
-      <c r="H111" s="11" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -5612,22 +5612,22 @@
         <v>224</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E112" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F112" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G112" s="11" t="s">
+        <v>609</v>
+      </c>
+      <c r="H112" s="11" t="s">
         <v>610</v>
-      </c>
-      <c r="H112" s="11" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5638,22 +5638,22 @@
         <v>24</v>
       </c>
       <c r="C113" s="6" t="s">
+        <v>718</v>
+      </c>
+      <c r="D113" s="8" t="s">
         <v>719</v>
       </c>
-      <c r="D113" s="8" t="s">
-        <v>720</v>
-      </c>
       <c r="E113" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F113" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G113" s="11" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="H113" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5664,22 +5664,22 @@
         <v>24</v>
       </c>
       <c r="C114" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="D114" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="D114" s="8" t="s">
-        <v>381</v>
-      </c>
       <c r="E114" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F114" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G114" s="11" t="s">
+        <v>650</v>
+      </c>
+      <c r="H114" s="11" t="s">
         <v>651</v>
-      </c>
-      <c r="H114" s="11" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -5690,22 +5690,22 @@
         <v>3</v>
       </c>
       <c r="C115" s="6" t="s">
+        <v>612</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E115" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="F115" s="11" t="s">
+        <v>597</v>
+      </c>
+      <c r="G115" s="11" t="s">
         <v>613</v>
       </c>
-      <c r="D115" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="E115" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="F115" s="11" t="s">
-        <v>598</v>
-      </c>
-      <c r="G115" s="11" t="s">
+      <c r="H115" s="11" t="s">
         <v>614</v>
-      </c>
-      <c r="H115" s="11" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -5716,22 +5716,22 @@
         <v>13</v>
       </c>
       <c r="C116" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="D116" s="8" t="s">
         <v>383</v>
       </c>
-      <c r="D116" s="8" t="s">
-        <v>384</v>
-      </c>
       <c r="E116" s="8" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="F116" s="11" t="s">
+        <v>615</v>
+      </c>
+      <c r="G116" s="11" t="s">
         <v>616</v>
       </c>
-      <c r="G116" s="11" t="s">
+      <c r="H116" s="11" t="s">
         <v>617</v>
-      </c>
-      <c r="H116" s="11" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5742,22 +5742,22 @@
         <v>48</v>
       </c>
       <c r="C117" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="D117" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="D117" s="8" t="s">
-        <v>386</v>
-      </c>
       <c r="E117" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F117" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G117" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="H117" s="11" t="s">
         <v>619</v>
-      </c>
-      <c r="H117" s="11" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5768,22 +5768,22 @@
         <v>48</v>
       </c>
       <c r="C118" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="D118" s="8" t="s">
         <v>387</v>
       </c>
-      <c r="D118" s="8" t="s">
-        <v>388</v>
-      </c>
       <c r="E118" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F118" s="11" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G118" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="H118" s="11" t="s">
         <v>621</v>
-      </c>
-      <c r="H118" s="11" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5794,22 +5794,22 @@
         <v>25</v>
       </c>
       <c r="C119" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="D119" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="D119" s="8" t="s">
-        <v>390</v>
-      </c>
       <c r="E119" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F119" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G119" s="11" t="s">
+        <v>622</v>
+      </c>
+      <c r="H119" s="11" t="s">
         <v>623</v>
-      </c>
-      <c r="H119" s="11" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -5820,22 +5820,22 @@
         <v>1</v>
       </c>
       <c r="C120" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="D120" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="D120" s="8" t="s">
-        <v>394</v>
-      </c>
       <c r="E120" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F120" s="11" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G120" s="11" t="s">
+        <v>624</v>
+      </c>
+      <c r="H120" s="11" t="s">
         <v>625</v>
-      </c>
-      <c r="H120" s="11" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -5846,22 +5846,22 @@
         <v>11</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E121" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F121" s="11" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G121" s="11" t="s">
+        <v>626</v>
+      </c>
+      <c r="H121" s="11" t="s">
         <v>627</v>
-      </c>
-      <c r="H121" s="11" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -5872,22 +5872,22 @@
         <v>2</v>
       </c>
       <c r="C122" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="D122" s="8" t="s">
         <v>396</v>
       </c>
-      <c r="D122" s="8" t="s">
-        <v>397</v>
-      </c>
       <c r="E122" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F122" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G122" s="11" t="s">
+        <v>628</v>
+      </c>
+      <c r="H122" s="11" t="s">
         <v>629</v>
-      </c>
-      <c r="H122" s="11" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -5898,22 +5898,22 @@
         <v>1</v>
       </c>
       <c r="C123" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="D123" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="D123" s="8" t="s">
-        <v>399</v>
-      </c>
       <c r="E123" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F123" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G123" s="11" t="s">
+        <v>630</v>
+      </c>
+      <c r="H123" s="11" t="s">
         <v>631</v>
-      </c>
-      <c r="H123" s="11" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5924,22 +5924,22 @@
         <v>24</v>
       </c>
       <c r="C124" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="D124" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="D124" s="8" t="s">
-        <v>401</v>
-      </c>
       <c r="E124" s="8" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="F124" s="11" t="s">
+        <v>632</v>
+      </c>
+      <c r="G124" s="11" t="s">
         <v>633</v>
       </c>
-      <c r="G124" s="11" t="s">
+      <c r="H124" s="11" t="s">
         <v>634</v>
-      </c>
-      <c r="H124" s="11" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5950,22 +5950,22 @@
         <v>26</v>
       </c>
       <c r="C125" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="D125" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="E125" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="F125" s="11" t="s">
+        <v>597</v>
+      </c>
+      <c r="G125" s="11" t="s">
         <v>636</v>
       </c>
-      <c r="D125" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="E125" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="F125" s="11" t="s">
-        <v>598</v>
-      </c>
-      <c r="G125" s="11" t="s">
+      <c r="H125" s="11" t="s">
         <v>637</v>
-      </c>
-      <c r="H125" s="11" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -5976,22 +5976,22 @@
         <v>1</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E126" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F126" s="11" t="s">
+        <v>638</v>
+      </c>
+      <c r="G126" s="11" t="s">
         <v>639</v>
       </c>
-      <c r="G126" s="11" t="s">
+      <c r="H126" s="11" t="s">
         <v>640</v>
-      </c>
-      <c r="H126" s="11" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -6002,22 +6002,22 @@
         <v>8</v>
       </c>
       <c r="C127" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="D127" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="D127" s="8" t="s">
-        <v>405</v>
-      </c>
       <c r="E127" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F127" s="11" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G127" s="11" t="s">
+        <v>641</v>
+      </c>
+      <c r="H127" s="11" t="s">
         <v>642</v>
-      </c>
-      <c r="H127" s="11" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -6028,22 +6028,22 @@
         <v>2</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E128" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F128" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G128" s="11" t="s">
+        <v>643</v>
+      </c>
+      <c r="H128" s="11" t="s">
         <v>644</v>
-      </c>
-      <c r="H128" s="11" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -6054,22 +6054,22 @@
         <v>24</v>
       </c>
       <c r="C129" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="D129" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="E129" s="8" t="s">
         <v>391</v>
       </c>
-      <c r="D129" s="8" t="s">
-        <v>408</v>
-      </c>
-      <c r="E129" s="8" t="s">
-        <v>392</v>
-      </c>
       <c r="F129" s="11" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G129" s="11" t="s">
+        <v>690</v>
+      </c>
+      <c r="H129" s="11" t="s">
         <v>691</v>
-      </c>
-      <c r="H129" s="11" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -6080,22 +6080,22 @@
         <v>1</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E130" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F130" s="11" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G130" s="11" t="s">
+        <v>645</v>
+      </c>
+      <c r="H130" s="11" t="s">
         <v>646</v>
-      </c>
-      <c r="H130" s="11" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -6106,22 +6106,22 @@
         <v>102</v>
       </c>
       <c r="C131" s="6" t="s">
+        <v>647</v>
+      </c>
+      <c r="D131" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="E131" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="F131" s="11" t="s">
+        <v>597</v>
+      </c>
+      <c r="G131" s="11" t="s">
         <v>648</v>
       </c>
-      <c r="D131" s="8" t="s">
-        <v>409</v>
-      </c>
-      <c r="E131" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="F131" s="11" t="s">
-        <v>598</v>
-      </c>
-      <c r="G131" s="11" t="s">
+      <c r="H131" s="11" t="s">
         <v>649</v>
-      </c>
-      <c r="H131" s="11" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -6132,22 +6132,22 @@
         <v>1</v>
       </c>
       <c r="C132" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="D132" s="8" t="s">
         <v>410</v>
       </c>
-      <c r="D132" s="8" t="s">
-        <v>411</v>
-      </c>
       <c r="E132" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F132" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G132" s="11" t="s">
+        <v>653</v>
+      </c>
+      <c r="H132" s="11" t="s">
         <v>654</v>
-      </c>
-      <c r="H132" s="11" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -6158,22 +6158,22 @@
         <v>1</v>
       </c>
       <c r="C133" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="D133" s="8" t="s">
         <v>412</v>
       </c>
-      <c r="D133" s="8" t="s">
-        <v>413</v>
-      </c>
       <c r="E133" s="8" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="F133" s="11" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G133" s="11" t="s">
+        <v>655</v>
+      </c>
+      <c r="H133" s="11" t="s">
         <v>656</v>
-      </c>
-      <c r="H133" s="11" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -6184,22 +6184,22 @@
         <v>55</v>
       </c>
       <c r="C134" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="D134" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="D134" s="8" t="s">
-        <v>415</v>
-      </c>
       <c r="E134" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F134" s="11" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G134" s="11" t="s">
+        <v>657</v>
+      </c>
+      <c r="H134" s="11" t="s">
         <v>658</v>
-      </c>
-      <c r="H134" s="11" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -6210,22 +6210,22 @@
         <v>25</v>
       </c>
       <c r="C135" s="6" t="s">
+        <v>659</v>
+      </c>
+      <c r="D135" s="8" t="s">
         <v>660</v>
       </c>
-      <c r="D135" s="8" t="s">
+      <c r="E135" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="F135" s="11" t="s">
+        <v>600</v>
+      </c>
+      <c r="G135" s="11" t="s">
         <v>661</v>
       </c>
-      <c r="E135" s="8" t="s">
-        <v>392</v>
-      </c>
-      <c r="F135" s="11" t="s">
-        <v>601</v>
-      </c>
-      <c r="G135" s="11" t="s">
+      <c r="H135" s="11" t="s">
         <v>662</v>
-      </c>
-      <c r="H135" s="11" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -6236,22 +6236,22 @@
         <v>9</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E136" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F136" s="11" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G136" s="11" t="s">
+        <v>663</v>
+      </c>
+      <c r="H136" s="11" t="s">
         <v>664</v>
-      </c>
-      <c r="H136" s="11" t="s">
-        <v>665</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -6262,22 +6262,22 @@
         <v>1</v>
       </c>
       <c r="C137" s="6" t="s">
+        <v>590</v>
+      </c>
+      <c r="D137" s="8" t="s">
         <v>591</v>
       </c>
-      <c r="D137" s="8" t="s">
-        <v>592</v>
-      </c>
       <c r="E137" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F137" s="11" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G137" s="11" t="s">
+        <v>665</v>
+      </c>
+      <c r="H137" s="11" t="s">
         <v>666</v>
-      </c>
-      <c r="H137" s="11" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -6288,22 +6288,22 @@
         <v>2</v>
       </c>
       <c r="C138" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="D138" s="8" t="s">
         <v>417</v>
       </c>
-      <c r="D138" s="8" t="s">
-        <v>418</v>
-      </c>
       <c r="E138" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F138" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G138" s="11" t="s">
+        <v>688</v>
+      </c>
+      <c r="H138" s="11" t="s">
         <v>689</v>
-      </c>
-      <c r="H138" s="11" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -6314,22 +6314,22 @@
         <v>1</v>
       </c>
       <c r="C139" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D139" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="D139" s="8" t="s">
-        <v>420</v>
-      </c>
       <c r="E139" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F139" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G139" s="11" t="s">
+        <v>667</v>
+      </c>
+      <c r="H139" s="11" t="s">
         <v>668</v>
-      </c>
-      <c r="H139" s="11" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -6340,22 +6340,22 @@
         <v>2</v>
       </c>
       <c r="C140" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="D140" s="8" t="s">
         <v>421</v>
       </c>
-      <c r="D140" s="8" t="s">
-        <v>422</v>
-      </c>
       <c r="E140" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F140" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G140" s="11" t="s">
+        <v>669</v>
+      </c>
+      <c r="H140" s="11" t="s">
         <v>670</v>
-      </c>
-      <c r="H140" s="11" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -6366,22 +6366,22 @@
         <v>1</v>
       </c>
       <c r="C141" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="D141" s="8" t="s">
         <v>423</v>
       </c>
-      <c r="D141" s="8" t="s">
-        <v>424</v>
-      </c>
       <c r="E141" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F141" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G141" s="11" t="s">
+        <v>671</v>
+      </c>
+      <c r="H141" s="11" t="s">
         <v>672</v>
-      </c>
-      <c r="H141" s="11" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="142" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -6392,13 +6392,13 @@
         <v>89</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E142" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F142" s="11" t="s">
         <v>196</v>
@@ -6407,7 +6407,7 @@
         <v>196</v>
       </c>
       <c r="H142" s="11" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="143" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -6418,22 +6418,22 @@
         <v>48</v>
       </c>
       <c r="C143" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="D143" s="8" t="s">
         <v>426</v>
       </c>
-      <c r="D143" s="8" t="s">
+      <c r="E143" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="E143" s="8" t="s">
+      <c r="F143" s="11" t="s">
         <v>428</v>
       </c>
-      <c r="F143" s="11" t="s">
+      <c r="G143" s="11" t="s">
         <v>429</v>
       </c>
-      <c r="G143" s="11" t="s">
+      <c r="H143" s="11" t="s">
         <v>430</v>
-      </c>
-      <c r="H143" s="11" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -6444,22 +6444,22 @@
         <v>66</v>
       </c>
       <c r="C144" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="D144" s="8" t="s">
         <v>432</v>
       </c>
-      <c r="D144" s="8" t="s">
+      <c r="E144" s="8" t="s">
         <v>433</v>
       </c>
-      <c r="E144" s="8" t="s">
+      <c r="F144" s="11" t="s">
         <v>434</v>
       </c>
-      <c r="F144" s="11" t="s">
+      <c r="G144" s="11" t="s">
         <v>435</v>
       </c>
-      <c r="G144" s="11" t="s">
+      <c r="H144" s="11" t="s">
         <v>436</v>
-      </c>
-      <c r="H144" s="11" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -6470,22 +6470,22 @@
         <v>1</v>
       </c>
       <c r="C145" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="D145" s="8" t="s">
         <v>438</v>
       </c>
-      <c r="D145" s="8" t="s">
+      <c r="E145" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="E145" s="8" t="s">
+      <c r="F145" s="11" t="s">
         <v>440</v>
       </c>
-      <c r="F145" s="11" t="s">
+      <c r="G145" s="11" t="s">
         <v>441</v>
       </c>
-      <c r="G145" s="11" t="s">
+      <c r="H145" s="11" t="s">
         <v>442</v>
-      </c>
-      <c r="H145" s="11" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
@@ -6496,22 +6496,22 @@
         <v>6</v>
       </c>
       <c r="C146" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="D146" s="8" t="s">
         <v>444</v>
       </c>
-      <c r="D146" s="8" t="s">
+      <c r="E146" s="8" t="s">
         <v>445</v>
       </c>
-      <c r="E146" s="8" t="s">
+      <c r="F146" s="11" t="s">
         <v>446</v>
       </c>
-      <c r="F146" s="11" t="s">
+      <c r="G146" s="11" t="s">
+        <v>444</v>
+      </c>
+      <c r="H146" s="11" t="s">
         <v>447</v>
-      </c>
-      <c r="G146" s="11" t="s">
-        <v>445</v>
-      </c>
-      <c r="H146" s="11" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -6522,22 +6522,22 @@
         <v>1</v>
       </c>
       <c r="C147" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="D147" s="8" t="s">
         <v>449</v>
       </c>
-      <c r="D147" s="8" t="s">
+      <c r="E147" s="8" t="s">
         <v>450</v>
       </c>
-      <c r="E147" s="8" t="s">
+      <c r="F147" s="11" t="s">
         <v>451</v>
       </c>
-      <c r="F147" s="11" t="s">
+      <c r="G147" s="11" t="s">
+        <v>722</v>
+      </c>
+      <c r="H147" s="11" t="s">
         <v>452</v>
-      </c>
-      <c r="G147" s="11" t="s">
-        <v>723</v>
-      </c>
-      <c r="H147" s="11" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
@@ -6548,22 +6548,22 @@
         <v>2</v>
       </c>
       <c r="C148" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="D148" s="8" t="s">
         <v>454</v>
       </c>
-      <c r="D148" s="8" t="s">
+      <c r="E148" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="F148" s="11" t="s">
         <v>455</v>
       </c>
-      <c r="E148" s="8" t="s">
-        <v>428</v>
-      </c>
-      <c r="F148" s="11" t="s">
+      <c r="G148" s="11" t="s">
         <v>456</v>
       </c>
-      <c r="G148" s="11" t="s">
-        <v>457</v>
-      </c>
       <c r="H148" s="11" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="149" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -6574,22 +6574,22 @@
         <v>30</v>
       </c>
       <c r="C149" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="D149" s="8" t="s">
         <v>458</v>
       </c>
-      <c r="D149" s="8" t="s">
+      <c r="E149" s="8" t="s">
         <v>459</v>
       </c>
-      <c r="E149" s="8" t="s">
+      <c r="F149" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="F149" s="11" t="s">
+      <c r="G149" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="H149" s="11" t="s">
         <v>461</v>
-      </c>
-      <c r="G149" s="11" t="s">
-        <v>459</v>
-      </c>
-      <c r="H149" s="11" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="150" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -6600,22 +6600,22 @@
         <v>24</v>
       </c>
       <c r="C150" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="D150" s="8" t="s">
         <v>463</v>
       </c>
-      <c r="D150" s="8" t="s">
+      <c r="E150" s="8" t="s">
         <v>464</v>
       </c>
-      <c r="E150" s="8" t="s">
-        <v>465</v>
-      </c>
       <c r="F150" s="11" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G150" s="11" t="s">
+        <v>730</v>
+      </c>
+      <c r="H150" s="11" t="s">
         <v>731</v>
-      </c>
-      <c r="H150" s="11" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -6626,22 +6626,22 @@
         <v>23</v>
       </c>
       <c r="C151" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="D151" s="8" t="s">
         <v>466</v>
       </c>
-      <c r="D151" s="8" t="s">
+      <c r="E151" s="8" t="s">
         <v>467</v>
       </c>
-      <c r="E151" s="8" t="s">
+      <c r="F151" s="11" t="s">
         <v>468</v>
       </c>
-      <c r="F151" s="11" t="s">
+      <c r="G151" s="11" t="s">
         <v>469</v>
       </c>
-      <c r="G151" s="11" t="s">
+      <c r="H151" s="11" t="s">
         <v>470</v>
-      </c>
-      <c r="H151" s="11" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -6652,22 +6652,22 @@
         <v>7</v>
       </c>
       <c r="C152" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="D152" s="8" t="s">
         <v>472</v>
       </c>
-      <c r="D152" s="8" t="s">
+      <c r="E152" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="F152" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="G152" s="11" t="s">
+        <v>744</v>
+      </c>
+      <c r="H152" s="11" t="s">
         <v>473</v>
-      </c>
-      <c r="E152" s="8" t="s">
-        <v>468</v>
-      </c>
-      <c r="F152" s="11" t="s">
-        <v>435</v>
-      </c>
-      <c r="G152" s="11" t="s">
-        <v>745</v>
-      </c>
-      <c r="H152" s="11" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -6678,22 +6678,22 @@
         <v>1</v>
       </c>
       <c r="C153" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="D153" s="8" t="s">
         <v>475</v>
       </c>
-      <c r="D153" s="8" t="s">
+      <c r="E153" s="8" t="s">
         <v>476</v>
       </c>
-      <c r="E153" s="8" t="s">
+      <c r="F153" s="11" t="s">
         <v>477</v>
       </c>
-      <c r="F153" s="11" t="s">
+      <c r="G153" s="11" t="s">
         <v>478</v>
       </c>
-      <c r="G153" s="11" t="s">
+      <c r="H153" s="11" t="s">
         <v>479</v>
-      </c>
-      <c r="H153" s="11" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -6704,13 +6704,13 @@
         <v>2</v>
       </c>
       <c r="C154" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="D154" s="8" t="s">
         <v>481</v>
       </c>
-      <c r="D154" s="8" t="s">
-        <v>482</v>
-      </c>
       <c r="E154" s="8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F154" s="11" t="s">
         <v>196</v>
@@ -6719,7 +6719,7 @@
         <v>196</v>
       </c>
       <c r="H154" s="11" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="155" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -6730,22 +6730,22 @@
         <v>24</v>
       </c>
       <c r="C155" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="D155" s="8" t="s">
         <v>484</v>
       </c>
-      <c r="D155" s="8" t="s">
+      <c r="E155" s="8" t="s">
         <v>485</v>
       </c>
-      <c r="E155" s="8" t="s">
+      <c r="F155" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="G155" s="11" t="s">
+        <v>676</v>
+      </c>
+      <c r="H155" s="11" t="s">
         <v>486</v>
-      </c>
-      <c r="F155" s="11" t="s">
-        <v>447</v>
-      </c>
-      <c r="G155" s="11" t="s">
-        <v>677</v>
-      </c>
-      <c r="H155" s="11" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -6756,22 +6756,22 @@
         <v>1</v>
       </c>
       <c r="C156" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="D156" s="8" t="s">
         <v>488</v>
       </c>
-      <c r="D156" s="8" t="s">
+      <c r="E156" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="F156" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="G156" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="H156" s="11" t="s">
         <v>489</v>
-      </c>
-      <c r="E156" s="8" t="s">
-        <v>486</v>
-      </c>
-      <c r="F156" s="11" t="s">
-        <v>447</v>
-      </c>
-      <c r="G156" s="11" t="s">
-        <v>489</v>
-      </c>
-      <c r="H156" s="11" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="157" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -6782,22 +6782,22 @@
         <v>24</v>
       </c>
       <c r="C157" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="D157" s="8" t="s">
         <v>491</v>
       </c>
-      <c r="D157" s="8" t="s">
-        <v>492</v>
-      </c>
       <c r="E157" s="8" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F157" s="11" t="s">
         <v>109</v>
       </c>
       <c r="G157" s="11" t="s">
+        <v>492</v>
+      </c>
+      <c r="H157" s="11" t="s">
         <v>493</v>
-      </c>
-      <c r="H157" s="11" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -6808,13 +6808,13 @@
         <v>125</v>
       </c>
       <c r="C158" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="D158" s="8" t="s">
         <v>495</v>
       </c>
-      <c r="D158" s="8" t="s">
+      <c r="E158" s="8" t="s">
         <v>496</v>
-      </c>
-      <c r="E158" s="8" t="s">
-        <v>497</v>
       </c>
       <c r="F158" s="11" t="s">
         <v>196</v>
@@ -6823,7 +6823,7 @@
         <v>196</v>
       </c>
       <c r="H158" s="11" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -6834,22 +6834,22 @@
         <v>1</v>
       </c>
       <c r="C159" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="D159" s="8" t="s">
         <v>498</v>
       </c>
-      <c r="D159" s="8" t="s">
+      <c r="E159" s="8" t="s">
         <v>499</v>
-      </c>
-      <c r="E159" s="8" t="s">
-        <v>500</v>
       </c>
       <c r="F159" s="11" t="s">
         <v>185</v>
       </c>
       <c r="G159" s="11" t="s">
+        <v>499</v>
+      </c>
+      <c r="H159" s="11" t="s">
         <v>500</v>
-      </c>
-      <c r="H159" s="11" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -6860,22 +6860,22 @@
         <v>2</v>
       </c>
       <c r="C160" s="6" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D160" s="8" t="s">
+        <v>501</v>
+      </c>
+      <c r="E160" s="8" t="s">
         <v>502</v>
-      </c>
-      <c r="E160" s="8" t="s">
-        <v>503</v>
       </c>
       <c r="F160" s="11" t="s">
         <v>185</v>
       </c>
       <c r="G160" s="11" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H160" s="11" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
@@ -6886,22 +6886,22 @@
         <v>1</v>
       </c>
       <c r="C161" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="D161" s="8" t="s">
         <v>505</v>
       </c>
-      <c r="D161" s="8" t="s">
+      <c r="E161" s="8" t="s">
         <v>506</v>
-      </c>
-      <c r="E161" s="8" t="s">
-        <v>507</v>
       </c>
       <c r="F161" s="11" t="s">
         <v>185</v>
       </c>
       <c r="G161" s="11" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H161" s="11" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
@@ -6912,22 +6912,22 @@
         <v>1</v>
       </c>
       <c r="C162" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="D162" s="8" t="s">
+        <v>505</v>
+      </c>
+      <c r="E162" s="8" t="s">
         <v>509</v>
-      </c>
-      <c r="D162" s="8" t="s">
-        <v>506</v>
-      </c>
-      <c r="E162" s="8" t="s">
-        <v>510</v>
       </c>
       <c r="F162" s="11" t="s">
         <v>185</v>
       </c>
       <c r="G162" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="H162" s="11" t="s">
         <v>511</v>
-      </c>
-      <c r="H162" s="11" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
@@ -6938,22 +6938,22 @@
         <v>1</v>
       </c>
       <c r="C163" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="D163" s="8" t="s">
         <v>513</v>
       </c>
-      <c r="D163" s="8" t="s">
+      <c r="E163" s="8" t="s">
         <v>514</v>
-      </c>
-      <c r="E163" s="8" t="s">
-        <v>515</v>
       </c>
       <c r="F163" s="11" t="s">
         <v>185</v>
       </c>
       <c r="G163" s="11" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H163" s="11" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
@@ -6964,22 +6964,22 @@
         <v>1</v>
       </c>
       <c r="C164" s="6" t="s">
+        <v>516</v>
+      </c>
+      <c r="D164" s="8" t="s">
+        <v>723</v>
+      </c>
+      <c r="E164" s="8" t="s">
         <v>517</v>
-      </c>
-      <c r="D164" s="8" t="s">
-        <v>724</v>
-      </c>
-      <c r="E164" s="8" t="s">
-        <v>518</v>
       </c>
       <c r="F164" s="11" t="s">
         <v>185</v>
       </c>
       <c r="G164" s="11" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="H164" s="11" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
@@ -6990,22 +6990,22 @@
         <v>1</v>
       </c>
       <c r="C165" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="D165" s="8" t="s">
         <v>519</v>
       </c>
-      <c r="D165" s="8" t="s">
+      <c r="E165" s="8" t="s">
         <v>520</v>
       </c>
-      <c r="E165" s="8" t="s">
+      <c r="F165" s="11" t="s">
         <v>521</v>
       </c>
-      <c r="F165" s="11" t="s">
+      <c r="G165" s="11" t="s">
         <v>522</v>
       </c>
-      <c r="G165" s="11" t="s">
+      <c r="H165" s="11" t="s">
         <v>523</v>
-      </c>
-      <c r="H165" s="11" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
@@ -7016,22 +7016,22 @@
         <v>1</v>
       </c>
       <c r="C166" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="D166" s="8" t="s">
         <v>525</v>
       </c>
-      <c r="D166" s="8" t="s">
+      <c r="E166" s="8" t="s">
         <v>526</v>
       </c>
-      <c r="E166" s="8" t="s">
+      <c r="F166" s="11" t="s">
         <v>527</v>
       </c>
-      <c r="F166" s="11" t="s">
+      <c r="G166" s="11" t="s">
         <v>528</v>
       </c>
-      <c r="G166" s="11" t="s">
+      <c r="H166" s="11" t="s">
         <v>529</v>
-      </c>
-      <c r="H166" s="11" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
@@ -7042,22 +7042,22 @@
         <v>1</v>
       </c>
       <c r="C167" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="D167" s="8" t="s">
         <v>531</v>
       </c>
-      <c r="D167" s="8" t="s">
+      <c r="E167" s="8" t="s">
         <v>532</v>
       </c>
-      <c r="E167" s="8" t="s">
-        <v>533</v>
-      </c>
       <c r="F167" s="11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G167" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="H167" s="11" t="s">
         <v>684</v>
-      </c>
-      <c r="H167" s="11" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
@@ -7068,22 +7068,22 @@
         <v>7</v>
       </c>
       <c r="C168" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="D168" s="8" t="s">
         <v>534</v>
       </c>
-      <c r="D168" s="8" t="s">
+      <c r="E168" s="8" t="s">
         <v>535</v>
-      </c>
-      <c r="E168" s="8" t="s">
-        <v>536</v>
       </c>
       <c r="F168" s="11" t="s">
         <v>185</v>
       </c>
       <c r="G168" s="11" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="H168" s="11" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>